<commit_message>
Added Inductor for 3.3V SPS
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="0" windowWidth="33000" windowHeight="21160" tabRatio="986"/>
+    <workbookView xWindow="-480" yWindow="21660" windowWidth="28000" windowHeight="17980" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="586">
   <si>
     <t>Part</t>
   </si>
@@ -1760,6 +1760,24 @@
   </si>
   <si>
     <t>OOPS!! This is not the right part.  Digikey/Mouser do not carry an 0603 cap with this value.  Consider changing to 0402 package</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>851-CDRH2D14NP-2R2NC</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>3.2 mm x 3.2 mm</t>
+  </si>
+  <si>
+    <t>Digikey has no stock</t>
   </si>
 </sst>
 </file>
@@ -2468,6 +2486,18 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2510,33 +2540,21 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="221">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3093,10 +3111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO60"/>
+  <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AO10" sqref="AO10"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="AJ28" sqref="AJ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3114,16 +3132,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="60" customFormat="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="69"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="75"/>
       <c r="I1" s="58"/>
       <c r="J1" s="58"/>
       <c r="K1" s="58"/>
@@ -3146,43 +3164,43 @@
       <c r="AB1" s="58"/>
       <c r="AC1" s="58"/>
       <c r="AD1" s="58"/>
-      <c r="AE1" s="65" t="s">
+      <c r="AE1" s="71" t="s">
         <v>254</v>
       </c>
-      <c r="AF1" s="65" t="s">
+      <c r="AF1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="AG1" s="65" t="s">
+      <c r="AG1" s="71" t="s">
         <v>257</v>
       </c>
-      <c r="AH1" s="77" t="s">
+      <c r="AH1" s="83" t="s">
         <v>259</v>
       </c>
-      <c r="AI1" s="77" t="s">
+      <c r="AI1" s="83" t="s">
         <v>516</v>
       </c>
-      <c r="AJ1" s="77" t="s">
+      <c r="AJ1" s="83" t="s">
         <v>556</v>
       </c>
-      <c r="AK1" s="75" t="s">
+      <c r="AK1" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" s="76"/>
-      <c r="AM1" s="76"/>
-      <c r="AN1" s="76"/>
-      <c r="AO1" s="73" t="s">
+      <c r="AL1" s="82"/>
+      <c r="AM1" s="82"/>
+      <c r="AN1" s="82"/>
+      <c r="AO1" s="79" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="60" customFormat="1" ht="15" thickBot="1">
-      <c r="A2" s="70"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="78"/>
       <c r="I2" s="59"/>
       <c r="J2" s="59"/>
       <c r="K2" s="59"/>
@@ -3205,12 +3223,12 @@
       <c r="AB2" s="59"/>
       <c r="AC2" s="59"/>
       <c r="AD2" s="59"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="78"/>
+      <c r="AE2" s="72"/>
+      <c r="AF2" s="72"/>
+      <c r="AG2" s="72"/>
+      <c r="AH2" s="84"/>
+      <c r="AI2" s="84"/>
+      <c r="AJ2" s="84"/>
       <c r="AK2" s="27">
         <v>1</v>
       </c>
@@ -3223,7 +3241,7 @@
       <c r="AN2" s="3">
         <v>1000</v>
       </c>
-      <c r="AO2" s="74"/>
+      <c r="AO2" s="80"/>
     </row>
     <row r="3" spans="1:41" s="60" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="38" t="s">
@@ -3755,69 +3773,69 @@
       <c r="AO9" s="37"/>
     </row>
     <row r="10" spans="1:41" s="60" customFormat="1">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="65" t="s">
         <v>310</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="85"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="85"/>
-      <c r="O10" s="85"/>
-      <c r="P10" s="85"/>
-      <c r="Q10" s="85"/>
-      <c r="R10" s="85"/>
-      <c r="S10" s="85"/>
-      <c r="T10" s="85"/>
-      <c r="U10" s="85"/>
-      <c r="V10" s="85"/>
-      <c r="W10" s="85"/>
-      <c r="X10" s="85"/>
-      <c r="Y10" s="85"/>
-      <c r="Z10" s="85"/>
-      <c r="AA10" s="85"/>
-      <c r="AB10" s="85"/>
-      <c r="AC10" s="85"/>
-      <c r="AD10" s="85"/>
-      <c r="AE10" s="86">
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
+      <c r="U10" s="66"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="66"/>
+      <c r="Y10" s="66"/>
+      <c r="Z10" s="66"/>
+      <c r="AA10" s="66"/>
+      <c r="AB10" s="66"/>
+      <c r="AC10" s="66"/>
+      <c r="AD10" s="66"/>
+      <c r="AE10" s="67">
         <v>2</v>
       </c>
-      <c r="AF10" s="86" t="s">
+      <c r="AF10" s="67" t="s">
         <v>264</v>
       </c>
-      <c r="AG10" s="86" t="s">
+      <c r="AG10" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="AH10" s="87" t="s">
+      <c r="AH10" s="68" t="s">
         <v>518</v>
       </c>
-      <c r="AI10" s="87" t="s">
+      <c r="AI10" s="68" t="s">
         <v>551</v>
       </c>
-      <c r="AJ10" s="87"/>
-      <c r="AK10" s="88">
+      <c r="AJ10" s="68"/>
+      <c r="AK10" s="69">
         <v>0.12</v>
       </c>
-      <c r="AL10" s="88">
+      <c r="AL10" s="69">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="AM10" s="88">
+      <c r="AM10" s="69">
         <v>3.9E-2</v>
       </c>
-      <c r="AN10" s="88">
+      <c r="AN10" s="69">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AO10" s="89" t="s">
+      <c r="AO10" s="70" t="s">
         <v>579</v>
       </c>
     </row>
@@ -4922,7 +4940,7 @@
     </row>
     <row r="28" spans="1:41" s="60" customFormat="1">
       <c r="A28" s="40" t="s">
-        <v>425</v>
+        <v>580</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -4957,165 +4975,167 @@
         <v>1</v>
       </c>
       <c r="AF28" s="57" t="s">
+        <v>581</v>
+      </c>
+      <c r="AG28" s="57" t="s">
+        <v>584</v>
+      </c>
+      <c r="AH28" s="39" t="s">
+        <v>583</v>
+      </c>
+      <c r="AI28" s="39"/>
+      <c r="AJ28" s="39" t="s">
+        <v>582</v>
+      </c>
+      <c r="AK28" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="AL28" s="30">
+        <v>0.77</v>
+      </c>
+      <c r="AM28" s="30">
+        <v>0.63</v>
+      </c>
+      <c r="AN28" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO28" s="37" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" s="60" customFormat="1">
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="47"/>
+      <c r="R29" s="47"/>
+      <c r="S29" s="47"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="47"/>
+      <c r="V29" s="47"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="47"/>
+      <c r="Y29" s="47"/>
+      <c r="Z29" s="47"/>
+      <c r="AA29" s="47"/>
+      <c r="AB29" s="47"/>
+      <c r="AC29" s="47"/>
+      <c r="AD29" s="47"/>
+      <c r="AE29" s="62"/>
+      <c r="AF29" s="62"/>
+      <c r="AG29" s="62"/>
+      <c r="AH29" s="49"/>
+      <c r="AI29" s="49"/>
+      <c r="AJ29" s="49"/>
+      <c r="AK29" s="32"/>
+      <c r="AL29" s="32"/>
+      <c r="AM29" s="32"/>
+      <c r="AN29" s="32"/>
+      <c r="AO29" s="48"/>
+    </row>
+    <row r="30" spans="1:41" s="60" customFormat="1">
+      <c r="A30" s="40" t="s">
+        <v>425</v>
+      </c>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="40"/>
+      <c r="T30" s="40"/>
+      <c r="U30" s="40"/>
+      <c r="V30" s="40"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="40"/>
+      <c r="Z30" s="40"/>
+      <c r="AA30" s="40"/>
+      <c r="AB30" s="40"/>
+      <c r="AC30" s="40"/>
+      <c r="AD30" s="40"/>
+      <c r="AE30" s="57">
+        <v>1</v>
+      </c>
+      <c r="AF30" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="AG28" s="57"/>
-      <c r="AH28" s="39" t="s">
+      <c r="AG30" s="57"/>
+      <c r="AH30" s="39" t="s">
         <v>426</v>
       </c>
-      <c r="AI28" s="39" t="s">
+      <c r="AI30" s="39" t="s">
         <v>557</v>
       </c>
-      <c r="AJ28" s="57" t="s">
+      <c r="AJ30" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="AK28" s="30">
+      <c r="AK30" s="30">
         <v>1.79</v>
       </c>
-      <c r="AL28" s="30">
+      <c r="AL30" s="30">
         <v>1.1599999999999999</v>
       </c>
-      <c r="AM28" s="30">
+      <c r="AM30" s="30">
         <v>1.03</v>
       </c>
-      <c r="AN28" s="30">
+      <c r="AN30" s="30">
         <v>0.67700000000000005</v>
       </c>
-      <c r="AO28" s="37" t="s">
+      <c r="AO30" s="37" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="29" spans="1:41" s="60" customFormat="1">
-      <c r="A29" s="40" t="s">
-        <v>396</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>397</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>398</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>399</v>
-      </c>
-      <c r="E29" s="40" t="s">
-        <v>400</v>
-      </c>
-      <c r="F29" s="40" t="s">
-        <v>401</v>
-      </c>
-      <c r="G29" s="40" t="s">
-        <v>402</v>
-      </c>
-      <c r="H29" s="40" t="s">
-        <v>403</v>
-      </c>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="40"/>
-      <c r="R29" s="40"/>
-      <c r="S29" s="40"/>
-      <c r="T29" s="40"/>
-      <c r="U29" s="40"/>
-      <c r="V29" s="40"/>
-      <c r="W29" s="40"/>
-      <c r="X29" s="40"/>
-      <c r="Y29" s="40"/>
-      <c r="Z29" s="40"/>
-      <c r="AA29" s="40"/>
-      <c r="AB29" s="40"/>
-      <c r="AC29" s="40"/>
-      <c r="AD29" s="40"/>
-      <c r="AE29" s="57">
-        <v>8</v>
-      </c>
-      <c r="AF29" s="57" t="s">
-        <v>369</v>
-      </c>
-      <c r="AG29" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH29" s="39" t="s">
-        <v>370</v>
-      </c>
-      <c r="AI29" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="AJ29" s="39"/>
-      <c r="AK29" s="30">
-        <v>0.09</v>
-      </c>
-      <c r="AL29" s="30">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="AM29" s="30">
-        <v>5.8799999999999998E-2</v>
-      </c>
-      <c r="AN29" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="AO29" s="37"/>
-    </row>
-    <row r="30" spans="1:41" s="60" customFormat="1">
-      <c r="A30" s="47"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="47"/>
-      <c r="Q30" s="47"/>
-      <c r="R30" s="47"/>
-      <c r="S30" s="47"/>
-      <c r="T30" s="47"/>
-      <c r="U30" s="47"/>
-      <c r="V30" s="47"/>
-      <c r="W30" s="47"/>
-      <c r="X30" s="47"/>
-      <c r="Y30" s="47"/>
-      <c r="Z30" s="47"/>
-      <c r="AA30" s="47"/>
-      <c r="AB30" s="47"/>
-      <c r="AC30" s="47"/>
-      <c r="AD30" s="47"/>
-      <c r="AE30" s="62"/>
-      <c r="AF30" s="62"/>
-      <c r="AG30" s="62"/>
-      <c r="AH30" s="49"/>
-      <c r="AI30" s="49"/>
-      <c r="AJ30" s="49"/>
-      <c r="AK30" s="32"/>
-      <c r="AL30" s="32"/>
-      <c r="AM30" s="32"/>
-      <c r="AN30" s="32"/>
-      <c r="AO30" s="48"/>
     </row>
     <row r="31" spans="1:41" s="60" customFormat="1">
       <c r="A31" s="40" t="s">
-        <v>333</v>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
+        <v>396</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>397</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>398</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>399</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>400</v>
+      </c>
+      <c r="F31" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>402</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>403</v>
+      </c>
       <c r="I31" s="40"/>
       <c r="J31" s="40"/>
       <c r="K31" s="40"/>
@@ -5139,32 +5159,32 @@
       <c r="AC31" s="40"/>
       <c r="AD31" s="40"/>
       <c r="AE31" s="57">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AF31" s="57" t="s">
-        <v>334</v>
+        <v>369</v>
       </c>
       <c r="AG31" s="57" t="s">
-        <v>335</v>
+        <v>70</v>
       </c>
       <c r="AH31" s="39" t="s">
-        <v>342</v>
+        <v>370</v>
       </c>
       <c r="AI31" s="39" t="s">
-        <v>559</v>
+        <v>185</v>
       </c>
       <c r="AJ31" s="39"/>
       <c r="AK31" s="30">
-        <v>0.22</v>
+        <v>0.09</v>
       </c>
       <c r="AL31" s="30">
-        <v>0.19800000000000001</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="AM31" s="30">
-        <v>0.111</v>
-      </c>
-      <c r="AN31" s="30">
-        <v>4.0500000000000001E-2</v>
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="AN31" s="30" t="s">
+        <v>26</v>
       </c>
       <c r="AO31" s="37"/>
     </row>
@@ -5212,15 +5232,11 @@
       <c r="AO32" s="48"/>
     </row>
     <row r="33" spans="1:41" s="60" customFormat="1">
-      <c r="A33" s="38" t="s">
-        <v>260</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>523</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>524</v>
-      </c>
+      <c r="A33" s="40" t="s">
+        <v>333</v>
+      </c>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
       <c r="D33" s="40"/>
       <c r="E33" s="40"/>
       <c r="F33" s="40"/>
@@ -5249,96 +5265,88 @@
       <c r="AC33" s="40"/>
       <c r="AD33" s="40"/>
       <c r="AE33" s="57">
-        <v>3</v>
-      </c>
-      <c r="AF33" s="57"/>
+        <v>1</v>
+      </c>
+      <c r="AF33" s="57" t="s">
+        <v>334</v>
+      </c>
       <c r="AG33" s="57" t="s">
-        <v>70</v>
+        <v>335</v>
       </c>
       <c r="AH33" s="39" t="s">
-        <v>525</v>
-      </c>
-      <c r="AI33" s="41"/>
-      <c r="AJ33" s="41"/>
-      <c r="AK33" s="28"/>
-      <c r="AL33" s="28"/>
-      <c r="AM33" s="28"/>
-      <c r="AN33" s="28"/>
+        <v>342</v>
+      </c>
+      <c r="AI33" s="39" t="s">
+        <v>559</v>
+      </c>
+      <c r="AJ33" s="39"/>
+      <c r="AK33" s="30">
+        <v>0.22</v>
+      </c>
+      <c r="AL33" s="30">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="AM33" s="30">
+        <v>0.111</v>
+      </c>
+      <c r="AN33" s="30">
+        <v>4.0500000000000001E-2</v>
+      </c>
       <c r="AO33" s="37"/>
     </row>
     <row r="34" spans="1:41" s="60" customFormat="1">
-      <c r="A34" s="51" t="s">
-        <v>530</v>
-      </c>
-      <c r="B34" s="51" t="s">
-        <v>531</v>
-      </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52"/>
-      <c r="R34" s="52"/>
-      <c r="S34" s="52"/>
-      <c r="T34" s="52"/>
-      <c r="U34" s="52"/>
-      <c r="V34" s="52"/>
-      <c r="W34" s="52"/>
-      <c r="X34" s="52"/>
-      <c r="Y34" s="52"/>
-      <c r="Z34" s="52"/>
-      <c r="AA34" s="52"/>
-      <c r="AB34" s="52"/>
-      <c r="AC34" s="52"/>
-      <c r="AD34" s="52"/>
-      <c r="AE34" s="63">
-        <v>2</v>
-      </c>
-      <c r="AF34" s="63" t="s">
-        <v>256</v>
-      </c>
-      <c r="AG34" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH34" s="54" t="s">
-        <v>561</v>
-      </c>
-      <c r="AI34" s="54" t="s">
-        <v>562</v>
-      </c>
-      <c r="AJ34" s="54"/>
-      <c r="AK34" s="35" t="s">
-        <v>563</v>
-      </c>
-      <c r="AL34" s="35">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AM34" s="35">
-        <v>4.7000000000000002E-3</v>
-      </c>
-      <c r="AN34" s="35">
-        <v>2.0999999999999999E-3</v>
-      </c>
-      <c r="AO34" s="53" t="s">
-        <v>560</v>
-      </c>
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
+      <c r="Q34" s="47"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="47"/>
+      <c r="T34" s="47"/>
+      <c r="U34" s="47"/>
+      <c r="V34" s="47"/>
+      <c r="W34" s="47"/>
+      <c r="X34" s="47"/>
+      <c r="Y34" s="47"/>
+      <c r="Z34" s="47"/>
+      <c r="AA34" s="47"/>
+      <c r="AB34" s="47"/>
+      <c r="AC34" s="47"/>
+      <c r="AD34" s="47"/>
+      <c r="AE34" s="62"/>
+      <c r="AF34" s="62"/>
+      <c r="AG34" s="62"/>
+      <c r="AH34" s="49"/>
+      <c r="AI34" s="49"/>
+      <c r="AJ34" s="49"/>
+      <c r="AK34" s="32"/>
+      <c r="AL34" s="32"/>
+      <c r="AM34" s="32"/>
+      <c r="AN34" s="32"/>
+      <c r="AO34" s="48"/>
     </row>
     <row r="35" spans="1:41" s="60" customFormat="1">
       <c r="A35" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
+        <v>260</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>523</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>524</v>
+      </c>
       <c r="D35" s="40"/>
       <c r="E35" s="40"/>
       <c r="F35" s="40"/>
@@ -5367,178 +5375,178 @@
       <c r="AC35" s="40"/>
       <c r="AD35" s="40"/>
       <c r="AE35" s="57">
-        <v>1</v>
-      </c>
-      <c r="AF35" s="57" t="s">
-        <v>256</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="AF35" s="57"/>
       <c r="AG35" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="AH35" s="39">
+      <c r="AH35" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="AI35" s="41"/>
+      <c r="AJ35" s="41"/>
+      <c r="AK35" s="28"/>
+      <c r="AL35" s="28"/>
+      <c r="AM35" s="28"/>
+      <c r="AN35" s="28"/>
+      <c r="AO35" s="37"/>
+    </row>
+    <row r="36" spans="1:41" s="60" customFormat="1">
+      <c r="A36" s="51" t="s">
+        <v>530</v>
+      </c>
+      <c r="B36" s="51" t="s">
+        <v>531</v>
+      </c>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
+      <c r="Q36" s="52"/>
+      <c r="R36" s="52"/>
+      <c r="S36" s="52"/>
+      <c r="T36" s="52"/>
+      <c r="U36" s="52"/>
+      <c r="V36" s="52"/>
+      <c r="W36" s="52"/>
+      <c r="X36" s="52"/>
+      <c r="Y36" s="52"/>
+      <c r="Z36" s="52"/>
+      <c r="AA36" s="52"/>
+      <c r="AB36" s="52"/>
+      <c r="AC36" s="52"/>
+      <c r="AD36" s="52"/>
+      <c r="AE36" s="63">
+        <v>2</v>
+      </c>
+      <c r="AF36" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG36" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH36" s="54" t="s">
+        <v>561</v>
+      </c>
+      <c r="AI36" s="54" t="s">
+        <v>562</v>
+      </c>
+      <c r="AJ36" s="54"/>
+      <c r="AK36" s="35" t="s">
+        <v>563</v>
+      </c>
+      <c r="AL36" s="35">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AM36" s="35">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="AN36" s="35">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="AO36" s="53" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="37" spans="1:41" s="60" customFormat="1">
+      <c r="A37" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="40"/>
+      <c r="O37" s="40"/>
+      <c r="P37" s="40"/>
+      <c r="Q37" s="40"/>
+      <c r="R37" s="40"/>
+      <c r="S37" s="40"/>
+      <c r="T37" s="40"/>
+      <c r="U37" s="40"/>
+      <c r="V37" s="40"/>
+      <c r="W37" s="40"/>
+      <c r="X37" s="40"/>
+      <c r="Y37" s="40"/>
+      <c r="Z37" s="40"/>
+      <c r="AA37" s="40"/>
+      <c r="AB37" s="40"/>
+      <c r="AC37" s="40"/>
+      <c r="AD37" s="40"/>
+      <c r="AE37" s="57">
+        <v>1</v>
+      </c>
+      <c r="AF37" s="57" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG37" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH37" s="39">
         <v>120</v>
       </c>
-      <c r="AI35" s="45" t="s">
+      <c r="AI37" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="AJ35" s="45"/>
-      <c r="AK35" s="31">
+      <c r="AJ37" s="45"/>
+      <c r="AK37" s="31">
         <v>0.17</v>
       </c>
-      <c r="AL35" s="31">
+      <c r="AL37" s="31">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AM35" s="31">
+      <c r="AM37" s="31">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="AN35" s="31">
+      <c r="AN37" s="31">
         <v>2.3560000000000001E-2</v>
       </c>
-      <c r="AO35" s="37"/>
-    </row>
-    <row r="36" spans="1:41" s="60" customFormat="1">
-      <c r="A36" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="B36" s="38" t="s">
-        <v>532</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>533</v>
-      </c>
-      <c r="D36" s="38" t="s">
-        <v>534</v>
-      </c>
-      <c r="E36" s="38" t="s">
-        <v>535</v>
-      </c>
-      <c r="F36" s="38" t="s">
-        <v>536</v>
-      </c>
-      <c r="G36" s="38" t="s">
-        <v>537</v>
-      </c>
-      <c r="H36" s="38" t="s">
-        <v>538</v>
-      </c>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40"/>
-      <c r="O36" s="40"/>
-      <c r="P36" s="40"/>
-      <c r="Q36" s="40"/>
-      <c r="R36" s="40"/>
-      <c r="S36" s="40"/>
-      <c r="T36" s="40"/>
-      <c r="U36" s="40"/>
-      <c r="V36" s="40"/>
-      <c r="W36" s="40"/>
-      <c r="X36" s="40"/>
-      <c r="Y36" s="40"/>
-      <c r="Z36" s="40"/>
-      <c r="AA36" s="40"/>
-      <c r="AB36" s="40"/>
-      <c r="AC36" s="40"/>
-      <c r="AD36" s="40"/>
-      <c r="AE36" s="57">
-        <v>8</v>
-      </c>
-      <c r="AF36" s="57" t="s">
-        <v>256</v>
-      </c>
-      <c r="AG36" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH36" s="39">
-        <v>649</v>
-      </c>
-      <c r="AI36" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="AJ36" s="41"/>
-      <c r="AK36" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="AL36" s="28">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AM36" s="28">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="AN36" s="28">
-        <v>3.8400000000000001E-3</v>
-      </c>
-      <c r="AO36" s="37"/>
-    </row>
-    <row r="37" spans="1:41" s="60" customFormat="1">
-      <c r="A37" s="42" t="s">
-        <v>262</v>
-      </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="42"/>
-      <c r="L37" s="42"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="42"/>
-      <c r="Q37" s="42"/>
-      <c r="R37" s="42"/>
-      <c r="S37" s="42"/>
-      <c r="T37" s="42"/>
-      <c r="U37" s="42"/>
-      <c r="V37" s="42"/>
-      <c r="W37" s="42"/>
-      <c r="X37" s="42"/>
-      <c r="Y37" s="42"/>
-      <c r="Z37" s="42"/>
-      <c r="AA37" s="42"/>
-      <c r="AB37" s="42"/>
-      <c r="AC37" s="42"/>
-      <c r="AD37" s="42"/>
-      <c r="AE37" s="61">
-        <v>1</v>
-      </c>
-      <c r="AF37" s="61" t="s">
-        <v>256</v>
-      </c>
-      <c r="AG37" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH37" s="44">
-        <v>675</v>
-      </c>
-      <c r="AI37" s="44"/>
-      <c r="AJ37" s="44"/>
-      <c r="AK37" s="29"/>
-      <c r="AL37" s="29"/>
-      <c r="AM37" s="29"/>
-      <c r="AN37" s="29"/>
-      <c r="AO37" s="43" t="s">
-        <v>564</v>
-      </c>
+      <c r="AO37" s="37"/>
     </row>
     <row r="38" spans="1:41" s="60" customFormat="1">
       <c r="A38" s="38" t="s">
-        <v>296</v>
-      </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
+        <v>285</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>532</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>533</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>534</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>535</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>536</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>537</v>
+      </c>
+      <c r="H38" s="38" t="s">
+        <v>538</v>
+      </c>
       <c r="I38" s="40"/>
       <c r="J38" s="40"/>
       <c r="K38" s="40"/>
@@ -5562,7 +5570,7 @@
       <c r="AC38" s="40"/>
       <c r="AD38" s="40"/>
       <c r="AE38" s="57">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AF38" s="57" t="s">
         <v>256</v>
@@ -5570,203 +5578,117 @@
       <c r="AG38" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="AH38" s="39" t="s">
-        <v>297</v>
-      </c>
-      <c r="AI38" s="39" t="s">
-        <v>565</v>
-      </c>
-      <c r="AJ38" s="57"/>
-      <c r="AK38" s="30">
-        <v>0.08</v>
-      </c>
-      <c r="AL38" s="30">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="AM38" s="30">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="AN38" s="30">
-        <v>2.4E-2</v>
+      <c r="AH38" s="39">
+        <v>649</v>
+      </c>
+      <c r="AI38" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="AJ38" s="41"/>
+      <c r="AK38" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="AL38" s="28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AM38" s="28">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="AN38" s="28">
+        <v>3.8400000000000001E-3</v>
       </c>
       <c r="AO38" s="37"/>
     </row>
     <row r="39" spans="1:41" s="60" customFormat="1">
-      <c r="A39" s="38" t="s">
-        <v>312</v>
-      </c>
-      <c r="B39" s="38" t="s">
-        <v>313</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>314</v>
-      </c>
-      <c r="D39" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="F39" s="38" t="s">
-        <v>317</v>
-      </c>
-      <c r="G39" s="38" t="s">
-        <v>318</v>
-      </c>
-      <c r="H39" s="38" t="s">
-        <v>319</v>
-      </c>
-      <c r="I39" s="38" t="s">
-        <v>320</v>
-      </c>
-      <c r="J39" s="38" t="s">
-        <v>321</v>
-      </c>
-      <c r="K39" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="40"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="40"/>
-      <c r="S39" s="40"/>
-      <c r="T39" s="40"/>
-      <c r="U39" s="40"/>
-      <c r="V39" s="40"/>
-      <c r="W39" s="40"/>
-      <c r="X39" s="40"/>
-      <c r="Y39" s="40"/>
-      <c r="Z39" s="40"/>
-      <c r="AA39" s="40"/>
-      <c r="AB39" s="40"/>
-      <c r="AC39" s="40"/>
-      <c r="AD39" s="40"/>
-      <c r="AE39" s="57">
-        <v>11</v>
-      </c>
-      <c r="AF39" s="57" t="s">
+      <c r="A39" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="42"/>
+      <c r="L39" s="42"/>
+      <c r="M39" s="42"/>
+      <c r="N39" s="42"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="42"/>
+      <c r="Q39" s="42"/>
+      <c r="R39" s="42"/>
+      <c r="S39" s="42"/>
+      <c r="T39" s="42"/>
+      <c r="U39" s="42"/>
+      <c r="V39" s="42"/>
+      <c r="W39" s="42"/>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
+      <c r="Z39" s="42"/>
+      <c r="AA39" s="42"/>
+      <c r="AB39" s="42"/>
+      <c r="AC39" s="42"/>
+      <c r="AD39" s="42"/>
+      <c r="AE39" s="61">
+        <v>1</v>
+      </c>
+      <c r="AF39" s="61" t="s">
         <v>256</v>
       </c>
-      <c r="AG39" s="57" t="s">
+      <c r="AG39" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="AH39" s="39" t="s">
-        <v>323</v>
-      </c>
-      <c r="AI39" s="39" t="s">
-        <v>566</v>
-      </c>
-      <c r="AJ39" s="57"/>
-      <c r="AK39" s="30">
-        <v>0.08</v>
-      </c>
-      <c r="AL39" s="30">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="AM39" s="30">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="AN39" s="30">
-        <v>2.4E-2</v>
-      </c>
-      <c r="AO39" s="37"/>
+      <c r="AH39" s="44">
+        <v>675</v>
+      </c>
+      <c r="AI39" s="44"/>
+      <c r="AJ39" s="44"/>
+      <c r="AK39" s="29"/>
+      <c r="AL39" s="29"/>
+      <c r="AM39" s="29"/>
+      <c r="AN39" s="29"/>
+      <c r="AO39" s="43" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="40" spans="1:41" s="60" customFormat="1">
       <c r="A40" s="38" t="s">
-        <v>431</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>432</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>433</v>
-      </c>
-      <c r="D40" s="38" t="s">
-        <v>434</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>435</v>
-      </c>
-      <c r="F40" s="38" t="s">
-        <v>436</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>437</v>
-      </c>
-      <c r="H40" s="38" t="s">
-        <v>438</v>
-      </c>
-      <c r="I40" s="38" t="s">
-        <v>439</v>
-      </c>
-      <c r="J40" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="K40" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="L40" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M40" s="38" t="s">
-        <v>443</v>
-      </c>
-      <c r="N40" s="38" t="s">
-        <v>444</v>
-      </c>
-      <c r="O40" s="38" t="s">
-        <v>445</v>
-      </c>
-      <c r="P40" s="38" t="s">
-        <v>446</v>
-      </c>
-      <c r="Q40" s="38" t="s">
-        <v>447</v>
-      </c>
-      <c r="R40" s="38" t="s">
-        <v>448</v>
-      </c>
-      <c r="S40" s="38" t="s">
-        <v>449</v>
-      </c>
-      <c r="T40" s="38" t="s">
-        <v>450</v>
-      </c>
-      <c r="U40" s="38" t="s">
-        <v>451</v>
-      </c>
-      <c r="V40" s="38" t="s">
-        <v>452</v>
-      </c>
-      <c r="W40" s="38" t="s">
-        <v>453</v>
-      </c>
-      <c r="X40" s="38" t="s">
-        <v>454</v>
-      </c>
-      <c r="Y40" s="38" t="s">
-        <v>455</v>
-      </c>
-      <c r="Z40" s="38" t="s">
-        <v>456</v>
-      </c>
-      <c r="AA40" s="38" t="s">
-        <v>457</v>
-      </c>
-      <c r="AB40" s="38" t="s">
-        <v>458</v>
-      </c>
-      <c r="AC40" s="38" t="s">
-        <v>459</v>
-      </c>
-      <c r="AD40" s="38" t="s">
-        <v>460</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="40"/>
+      <c r="N40" s="40"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="40"/>
+      <c r="Q40" s="40"/>
+      <c r="R40" s="40"/>
+      <c r="S40" s="40"/>
+      <c r="T40" s="40"/>
+      <c r="U40" s="40"/>
+      <c r="V40" s="40"/>
+      <c r="W40" s="40"/>
+      <c r="X40" s="40"/>
+      <c r="Y40" s="40"/>
+      <c r="Z40" s="40"/>
+      <c r="AA40" s="40"/>
+      <c r="AB40" s="40"/>
+      <c r="AC40" s="40"/>
+      <c r="AD40" s="40"/>
       <c r="AE40" s="57">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AF40" s="57" t="s">
         <v>256</v>
@@ -5775,38 +5697,60 @@
         <v>70</v>
       </c>
       <c r="AH40" s="39" t="s">
-        <v>539</v>
+        <v>297</v>
       </c>
       <c r="AI40" s="39" t="s">
-        <v>540</v>
-      </c>
-      <c r="AJ40" s="39"/>
+        <v>565</v>
+      </c>
+      <c r="AJ40" s="57"/>
       <c r="AK40" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="AL40" s="30"/>
+        <v>0.08</v>
+      </c>
+      <c r="AL40" s="30">
+        <v>6.9000000000000006E-2</v>
+      </c>
       <c r="AM40" s="30">
-        <v>1.4999999999999999E-2</v>
+        <v>4.0800000000000003E-2</v>
       </c>
       <c r="AN40" s="30">
-        <v>4.0000000000000001E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="AO40" s="37"/>
     </row>
     <row r="41" spans="1:41" s="60" customFormat="1">
-      <c r="A41" s="40" t="s">
-        <v>327</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
+      <c r="A41" s="38" t="s">
+        <v>312</v>
+      </c>
+      <c r="B41" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="D41" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="F41" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="G41" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="H41" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="I41" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="J41" s="38" t="s">
+        <v>321</v>
+      </c>
+      <c r="K41" s="38" t="s">
+        <v>322</v>
+      </c>
       <c r="L41" s="40"/>
       <c r="M41" s="40"/>
       <c r="N41" s="40"/>
@@ -5827,7 +5771,7 @@
       <c r="AC41" s="40"/>
       <c r="AD41" s="40"/>
       <c r="AE41" s="57">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AF41" s="57" t="s">
         <v>256</v>
@@ -5836,71 +5780,119 @@
         <v>70</v>
       </c>
       <c r="AH41" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI41" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ41" s="41"/>
-      <c r="AK41" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="AL41" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM41" s="28">
-        <v>1.14E-2</v>
-      </c>
-      <c r="AN41" s="28">
-        <v>4.1599999999999996E-3</v>
+        <v>323</v>
+      </c>
+      <c r="AI41" s="39" t="s">
+        <v>566</v>
+      </c>
+      <c r="AJ41" s="57"/>
+      <c r="AK41" s="30">
+        <v>0.08</v>
+      </c>
+      <c r="AL41" s="30">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AM41" s="30">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="AN41" s="30">
+        <v>2.4E-2</v>
       </c>
       <c r="AO41" s="37"/>
     </row>
     <row r="42" spans="1:41" s="60" customFormat="1">
       <c r="A42" s="38" t="s">
-        <v>263</v>
+        <v>431</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>286</v>
+        <v>432</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>326</v>
+        <v>433</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>390</v>
+        <v>434</v>
       </c>
       <c r="E42" s="38" t="s">
-        <v>526</v>
+        <v>435</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>527</v>
-      </c>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="40"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
-      <c r="P42" s="40"/>
-      <c r="Q42" s="40"/>
-      <c r="R42" s="40"/>
-      <c r="S42" s="40"/>
-      <c r="T42" s="40"/>
-      <c r="U42" s="40"/>
-      <c r="V42" s="40"/>
-      <c r="W42" s="40"/>
-      <c r="X42" s="40"/>
-      <c r="Y42" s="40"/>
-      <c r="Z42" s="40"/>
-      <c r="AA42" s="40"/>
-      <c r="AB42" s="40"/>
-      <c r="AC42" s="40"/>
-      <c r="AD42" s="40"/>
+        <v>436</v>
+      </c>
+      <c r="G42" s="38" t="s">
+        <v>437</v>
+      </c>
+      <c r="H42" s="38" t="s">
+        <v>438</v>
+      </c>
+      <c r="I42" s="38" t="s">
+        <v>439</v>
+      </c>
+      <c r="J42" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="K42" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="L42" s="38" t="s">
+        <v>442</v>
+      </c>
+      <c r="M42" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="N42" s="38" t="s">
+        <v>444</v>
+      </c>
+      <c r="O42" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="P42" s="38" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q42" s="38" t="s">
+        <v>447</v>
+      </c>
+      <c r="R42" s="38" t="s">
+        <v>448</v>
+      </c>
+      <c r="S42" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="T42" s="38" t="s">
+        <v>450</v>
+      </c>
+      <c r="U42" s="38" t="s">
+        <v>451</v>
+      </c>
+      <c r="V42" s="38" t="s">
+        <v>452</v>
+      </c>
+      <c r="W42" s="38" t="s">
+        <v>453</v>
+      </c>
+      <c r="X42" s="38" t="s">
+        <v>454</v>
+      </c>
+      <c r="Y42" s="38" t="s">
+        <v>455</v>
+      </c>
+      <c r="Z42" s="38" t="s">
+        <v>456</v>
+      </c>
+      <c r="AA42" s="38" t="s">
+        <v>457</v>
+      </c>
+      <c r="AB42" s="38" t="s">
+        <v>458</v>
+      </c>
+      <c r="AC42" s="38" t="s">
+        <v>459</v>
+      </c>
+      <c r="AD42" s="38" t="s">
+        <v>460</v>
+      </c>
       <c r="AE42" s="57">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="AF42" s="57" t="s">
         <v>256</v>
@@ -5909,29 +5901,27 @@
         <v>70</v>
       </c>
       <c r="AH42" s="39" t="s">
-        <v>287</v>
+        <v>539</v>
       </c>
       <c r="AI42" s="39" t="s">
-        <v>567</v>
+        <v>540</v>
       </c>
       <c r="AJ42" s="39"/>
       <c r="AK42" s="30">
-        <v>0.08</v>
-      </c>
-      <c r="AL42" s="30">
-        <v>6.9000000000000006E-2</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="AL42" s="30"/>
       <c r="AM42" s="30">
-        <v>4.0800000000000003E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AN42" s="30">
-        <v>2.4E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AO42" s="37"/>
     </row>
     <row r="43" spans="1:41" s="60" customFormat="1">
       <c r="A43" s="40" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B43" s="40"/>
       <c r="C43" s="40"/>
@@ -5972,17 +5962,17 @@
         <v>70</v>
       </c>
       <c r="AH43" s="39" t="s">
-        <v>198</v>
+        <v>102</v>
       </c>
       <c r="AI43" s="41" t="s">
-        <v>201</v>
+        <v>107</v>
       </c>
       <c r="AJ43" s="41"/>
       <c r="AK43" s="28">
         <v>0.1</v>
       </c>
-      <c r="AL43" s="28">
-        <v>1.4999999999999999E-2</v>
+      <c r="AL43" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="AM43" s="28">
         <v>1.14E-2</v>
@@ -5994,13 +5984,23 @@
     </row>
     <row r="44" spans="1:41" s="60" customFormat="1">
       <c r="A44" s="38" t="s">
-        <v>528</v>
-      </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
+        <v>263</v>
+      </c>
+      <c r="B44" s="38" t="s">
+        <v>286</v>
+      </c>
+      <c r="C44" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="D44" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="E44" s="38" t="s">
+        <v>526</v>
+      </c>
+      <c r="F44" s="38" t="s">
+        <v>527</v>
+      </c>
       <c r="G44" s="40"/>
       <c r="H44" s="40"/>
       <c r="I44" s="40"/>
@@ -6026,7 +6026,7 @@
       <c r="AC44" s="40"/>
       <c r="AD44" s="40"/>
       <c r="AE44" s="57">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AF44" s="57" t="s">
         <v>256</v>
@@ -6035,12 +6035,12 @@
         <v>70</v>
       </c>
       <c r="AH44" s="39" t="s">
-        <v>529</v>
-      </c>
-      <c r="AI44" s="41" t="s">
-        <v>568</v>
-      </c>
-      <c r="AJ44" s="41"/>
+        <v>287</v>
+      </c>
+      <c r="AI44" s="39" t="s">
+        <v>567</v>
+      </c>
+      <c r="AJ44" s="39"/>
       <c r="AK44" s="30">
         <v>0.08</v>
       </c>
@@ -6056,55 +6056,73 @@
       <c r="AO44" s="37"/>
     </row>
     <row r="45" spans="1:41" s="60" customFormat="1">
-      <c r="A45" s="47"/>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="47"/>
-      <c r="M45" s="47"/>
-      <c r="N45" s="47"/>
-      <c r="O45" s="47"/>
-      <c r="P45" s="47"/>
-      <c r="Q45" s="47"/>
-      <c r="R45" s="47"/>
-      <c r="S45" s="47"/>
-      <c r="T45" s="47"/>
-      <c r="U45" s="47"/>
-      <c r="V45" s="47"/>
-      <c r="W45" s="47"/>
-      <c r="X45" s="47"/>
-      <c r="Y45" s="47"/>
-      <c r="Z45" s="47"/>
-      <c r="AA45" s="47"/>
-      <c r="AB45" s="47"/>
-      <c r="AC45" s="47"/>
-      <c r="AD45" s="47"/>
-      <c r="AE45" s="62"/>
-      <c r="AF45" s="62"/>
-      <c r="AG45" s="62"/>
-      <c r="AH45" s="49"/>
-      <c r="AI45" s="49"/>
-      <c r="AJ45" s="49"/>
-      <c r="AK45" s="32"/>
-      <c r="AL45" s="32"/>
-      <c r="AM45" s="32"/>
-      <c r="AN45" s="32"/>
-      <c r="AO45" s="48"/>
+      <c r="A45" s="40" t="s">
+        <v>326</v>
+      </c>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="40"/>
+      <c r="N45" s="40"/>
+      <c r="O45" s="40"/>
+      <c r="P45" s="40"/>
+      <c r="Q45" s="40"/>
+      <c r="R45" s="40"/>
+      <c r="S45" s="40"/>
+      <c r="T45" s="40"/>
+      <c r="U45" s="40"/>
+      <c r="V45" s="40"/>
+      <c r="W45" s="40"/>
+      <c r="X45" s="40"/>
+      <c r="Y45" s="40"/>
+      <c r="Z45" s="40"/>
+      <c r="AA45" s="40"/>
+      <c r="AB45" s="40"/>
+      <c r="AC45" s="40"/>
+      <c r="AD45" s="40"/>
+      <c r="AE45" s="57">
+        <v>1</v>
+      </c>
+      <c r="AF45" s="57" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG45" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH45" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI45" s="41" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ45" s="41"/>
+      <c r="AK45" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="AL45" s="28">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AM45" s="28">
+        <v>1.14E-2</v>
+      </c>
+      <c r="AN45" s="28">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="AO45" s="37"/>
     </row>
     <row r="46" spans="1:41" s="60" customFormat="1">
-      <c r="A46" s="40" t="s">
-        <v>514</v>
-      </c>
-      <c r="B46" s="40" t="s">
-        <v>515</v>
-      </c>
+      <c r="A46" s="38" t="s">
+        <v>528</v>
+      </c>
+      <c r="B46" s="40"/>
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
       <c r="E46" s="40"/>
@@ -6134,32 +6152,32 @@
       <c r="AC46" s="40"/>
       <c r="AD46" s="40"/>
       <c r="AE46" s="57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF46" s="57" t="s">
-        <v>415</v>
+        <v>256</v>
       </c>
       <c r="AG46" s="57" t="s">
-        <v>416</v>
+        <v>70</v>
       </c>
       <c r="AH46" s="39" t="s">
-        <v>417</v>
-      </c>
-      <c r="AI46" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="AJ46" s="46"/>
-      <c r="AK46" s="28">
-        <v>0.21</v>
-      </c>
-      <c r="AL46" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="AM46" s="28">
-        <v>0.18</v>
-      </c>
-      <c r="AN46" s="28" t="s">
-        <v>125</v>
+        <v>529</v>
+      </c>
+      <c r="AI46" s="41" t="s">
+        <v>568</v>
+      </c>
+      <c r="AJ46" s="41"/>
+      <c r="AK46" s="30">
+        <v>0.08</v>
+      </c>
+      <c r="AL46" s="30">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AM46" s="30">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="AN46" s="30">
+        <v>2.4E-2</v>
       </c>
       <c r="AO46" s="37"/>
     </row>
@@ -6200,17 +6218,19 @@
       <c r="AH47" s="49"/>
       <c r="AI47" s="49"/>
       <c r="AJ47" s="49"/>
-      <c r="AK47" s="36"/>
-      <c r="AL47" s="36"/>
-      <c r="AM47" s="36"/>
-      <c r="AN47" s="36"/>
+      <c r="AK47" s="32"/>
+      <c r="AL47" s="32"/>
+      <c r="AM47" s="32"/>
+      <c r="AN47" s="32"/>
       <c r="AO47" s="48"/>
     </row>
     <row r="48" spans="1:41" s="60" customFormat="1">
       <c r="A48" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="B48" s="40"/>
+        <v>514</v>
+      </c>
+      <c r="B48" s="40" t="s">
+        <v>515</v>
+      </c>
       <c r="C48" s="40"/>
       <c r="D48" s="40"/>
       <c r="E48" s="40"/>
@@ -6240,101 +6260,81 @@
       <c r="AC48" s="40"/>
       <c r="AD48" s="40"/>
       <c r="AE48" s="57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF48" s="57" t="s">
-        <v>343</v>
+        <v>415</v>
       </c>
       <c r="AG48" s="57" t="s">
-        <v>258</v>
+        <v>416</v>
       </c>
       <c r="AH48" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI48" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ48" s="50"/>
+        <v>417</v>
+      </c>
+      <c r="AI48" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ48" s="46"/>
       <c r="AK48" s="28">
-        <v>15.75</v>
+        <v>0.21</v>
       </c>
       <c r="AL48" s="28">
-        <v>14.318</v>
+        <v>0.2</v>
       </c>
       <c r="AM48" s="28">
-        <v>12.170299999999999</v>
-      </c>
-      <c r="AN48" s="28">
-        <v>9.5214700000000008</v>
+        <v>0.18</v>
+      </c>
+      <c r="AN48" s="28" t="s">
+        <v>125</v>
       </c>
       <c r="AO48" s="37"/>
     </row>
     <row r="49" spans="1:41" s="60" customFormat="1">
-      <c r="A49" s="40" t="s">
-        <v>410</v>
-      </c>
-      <c r="B49" s="40"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="40"/>
-      <c r="J49" s="40"/>
-      <c r="K49" s="40"/>
-      <c r="L49" s="40"/>
-      <c r="M49" s="40"/>
-      <c r="N49" s="40"/>
-      <c r="O49" s="40"/>
-      <c r="P49" s="40"/>
-      <c r="Q49" s="40"/>
-      <c r="R49" s="40"/>
-      <c r="S49" s="40"/>
-      <c r="T49" s="40"/>
-      <c r="U49" s="40"/>
-      <c r="V49" s="40"/>
-      <c r="W49" s="40"/>
-      <c r="X49" s="40"/>
-      <c r="Y49" s="40"/>
-      <c r="Z49" s="40"/>
-      <c r="AA49" s="40"/>
-      <c r="AB49" s="40"/>
-      <c r="AC49" s="40"/>
-      <c r="AD49" s="40"/>
-      <c r="AE49" s="57">
-        <v>1</v>
-      </c>
-      <c r="AF49" s="57" t="s">
-        <v>548</v>
-      </c>
-      <c r="AG49" s="57" t="s">
-        <v>544</v>
-      </c>
-      <c r="AH49" s="39" t="s">
-        <v>543</v>
-      </c>
-      <c r="AI49" s="50" t="s">
-        <v>571</v>
-      </c>
-      <c r="AJ49" s="50"/>
-      <c r="AK49" s="28">
-        <v>0.61</v>
-      </c>
-      <c r="AL49" s="28">
-        <v>0.51</v>
-      </c>
-      <c r="AM49" s="28">
-        <v>0.39</v>
-      </c>
-      <c r="AN49" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="AO49" s="37"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="47"/>
+      <c r="J49" s="47"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="47"/>
+      <c r="N49" s="47"/>
+      <c r="O49" s="47"/>
+      <c r="P49" s="47"/>
+      <c r="Q49" s="47"/>
+      <c r="R49" s="47"/>
+      <c r="S49" s="47"/>
+      <c r="T49" s="47"/>
+      <c r="U49" s="47"/>
+      <c r="V49" s="47"/>
+      <c r="W49" s="47"/>
+      <c r="X49" s="47"/>
+      <c r="Y49" s="47"/>
+      <c r="Z49" s="47"/>
+      <c r="AA49" s="47"/>
+      <c r="AB49" s="47"/>
+      <c r="AC49" s="47"/>
+      <c r="AD49" s="47"/>
+      <c r="AE49" s="62"/>
+      <c r="AF49" s="62"/>
+      <c r="AG49" s="62"/>
+      <c r="AH49" s="49"/>
+      <c r="AI49" s="49"/>
+      <c r="AJ49" s="49"/>
+      <c r="AK49" s="36"/>
+      <c r="AL49" s="36"/>
+      <c r="AM49" s="36"/>
+      <c r="AN49" s="36"/>
+      <c r="AO49" s="48"/>
     </row>
     <row r="50" spans="1:41" s="60" customFormat="1">
       <c r="A50" s="40" t="s">
-        <v>421</v>
+        <v>255</v>
       </c>
       <c r="B50" s="40"/>
       <c r="C50" s="40"/>
@@ -6369,35 +6369,35 @@
         <v>1</v>
       </c>
       <c r="AF50" s="57" t="s">
-        <v>545</v>
+        <v>343</v>
       </c>
       <c r="AG50" s="57" t="s">
-        <v>546</v>
+        <v>258</v>
       </c>
       <c r="AH50" s="39" t="s">
-        <v>547</v>
+        <v>18</v>
       </c>
       <c r="AI50" s="50" t="s">
-        <v>572</v>
-      </c>
-      <c r="AJ50" s="57"/>
+        <v>24</v>
+      </c>
+      <c r="AJ50" s="50"/>
       <c r="AK50" s="28">
-        <v>0.97</v>
+        <v>15.75</v>
       </c>
       <c r="AL50" s="28">
-        <v>8.6199999999999999E-2</v>
+        <v>14.318</v>
       </c>
       <c r="AM50" s="28">
-        <v>0.72</v>
-      </c>
-      <c r="AN50" s="28" t="s">
-        <v>26</v>
+        <v>12.170299999999999</v>
+      </c>
+      <c r="AN50" s="28">
+        <v>9.5214700000000008</v>
       </c>
       <c r="AO50" s="37"/>
     </row>
     <row r="51" spans="1:41" s="60" customFormat="1">
       <c r="A51" s="40" t="s">
-        <v>328</v>
+        <v>410</v>
       </c>
       <c r="B51" s="40"/>
       <c r="C51" s="40"/>
@@ -6432,35 +6432,35 @@
         <v>1</v>
       </c>
       <c r="AF51" s="57" t="s">
-        <v>329</v>
+        <v>548</v>
       </c>
       <c r="AG51" s="57" t="s">
-        <v>330</v>
+        <v>544</v>
       </c>
       <c r="AH51" s="39" t="s">
-        <v>549</v>
-      </c>
-      <c r="AI51" s="46" t="s">
-        <v>573</v>
-      </c>
-      <c r="AJ51" s="46"/>
+        <v>543</v>
+      </c>
+      <c r="AI51" s="50" t="s">
+        <v>571</v>
+      </c>
+      <c r="AJ51" s="50"/>
       <c r="AK51" s="28">
-        <v>0.79</v>
+        <v>0.61</v>
       </c>
       <c r="AL51" s="28">
-        <v>0.61299999999999999</v>
+        <v>0.51</v>
       </c>
       <c r="AM51" s="28">
-        <v>0.39600000000000002</v>
-      </c>
-      <c r="AN51" s="28">
-        <v>0.317</v>
+        <v>0.39</v>
+      </c>
+      <c r="AN51" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="AO51" s="37"/>
     </row>
     <row r="52" spans="1:41" s="60" customFormat="1">
       <c r="A52" s="40" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
       <c r="B52" s="40"/>
       <c r="C52" s="40"/>
@@ -6495,35 +6495,35 @@
         <v>1</v>
       </c>
       <c r="AF52" s="57" t="s">
-        <v>407</v>
+        <v>545</v>
       </c>
       <c r="AG52" s="57" t="s">
-        <v>408</v>
+        <v>546</v>
       </c>
       <c r="AH52" s="39" t="s">
-        <v>409</v>
-      </c>
-      <c r="AI52" s="55" t="s">
-        <v>219</v>
-      </c>
-      <c r="AJ52" s="55"/>
-      <c r="AK52" s="31">
-        <v>1.82</v>
-      </c>
-      <c r="AL52" s="31">
-        <v>1.7290000000000001</v>
-      </c>
-      <c r="AM52" s="31">
-        <v>1.5556000000000001</v>
-      </c>
-      <c r="AN52" s="31" t="s">
+        <v>547</v>
+      </c>
+      <c r="AI52" s="50" t="s">
+        <v>572</v>
+      </c>
+      <c r="AJ52" s="57"/>
+      <c r="AK52" s="28">
+        <v>0.97</v>
+      </c>
+      <c r="AL52" s="28">
+        <v>8.6199999999999999E-2</v>
+      </c>
+      <c r="AM52" s="28">
+        <v>0.72</v>
+      </c>
+      <c r="AN52" s="28" t="s">
         <v>26</v>
       </c>
       <c r="AO52" s="37"/>
     </row>
-    <row r="53" spans="1:41" s="60" customFormat="1" ht="15" customHeight="1">
+    <row r="53" spans="1:41" s="60" customFormat="1">
       <c r="A53" s="40" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="B53" s="40"/>
       <c r="C53" s="40"/>
@@ -6558,45 +6558,39 @@
         <v>1</v>
       </c>
       <c r="AF53" s="57" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="AG53" s="57" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="AH53" s="39" t="s">
-        <v>350</v>
-      </c>
-      <c r="AI53" s="55" t="s">
-        <v>226</v>
-      </c>
-      <c r="AJ53" s="55"/>
-      <c r="AK53" s="31">
-        <v>6.97</v>
-      </c>
-      <c r="AL53" s="31">
-        <v>6.26</v>
-      </c>
-      <c r="AM53" s="31">
-        <v>5.157</v>
-      </c>
-      <c r="AN53" s="31">
-        <v>3.375</v>
+        <v>549</v>
+      </c>
+      <c r="AI53" s="46" t="s">
+        <v>573</v>
+      </c>
+      <c r="AJ53" s="46"/>
+      <c r="AK53" s="28">
+        <v>0.79</v>
+      </c>
+      <c r="AL53" s="28">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="AM53" s="28">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="AN53" s="28">
+        <v>0.317</v>
       </c>
       <c r="AO53" s="37"/>
     </row>
     <row r="54" spans="1:41" s="60" customFormat="1">
       <c r="A54" s="40" t="s">
-        <v>371</v>
-      </c>
-      <c r="B54" s="40" t="s">
-        <v>372</v>
-      </c>
-      <c r="C54" s="40" t="s">
-        <v>373</v>
-      </c>
-      <c r="D54" s="40" t="s">
-        <v>374</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
       <c r="E54" s="40"/>
       <c r="F54" s="40"/>
       <c r="G54" s="40"/>
@@ -6624,38 +6618,38 @@
       <c r="AC54" s="40"/>
       <c r="AD54" s="40"/>
       <c r="AE54" s="57">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AF54" s="57" t="s">
-        <v>375</v>
+        <v>407</v>
       </c>
       <c r="AG54" s="57" t="s">
-        <v>376</v>
+        <v>408</v>
       </c>
       <c r="AH54" s="39" t="s">
-        <v>377</v>
-      </c>
-      <c r="AI54" s="56" t="s">
-        <v>253</v>
-      </c>
-      <c r="AJ54" s="56"/>
+        <v>409</v>
+      </c>
+      <c r="AI54" s="55" t="s">
+        <v>219</v>
+      </c>
+      <c r="AJ54" s="55"/>
       <c r="AK54" s="31">
-        <v>0.9</v>
+        <v>1.82</v>
       </c>
       <c r="AL54" s="31">
-        <v>0.79800000000000004</v>
+        <v>1.7290000000000001</v>
       </c>
       <c r="AM54" s="31">
-        <v>0.63</v>
-      </c>
-      <c r="AN54" s="31">
-        <v>0.38750000000000001</v>
+        <v>1.5556000000000001</v>
+      </c>
+      <c r="AN54" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="AO54" s="37"/>
     </row>
-    <row r="55" spans="1:41" s="60" customFormat="1">
+    <row r="55" spans="1:41" s="60" customFormat="1" ht="15" customHeight="1">
       <c r="A55" s="40" t="s">
-        <v>392</v>
+        <v>347</v>
       </c>
       <c r="B55" s="40"/>
       <c r="C55" s="40"/>
@@ -6690,39 +6684,45 @@
         <v>1</v>
       </c>
       <c r="AF55" s="57" t="s">
-        <v>395</v>
+        <v>348</v>
       </c>
       <c r="AG55" s="57" t="s">
-        <v>394</v>
+        <v>349</v>
       </c>
       <c r="AH55" s="39" t="s">
-        <v>393</v>
-      </c>
-      <c r="AI55" s="39" t="s">
-        <v>574</v>
-      </c>
-      <c r="AJ55" s="39"/>
-      <c r="AK55" s="30">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="AL55" s="30">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="AM55" s="30">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="AN55" s="30">
-        <v>0.21657999999999999</v>
+        <v>350</v>
+      </c>
+      <c r="AI55" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="AJ55" s="55"/>
+      <c r="AK55" s="31">
+        <v>6.97</v>
+      </c>
+      <c r="AL55" s="31">
+        <v>6.26</v>
+      </c>
+      <c r="AM55" s="31">
+        <v>5.157</v>
+      </c>
+      <c r="AN55" s="31">
+        <v>3.375</v>
       </c>
       <c r="AO55" s="37"/>
     </row>
     <row r="56" spans="1:41" s="60" customFormat="1">
       <c r="A56" s="40" t="s">
-        <v>344</v>
-      </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
+        <v>371</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>372</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>373</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>374</v>
+      </c>
       <c r="E56" s="40"/>
       <c r="F56" s="40"/>
       <c r="G56" s="40"/>
@@ -6750,38 +6750,38 @@
       <c r="AC56" s="40"/>
       <c r="AD56" s="40"/>
       <c r="AE56" s="57">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AF56" s="57" t="s">
-        <v>345</v>
-      </c>
-      <c r="AG56" s="57"/>
+        <v>375</v>
+      </c>
+      <c r="AG56" s="57" t="s">
+        <v>376</v>
+      </c>
       <c r="AH56" s="39" t="s">
-        <v>346</v>
-      </c>
-      <c r="AI56" s="39" t="s">
-        <v>575</v>
-      </c>
-      <c r="AJ56" s="57" t="s">
-        <v>576</v>
-      </c>
-      <c r="AK56" s="30">
-        <v>1.88</v>
-      </c>
-      <c r="AL56" s="30">
-        <v>1.704</v>
-      </c>
-      <c r="AM56" s="30">
-        <v>1.4608000000000001</v>
-      </c>
-      <c r="AN56" s="30">
-        <v>1.0229999999999999</v>
+        <v>377</v>
+      </c>
+      <c r="AI56" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ56" s="56"/>
+      <c r="AK56" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="AL56" s="31">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="AM56" s="31">
+        <v>0.63</v>
+      </c>
+      <c r="AN56" s="31">
+        <v>0.38750000000000001</v>
       </c>
       <c r="AO56" s="37"/>
     </row>
     <row r="57" spans="1:41" s="60" customFormat="1">
       <c r="A57" s="40" t="s">
-        <v>427</v>
+        <v>392</v>
       </c>
       <c r="B57" s="40"/>
       <c r="C57" s="40"/>
@@ -6816,78 +6816,98 @@
         <v>1</v>
       </c>
       <c r="AF57" s="57" t="s">
-        <v>428</v>
+        <v>395</v>
       </c>
       <c r="AG57" s="57" t="s">
-        <v>429</v>
+        <v>394</v>
       </c>
       <c r="AH57" s="39" t="s">
-        <v>430</v>
+        <v>393</v>
       </c>
       <c r="AI57" s="39" t="s">
-        <v>577</v>
-      </c>
-      <c r="AJ57" s="57"/>
+        <v>574</v>
+      </c>
+      <c r="AJ57" s="39"/>
       <c r="AK57" s="30">
-        <v>1.86</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL57" s="30">
-        <v>1.55</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="AM57" s="30">
-        <v>1.18</v>
-      </c>
-      <c r="AN57" s="30" t="s">
-        <v>26</v>
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="AN57" s="30">
+        <v>0.21657999999999999</v>
       </c>
       <c r="AO57" s="37"/>
     </row>
     <row r="58" spans="1:41" s="60" customFormat="1">
-      <c r="A58" s="47"/>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="47"/>
-      <c r="J58" s="47"/>
-      <c r="K58" s="47"/>
-      <c r="L58" s="47"/>
-      <c r="M58" s="47"/>
-      <c r="N58" s="47"/>
-      <c r="O58" s="47"/>
-      <c r="P58" s="47"/>
-      <c r="Q58" s="47"/>
-      <c r="R58" s="47"/>
-      <c r="S58" s="47"/>
-      <c r="T58" s="47"/>
-      <c r="U58" s="47"/>
-      <c r="V58" s="47"/>
-      <c r="W58" s="47"/>
-      <c r="X58" s="47"/>
-      <c r="Y58" s="47"/>
-      <c r="Z58" s="47"/>
-      <c r="AA58" s="47"/>
-      <c r="AB58" s="47"/>
-      <c r="AC58" s="47"/>
-      <c r="AD58" s="47"/>
-      <c r="AE58" s="62"/>
-      <c r="AF58" s="62"/>
-      <c r="AG58" s="62"/>
-      <c r="AH58" s="49"/>
-      <c r="AI58" s="49"/>
-      <c r="AJ58" s="49"/>
-      <c r="AK58" s="33"/>
-      <c r="AL58" s="33"/>
-      <c r="AM58" s="33"/>
-      <c r="AN58" s="33"/>
-      <c r="AO58" s="48"/>
-    </row>
-    <row r="59" spans="1:41">
+      <c r="A58" s="40" t="s">
+        <v>344</v>
+      </c>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="40"/>
+      <c r="K58" s="40"/>
+      <c r="L58" s="40"/>
+      <c r="M58" s="40"/>
+      <c r="N58" s="40"/>
+      <c r="O58" s="40"/>
+      <c r="P58" s="40"/>
+      <c r="Q58" s="40"/>
+      <c r="R58" s="40"/>
+      <c r="S58" s="40"/>
+      <c r="T58" s="40"/>
+      <c r="U58" s="40"/>
+      <c r="V58" s="40"/>
+      <c r="W58" s="40"/>
+      <c r="X58" s="40"/>
+      <c r="Y58" s="40"/>
+      <c r="Z58" s="40"/>
+      <c r="AA58" s="40"/>
+      <c r="AB58" s="40"/>
+      <c r="AC58" s="40"/>
+      <c r="AD58" s="40"/>
+      <c r="AE58" s="57">
+        <v>1</v>
+      </c>
+      <c r="AF58" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="AG58" s="57"/>
+      <c r="AH58" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="AI58" s="39" t="s">
+        <v>575</v>
+      </c>
+      <c r="AJ58" s="57" t="s">
+        <v>576</v>
+      </c>
+      <c r="AK58" s="30">
+        <v>1.88</v>
+      </c>
+      <c r="AL58" s="30">
+        <v>1.704</v>
+      </c>
+      <c r="AM58" s="30">
+        <v>1.4608000000000001</v>
+      </c>
+      <c r="AN58" s="30">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="AO58" s="37"/>
+    </row>
+    <row r="59" spans="1:41" s="60" customFormat="1">
       <c r="A59" s="40" t="s">
-        <v>331</v>
+        <v>427</v>
       </c>
       <c r="B59" s="40"/>
       <c r="C59" s="40"/>
@@ -6922,92 +6942,198 @@
         <v>1</v>
       </c>
       <c r="AF59" s="57" t="s">
+        <v>428</v>
+      </c>
+      <c r="AG59" s="57" t="s">
+        <v>429</v>
+      </c>
+      <c r="AH59" s="39" t="s">
+        <v>430</v>
+      </c>
+      <c r="AI59" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="AJ59" s="57"/>
+      <c r="AK59" s="30">
+        <v>1.86</v>
+      </c>
+      <c r="AL59" s="30">
+        <v>1.55</v>
+      </c>
+      <c r="AM59" s="30">
+        <v>1.18</v>
+      </c>
+      <c r="AN59" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO59" s="37"/>
+    </row>
+    <row r="60" spans="1:41" s="60" customFormat="1">
+      <c r="A60" s="47"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="47"/>
+      <c r="J60" s="47"/>
+      <c r="K60" s="47"/>
+      <c r="L60" s="47"/>
+      <c r="M60" s="47"/>
+      <c r="N60" s="47"/>
+      <c r="O60" s="47"/>
+      <c r="P60" s="47"/>
+      <c r="Q60" s="47"/>
+      <c r="R60" s="47"/>
+      <c r="S60" s="47"/>
+      <c r="T60" s="47"/>
+      <c r="U60" s="47"/>
+      <c r="V60" s="47"/>
+      <c r="W60" s="47"/>
+      <c r="X60" s="47"/>
+      <c r="Y60" s="47"/>
+      <c r="Z60" s="47"/>
+      <c r="AA60" s="47"/>
+      <c r="AB60" s="47"/>
+      <c r="AC60" s="47"/>
+      <c r="AD60" s="47"/>
+      <c r="AE60" s="62"/>
+      <c r="AF60" s="62"/>
+      <c r="AG60" s="62"/>
+      <c r="AH60" s="49"/>
+      <c r="AI60" s="49"/>
+      <c r="AJ60" s="49"/>
+      <c r="AK60" s="33"/>
+      <c r="AL60" s="33"/>
+      <c r="AM60" s="33"/>
+      <c r="AN60" s="33"/>
+      <c r="AO60" s="48"/>
+    </row>
+    <row r="61" spans="1:41">
+      <c r="A61" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="40"/>
+      <c r="J61" s="40"/>
+      <c r="K61" s="40"/>
+      <c r="L61" s="40"/>
+      <c r="M61" s="40"/>
+      <c r="N61" s="40"/>
+      <c r="O61" s="40"/>
+      <c r="P61" s="40"/>
+      <c r="Q61" s="40"/>
+      <c r="R61" s="40"/>
+      <c r="S61" s="40"/>
+      <c r="T61" s="40"/>
+      <c r="U61" s="40"/>
+      <c r="V61" s="40"/>
+      <c r="W61" s="40"/>
+      <c r="X61" s="40"/>
+      <c r="Y61" s="40"/>
+      <c r="Z61" s="40"/>
+      <c r="AA61" s="40"/>
+      <c r="AB61" s="40"/>
+      <c r="AC61" s="40"/>
+      <c r="AD61" s="40"/>
+      <c r="AE61" s="57">
+        <v>1</v>
+      </c>
+      <c r="AF61" s="57" t="s">
         <v>332</v>
       </c>
-      <c r="AG59" s="57"/>
-      <c r="AH59" s="39" t="s">
+      <c r="AG61" s="57"/>
+      <c r="AH61" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="AI59" s="55" t="s">
+      <c r="AI61" s="55" t="s">
         <v>231</v>
       </c>
-      <c r="AJ59" s="55"/>
-      <c r="AK59" s="31">
+      <c r="AJ61" s="55"/>
+      <c r="AK61" s="31">
         <v>0.73</v>
       </c>
-      <c r="AL59" s="31">
+      <c r="AL61" s="31">
         <v>0.65</v>
       </c>
-      <c r="AM59" s="31">
+      <c r="AM61" s="31">
         <v>0.53800000000000003</v>
       </c>
-      <c r="AN59" s="31">
+      <c r="AN61" s="31">
         <v>0.42502000000000001</v>
       </c>
-      <c r="AO59" s="37"/>
-    </row>
-    <row r="60" spans="1:41">
-      <c r="A60" s="40" t="s">
+      <c r="AO61" s="37"/>
+    </row>
+    <row r="62" spans="1:41">
+      <c r="A62" s="40" t="s">
         <v>412</v>
       </c>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="40"/>
-      <c r="L60" s="40"/>
-      <c r="M60" s="40"/>
-      <c r="N60" s="40"/>
-      <c r="O60" s="40"/>
-      <c r="P60" s="40"/>
-      <c r="Q60" s="40"/>
-      <c r="R60" s="40"/>
-      <c r="S60" s="40"/>
-      <c r="T60" s="40"/>
-      <c r="U60" s="40"/>
-      <c r="V60" s="40"/>
-      <c r="W60" s="40"/>
-      <c r="X60" s="40"/>
-      <c r="Y60" s="40"/>
-      <c r="Z60" s="40"/>
-      <c r="AA60" s="40"/>
-      <c r="AB60" s="40"/>
-      <c r="AC60" s="40"/>
-      <c r="AD60" s="40"/>
-      <c r="AE60" s="57">
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="40"/>
+      <c r="J62" s="40"/>
+      <c r="K62" s="40"/>
+      <c r="L62" s="40"/>
+      <c r="M62" s="40"/>
+      <c r="N62" s="40"/>
+      <c r="O62" s="40"/>
+      <c r="P62" s="40"/>
+      <c r="Q62" s="40"/>
+      <c r="R62" s="40"/>
+      <c r="S62" s="40"/>
+      <c r="T62" s="40"/>
+      <c r="U62" s="40"/>
+      <c r="V62" s="40"/>
+      <c r="W62" s="40"/>
+      <c r="X62" s="40"/>
+      <c r="Y62" s="40"/>
+      <c r="Z62" s="40"/>
+      <c r="AA62" s="40"/>
+      <c r="AB62" s="40"/>
+      <c r="AC62" s="40"/>
+      <c r="AD62" s="40"/>
+      <c r="AE62" s="57">
         <v>1</v>
       </c>
-      <c r="AF60" s="57" t="s">
+      <c r="AF62" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="AG60" s="57" t="s">
+      <c r="AG62" s="57" t="s">
         <v>413</v>
       </c>
-      <c r="AH60" s="39" t="s">
+      <c r="AH62" s="39" t="s">
         <v>414</v>
       </c>
-      <c r="AI60" s="41" t="s">
+      <c r="AI62" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="AJ60" s="41"/>
-      <c r="AK60" s="64">
+      <c r="AJ62" s="41"/>
+      <c r="AK62" s="64">
         <v>0.95</v>
       </c>
-      <c r="AL60" s="64">
+      <c r="AL62" s="64">
         <v>0.84</v>
       </c>
-      <c r="AM60" s="64">
+      <c r="AM62" s="64">
         <v>0.69</v>
       </c>
-      <c r="AN60" s="64">
+      <c r="AN62" s="64">
         <v>0.54</v>
       </c>
-      <c r="AO60" s="37"/>
+      <c r="AO62" s="37"/>
     </row>
   </sheetData>
   <sortState ref="A19:AP30">
@@ -7027,7 +7153,7 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="AG6 AG29 AG3 AG34 AG36:AG37 AG43 AG8:AG13" numberStoredAsText="1"/>
+    <ignoredError sqref="AG6 AG31 AG3 AG36 AG38:AG39 AG45 AG8:AG13" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -7062,54 +7188,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="80" t="s">
+      <c r="G1" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="81" t="s">
+      <c r="I1" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="82"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
@@ -8731,17 +8857,17 @@
     <sortCondition ref="B3:B46"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>

<commit_message>
Added component description field to spread sheet
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="22040" windowWidth="26760" windowHeight="17120" tabRatio="986"/>
+    <workbookView xWindow="5160" yWindow="0" windowWidth="19620" windowHeight="16280" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="475">
   <si>
     <t>Part</t>
   </si>
@@ -1117,9 +1117,6 @@
     <t>BSS84CT-ND</t>
   </si>
   <si>
-    <t>Don’t forget to change resistor values from 50 to 51</t>
-  </si>
-  <si>
     <t>51</t>
   </si>
   <si>
@@ -1138,9 +1135,6 @@
     <t>MCT0603-4.70K-CFCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">	MCT0603-10.0K-CFCT-ND</t>
-  </si>
-  <si>
     <t>MCT0603-100K-CFCT-ND</t>
   </si>
   <si>
@@ -1276,12 +1270,6 @@
     <t>VJ0603A100JXQPW1BC</t>
   </si>
   <si>
-    <t>1276-1282-1-ND</t>
-  </si>
-  <si>
-    <t>CL10C4R7CB8NNNC</t>
-  </si>
-  <si>
     <t>490-1494-1-ND</t>
   </si>
   <si>
@@ -1355,6 +1343,108 @@
   </si>
   <si>
     <t>C0603C100J5GACTU</t>
+  </si>
+  <si>
+    <t>CAP CER 10PF 50V 5% NP0 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 11PF 50V 5% NP0 0603</t>
+  </si>
+  <si>
+    <t>311-1455-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 10V 10% X5R 0603</t>
+  </si>
+  <si>
+    <t>CC0603KRX5R6BB475</t>
+  </si>
+  <si>
+    <t>for v2 might need to find x7r temp rated cap</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 50V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3.3VWM 8.1VC 14-DFN</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A DUAL 6POS GOLD</t>
+  </si>
+  <si>
+    <t>CONN HEADER 8POS .100 R/A 15AU</t>
+  </si>
+  <si>
+    <t>CONN HEADER 20POS .100 R/A 15AU</t>
+  </si>
+  <si>
+    <t>Connector Receptacle USB - micro B 2.0 5 Position Surface Mount, Right Angle, Horizontal</t>
+  </si>
+  <si>
+    <t>FIXED IND 2.2UH 1.6A 94 MOHM SMD</t>
+  </si>
+  <si>
+    <t>LED 1.6X1.2MM B/R/G WTR/CLR SMD</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 50V 130MA SOT-23</t>
+  </si>
+  <si>
+    <t>RES SMD 51 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 120 OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 7.5K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>MCT0603-10.0K-CFCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>IC REG LDO 3.3V 0.5A SOT223-3</t>
+  </si>
+  <si>
+    <t>IC REG BUCK SYNC 3.3V SOT23-5</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 1MHZ RRO 14SOIC</t>
+  </si>
+  <si>
+    <t>IC EEPROM 4KBIT 1MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>CONN MICRO SD CARD PUSH-PULL</t>
+  </si>
+  <si>
+    <t>MULTI-FREQ USB 2.0 ULPI PHY</t>
+  </si>
+  <si>
+    <t>Crystal 32.7680kHz 20ppm 6pF 55 kOhm -40°C - 85°C Surface Mount 2-SMD</t>
+  </si>
+  <si>
+    <t>Crystal 16.0000MHz 10ppm 7.2pF 80 Ohm -30°C - 85°C Surface Mount 4-SMD, No Lead (DFN, LCC)</t>
+  </si>
+  <si>
+    <t>732-5315-ND</t>
+  </si>
+  <si>
+    <t>61300211121</t>
+  </si>
+  <si>
+    <t>CONN HEADER 2 POS 2.54</t>
   </si>
 </sst>
 </file>
@@ -1405,11 +1495,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1417,8 +1502,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1446,12 +1538,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1959,7 +2045,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2043,142 +2129,60 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2196,19 +2200,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="340">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2884,2048 +2951,2209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="112.5" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.5" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="96.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="96.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="52" customFormat="1">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:14" s="37" customFormat="1">
+      <c r="A1" s="41" t="s">
         <v>254</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="41" t="s">
+        <v>413</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>414</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>341</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="43" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="37" customFormat="1" ht="15" thickBot="1">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="27">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2">
+        <v>100</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="44"/>
+    </row>
+    <row r="3" spans="1:14" s="60" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="33">
+        <v>25</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L3" s="28">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="M3" s="28">
+        <v>6.3E-3</v>
+      </c>
+      <c r="N3" s="59"/>
+    </row>
+    <row r="4" spans="1:14" s="60" customFormat="1">
+      <c r="A4" s="61">
+        <v>1</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>304</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>264</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>441</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>440</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>439</v>
+      </c>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64">
+        <v>0.26</v>
+      </c>
+      <c r="K4" s="64">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="L4" s="64">
+        <v>0.1017</v>
+      </c>
+      <c r="M4" s="64">
+        <v>0.06</v>
+      </c>
+      <c r="N4" s="65"/>
+    </row>
+    <row r="5" spans="1:14" s="60" customFormat="1">
+      <c r="A5" s="33">
+        <v>1</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="82"/>
+      <c r="G5" s="58" t="s">
         <v>415</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="H5" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>372</v>
+      </c>
+      <c r="J5" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="59" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="60" customFormat="1">
+      <c r="A6" s="33">
+        <v>3</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>392</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="84" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" s="32"/>
+      <c r="J6" s="28">
+        <v>0.32</v>
+      </c>
+      <c r="K6" s="28">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L6" s="28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M6" s="28">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="N6" s="59"/>
+    </row>
+    <row r="7" spans="1:14" s="60" customFormat="1">
+      <c r="A7" s="33">
+        <v>2</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>393</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="F7" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="G7" s="58" t="s">
+        <v>436</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="I7" s="33"/>
+      <c r="J7" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="K7" s="29">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L7" s="29">
+        <v>2.1899999999999999E-2</v>
+      </c>
+      <c r="M7" s="29">
+        <v>1.17E-2</v>
+      </c>
+      <c r="N7" s="59"/>
+    </row>
+    <row r="8" spans="1:14" s="60" customFormat="1">
+      <c r="A8" s="33">
+        <v>14</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>394</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="32"/>
+      <c r="J8" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="K8" s="28">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="L8" s="28">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="M8" s="28">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="N8" s="59"/>
+    </row>
+    <row r="9" spans="1:14" s="60" customFormat="1">
+      <c r="A9" s="33">
+        <v>3</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>395</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="32"/>
+      <c r="J9" s="28">
+        <v>0.17</v>
+      </c>
+      <c r="K9" s="28">
+        <v>0.115</v>
+      </c>
+      <c r="L9" s="28">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="M9" s="28">
+        <v>0.31630000000000003</v>
+      </c>
+      <c r="N9" s="59"/>
+    </row>
+    <row r="10" spans="1:14" s="60" customFormat="1">
+      <c r="A10" s="67">
+        <v>2</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>396</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="F10" s="85"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="38">
+        <v>0.12</v>
+      </c>
+      <c r="K10" s="38">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="L10" s="38">
+        <v>3.9E-2</v>
+      </c>
+      <c r="M10" s="38">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="N10" s="39" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="60" customFormat="1">
+      <c r="A11" s="33">
+        <v>2</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>397</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="84" t="s">
+        <v>444</v>
+      </c>
+      <c r="G11" s="58" t="s">
+        <v>445</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="I11" s="32"/>
+      <c r="J11" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="K11" s="28">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="L11" s="28">
+        <v>6.93E-2</v>
+      </c>
+      <c r="M11" s="28">
+        <v>4.2079999999999999E-2</v>
+      </c>
+      <c r="N11" s="59" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="60" customFormat="1">
+      <c r="A12" s="33">
+        <v>30</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>390</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>344</v>
+      </c>
+      <c r="F12" s="84" t="s">
+        <v>447</v>
+      </c>
+      <c r="G12" s="58" t="s">
+        <v>417</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>416</v>
+      </c>
+      <c r="J12" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L12" s="28">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="M12" s="28">
+        <v>6.1500000000000001E-3</v>
+      </c>
+      <c r="N12" s="59"/>
+    </row>
+    <row r="13" spans="1:14" s="60" customFormat="1">
+      <c r="A13" s="33">
         <v>1</v>
       </c>
-      <c r="D1" s="71" t="s">
-        <v>257</v>
-      </c>
-      <c r="E1" s="77" t="s">
-        <v>259</v>
-      </c>
-      <c r="F1" s="77" t="s">
-        <v>416</v>
-      </c>
-      <c r="G1" s="77" t="s">
-        <v>341</v>
-      </c>
-      <c r="H1" s="77" t="s">
-        <v>361</v>
-      </c>
-      <c r="I1" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="73" t="s">
+      <c r="B13" s="57" t="s">
+        <v>315</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>335</v>
+      </c>
+      <c r="F13" s="82"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="59"/>
+    </row>
+    <row r="14" spans="1:14" s="60" customFormat="1">
+      <c r="A14" s="33">
+        <v>1</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="I14" s="34"/>
+      <c r="J14" s="28">
+        <v>1.41</v>
+      </c>
+      <c r="K14" s="28">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="L14" s="28">
+        <v>0.83</v>
+      </c>
+      <c r="M14" s="28">
+        <v>0.52</v>
+      </c>
+      <c r="N14" s="59"/>
+    </row>
+    <row r="15" spans="1:14" s="60" customFormat="1">
+      <c r="A15" s="70"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="73"/>
+    </row>
+    <row r="16" spans="1:14" s="60" customFormat="1">
+      <c r="A16" s="33">
+        <v>4</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>398</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="34"/>
+      <c r="J16" s="28">
+        <v>0.4</v>
+      </c>
+      <c r="K16" s="28">
+        <v>0.31</v>
+      </c>
+      <c r="L16" s="28">
+        <v>0.216</v>
+      </c>
+      <c r="M16" s="28">
+        <v>0.11</v>
+      </c>
+      <c r="N16" s="59"/>
+    </row>
+    <row r="17" spans="1:14" s="60" customFormat="1" ht="16" customHeight="1">
+      <c r="A17" s="33">
+        <v>13</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>399</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>294</v>
+      </c>
+      <c r="F17" s="82" t="s">
+        <v>448</v>
+      </c>
+      <c r="G17" s="58" t="s">
+        <v>248</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="I17" s="25"/>
+      <c r="J17" s="29">
+        <v>0.77</v>
+      </c>
+      <c r="K17" s="29">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="L17" s="29">
+        <v>0.51990000000000003</v>
+      </c>
+      <c r="M17" s="29">
+        <v>0.30854999999999999</v>
+      </c>
+      <c r="N17" s="59"/>
+    </row>
+    <row r="18" spans="1:14" s="60" customFormat="1">
+      <c r="A18" s="70"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="73"/>
+    </row>
+    <row r="19" spans="1:14" s="60" customFormat="1">
+      <c r="A19" s="33">
+        <v>6</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>400</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="E19" s="58"/>
+      <c r="F19" s="82" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="I19" s="58"/>
+      <c r="J19" s="29">
+        <v>0.33</v>
+      </c>
+      <c r="K19" s="29">
+        <v>0.315</v>
+      </c>
+      <c r="L19" s="29">
+        <v>0.2205</v>
+      </c>
+      <c r="M19" s="29">
+        <v>0.1575</v>
+      </c>
+      <c r="N19" s="59"/>
+    </row>
+    <row r="20" spans="1:14" s="60" customFormat="1" ht="14" customHeight="1">
+      <c r="A20" s="33">
+        <v>2</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>401</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="E20" s="58"/>
+      <c r="F20" s="82" t="s">
+        <v>449</v>
+      </c>
+      <c r="G20" s="58" t="s">
+        <v>418</v>
+      </c>
+      <c r="H20" s="58" t="s">
+        <v>357</v>
+      </c>
+      <c r="I20" s="58"/>
+      <c r="J20" s="29">
+        <v>0.45</v>
+      </c>
+      <c r="K20" s="29">
+        <v>0.42</v>
+      </c>
+      <c r="L20" s="29">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M20" s="29">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="N20" s="59"/>
+    </row>
+    <row r="21" spans="1:14" s="60" customFormat="1" ht="14" customHeight="1">
+      <c r="A21" s="33">
+        <v>2</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>402</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="E21" s="58"/>
+      <c r="F21" s="84" t="s">
+        <v>450</v>
+      </c>
+      <c r="G21" s="58" t="s">
+        <v>419</v>
+      </c>
+      <c r="H21" s="58" t="s">
+        <v>358</v>
+      </c>
+      <c r="I21" s="58"/>
+      <c r="J21" s="29">
+        <v>0.45</v>
+      </c>
+      <c r="K21" s="29">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L21" s="29">
+        <v>0.32379999999999998</v>
+      </c>
+      <c r="M21" s="29">
+        <v>0.23232</v>
+      </c>
+      <c r="N21" s="59"/>
+    </row>
+    <row r="22" spans="1:14" s="60" customFormat="1">
+      <c r="A22" s="33">
+        <v>4</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>403</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="E22" s="58"/>
+      <c r="F22" s="82" t="s">
+        <v>451</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>420</v>
+      </c>
+      <c r="H22" s="58" t="s">
+        <v>359</v>
+      </c>
+      <c r="I22" s="58"/>
+      <c r="J22" s="29">
+        <v>0.77</v>
+      </c>
+      <c r="K22" s="29">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="L22" s="29">
+        <v>0.58209999999999995</v>
+      </c>
+      <c r="M22" s="29">
+        <v>0.42336000000000001</v>
+      </c>
+      <c r="N22" s="59"/>
+    </row>
+    <row r="23" spans="1:14" s="60" customFormat="1">
+      <c r="A23" s="33">
+        <v>1</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>342</v>
+      </c>
+      <c r="F23" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="74"/>
+      <c r="J23" s="28">
+        <v>0.97</v>
+      </c>
+      <c r="K23" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="L23" s="28">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M23" s="28">
+        <v>0.41</v>
+      </c>
+      <c r="N23" s="59"/>
+    </row>
+    <row r="24" spans="1:14" s="60" customFormat="1">
+      <c r="A24" s="33">
+        <v>7</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>404</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="E24" s="58"/>
+      <c r="F24" s="82" t="s">
+        <v>474</v>
+      </c>
+      <c r="G24" s="58" t="s">
+        <v>473</v>
+      </c>
+      <c r="H24" s="58" t="s">
+        <v>472</v>
+      </c>
+      <c r="I24" s="58"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="59"/>
+    </row>
+    <row r="25" spans="1:14" s="60" customFormat="1">
+      <c r="A25" s="33">
+        <v>1</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>322</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="E25" s="58"/>
+      <c r="F25" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="34"/>
+      <c r="J25" s="28">
+        <v>0.48</v>
+      </c>
+      <c r="K25" s="28">
+        <v>0.45</v>
+      </c>
+      <c r="L25" s="28">
+        <v>0.35</v>
+      </c>
+      <c r="M25" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="N25" s="59"/>
+    </row>
+    <row r="26" spans="1:14" s="60" customFormat="1">
+      <c r="A26" s="33">
+        <v>1</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>326</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>328</v>
+      </c>
+      <c r="E26" s="58"/>
+      <c r="F26" s="84" t="s">
+        <v>452</v>
+      </c>
+      <c r="G26" s="58" t="s">
+        <v>328</v>
+      </c>
+      <c r="H26" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="I26" s="58"/>
+      <c r="J26" s="29">
+        <v>1.2</v>
+      </c>
+      <c r="K26" s="29">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="L26" s="29">
+        <v>0.9133</v>
+      </c>
+      <c r="M26" s="29">
+        <v>0.6512</v>
+      </c>
+      <c r="N26" s="59"/>
+    </row>
+    <row r="27" spans="1:14" s="60" customFormat="1">
+      <c r="A27" s="70"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="73"/>
+    </row>
+    <row r="28" spans="1:14" s="60" customFormat="1">
+      <c r="A28" s="33">
+        <v>1</v>
+      </c>
+      <c r="B28" s="57" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" s="52" customFormat="1" ht="15" thickBot="1">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="27">
+      <c r="C28" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>386</v>
+      </c>
+      <c r="F28" s="82" t="s">
+        <v>453</v>
+      </c>
+      <c r="G28" s="58" t="s">
+        <v>422</v>
+      </c>
+      <c r="H28" s="58" t="s">
+        <v>421</v>
+      </c>
+      <c r="I28" s="58" t="s">
+        <v>385</v>
+      </c>
+      <c r="J28" s="29">
+        <v>0.95</v>
+      </c>
+      <c r="K28" s="29">
+        <v>0.77</v>
+      </c>
+      <c r="L28" s="29">
+        <v>0.63</v>
+      </c>
+      <c r="M28" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N28" s="59" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="60" customFormat="1">
+      <c r="A29" s="70"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="73"/>
+    </row>
+    <row r="30" spans="1:14" s="60" customFormat="1">
+      <c r="A30" s="33">
         <v>1</v>
       </c>
-      <c r="J2" s="2">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2">
-        <v>100</v>
-      </c>
-      <c r="L2" s="3">
-        <v>1000</v>
-      </c>
-      <c r="M2" s="74"/>
-    </row>
-    <row r="3" spans="1:13" s="52" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="51">
-        <v>25</v>
-      </c>
-      <c r="B3" s="61" t="s">
-        <v>391</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D3" s="51" t="s">
+      <c r="B30" s="57" t="s">
+        <v>329</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="58" t="s">
+        <v>330</v>
+      </c>
+      <c r="F30" s="82" t="s">
+        <v>454</v>
+      </c>
+      <c r="G30" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="58" t="s">
+        <v>362</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="J30" s="29">
+        <v>1.79</v>
+      </c>
+      <c r="K30" s="29">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="L30" s="29">
+        <v>1.03</v>
+      </c>
+      <c r="M30" s="29">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="N30" s="59" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="60" customFormat="1">
+      <c r="A31" s="33">
+        <v>8</v>
+      </c>
+      <c r="B31" s="57" t="s">
+        <v>405</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="D31" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="J3" s="28">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K3" s="28">
-        <v>1.1599999999999999E-2</v>
-      </c>
-      <c r="L3" s="28">
-        <v>6.3E-3</v>
-      </c>
-      <c r="M3" s="37"/>
-    </row>
-    <row r="4" spans="1:13" s="52" customFormat="1">
-      <c r="A4" s="84">
+      <c r="E31" s="58" t="s">
+        <v>296</v>
+      </c>
+      <c r="F31" s="84" t="s">
+        <v>183</v>
+      </c>
+      <c r="G31" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="H31" s="58" t="s">
+        <v>185</v>
+      </c>
+      <c r="I31" s="58"/>
+      <c r="J31" s="29">
+        <v>0.09</v>
+      </c>
+      <c r="K31" s="29">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="L31" s="29">
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="M31" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N31" s="59"/>
+    </row>
+    <row r="32" spans="1:14" s="60" customFormat="1">
+      <c r="A32" s="70"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="73"/>
+    </row>
+    <row r="33" spans="1:14" s="60" customFormat="1">
+      <c r="A33" s="33">
         <v>1</v>
       </c>
-      <c r="B4" s="85" t="s">
-        <v>304</v>
-      </c>
-      <c r="C4" s="84" t="s">
-        <v>262</v>
-      </c>
-      <c r="D4" s="84" t="s">
+      <c r="B33" s="57" t="s">
+        <v>276</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="E33" s="58" t="s">
+        <v>281</v>
+      </c>
+      <c r="F33" s="84" t="s">
+        <v>455</v>
+      </c>
+      <c r="G33" s="58" t="s">
+        <v>281</v>
+      </c>
+      <c r="H33" s="58" t="s">
+        <v>364</v>
+      </c>
+      <c r="I33" s="58"/>
+      <c r="J33" s="29">
+        <v>0.22</v>
+      </c>
+      <c r="K33" s="29">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="L33" s="29">
+        <v>0.111</v>
+      </c>
+      <c r="M33" s="29">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="N33" s="59"/>
+    </row>
+    <row r="34" spans="1:14" s="60" customFormat="1">
+      <c r="A34" s="70"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="73"/>
+    </row>
+    <row r="35" spans="1:14" s="60" customFormat="1">
+      <c r="A35" s="33">
+        <v>3</v>
+      </c>
+      <c r="B35" s="57" t="s">
+        <v>406</v>
+      </c>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="86" t="s">
-        <v>264</v>
-      </c>
-      <c r="F4" s="86" t="s">
-        <v>444</v>
-      </c>
-      <c r="G4" s="84" t="s">
-        <v>443</v>
-      </c>
-      <c r="H4" s="86"/>
-      <c r="I4" s="87">
-        <v>0.26</v>
-      </c>
-      <c r="J4" s="87">
-        <v>0.17899999999999999</v>
-      </c>
-      <c r="K4" s="87">
-        <v>0.1017</v>
-      </c>
-      <c r="L4" s="87">
-        <v>0.06</v>
-      </c>
-      <c r="M4" s="88"/>
-    </row>
-    <row r="5" spans="1:13" s="52" customFormat="1">
-      <c r="A5" s="51">
-        <v>1</v>
-      </c>
-      <c r="B5" s="62" t="s">
-        <v>267</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>417</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="51" t="s">
-        <v>374</v>
-      </c>
-      <c r="I5" s="30">
-        <v>0.08</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="30">
-        <v>0.05</v>
-      </c>
-      <c r="L5" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="37" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="52" customFormat="1">
-      <c r="A6" s="51">
-        <v>3</v>
-      </c>
-      <c r="B6" s="61" t="s">
-        <v>394</v>
-      </c>
-      <c r="C6" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="28">
-        <v>0.32</v>
-      </c>
-      <c r="J6" s="28">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="K6" s="28">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L6" s="28">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="M6" s="37"/>
-    </row>
-    <row r="7" spans="1:13" s="52" customFormat="1">
-      <c r="A7" s="51">
-        <v>2</v>
-      </c>
-      <c r="B7" s="61" t="s">
-        <v>395</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D7" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>232</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>439</v>
-      </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="31">
-        <v>0.1</v>
-      </c>
-      <c r="J7" s="31">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="K7" s="31">
-        <v>2.1899999999999999E-2</v>
-      </c>
-      <c r="L7" s="31">
-        <v>1.17E-2</v>
-      </c>
-      <c r="M7" s="37"/>
-    </row>
-    <row r="8" spans="1:13" s="52" customFormat="1">
-      <c r="A8" s="51">
-        <v>14</v>
-      </c>
-      <c r="B8" s="61" t="s">
-        <v>396</v>
-      </c>
-      <c r="C8" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D8" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="J8" s="28">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="K8" s="28">
-        <v>1.8700000000000001E-2</v>
-      </c>
-      <c r="L8" s="28">
-        <v>1.0200000000000001E-2</v>
-      </c>
-      <c r="M8" s="37"/>
-    </row>
-    <row r="9" spans="1:13" s="52" customFormat="1">
-      <c r="A9" s="51">
-        <v>3</v>
-      </c>
-      <c r="B9" s="61" t="s">
-        <v>397</v>
-      </c>
-      <c r="C9" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D9" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="28">
-        <v>0.17</v>
-      </c>
-      <c r="J9" s="28">
-        <v>0.115</v>
-      </c>
-      <c r="K9" s="28">
-        <v>0.54600000000000004</v>
-      </c>
-      <c r="L9" s="28">
-        <v>0.31630000000000003</v>
-      </c>
-      <c r="M9" s="37"/>
-    </row>
-    <row r="10" spans="1:13" s="52" customFormat="1">
-      <c r="A10" s="57">
-        <v>2</v>
-      </c>
-      <c r="B10" s="63" t="s">
-        <v>398</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>262</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="58" t="s">
-        <v>343</v>
-      </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="59">
-        <v>0.12</v>
-      </c>
-      <c r="J10" s="59">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="K10" s="59">
-        <v>3.9E-2</v>
-      </c>
-      <c r="L10" s="59">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="M10" s="60" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="52" customFormat="1">
-      <c r="A11" s="51">
-        <v>2</v>
-      </c>
-      <c r="B11" s="61" t="s">
-        <v>399</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>419</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>418</v>
-      </c>
-      <c r="H11" s="39"/>
-      <c r="I11" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="J11" s="28">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="K11" s="28">
-        <v>6.93E-2</v>
-      </c>
-      <c r="L11" s="28">
-        <v>4.2079999999999999E-2</v>
-      </c>
-      <c r="M11" s="37"/>
-    </row>
-    <row r="12" spans="1:13" s="52" customFormat="1">
-      <c r="A12" s="51">
-        <v>30</v>
-      </c>
-      <c r="B12" s="61" t="s">
-        <v>392</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D12" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>344</v>
-      </c>
-      <c r="F12" s="38" t="s">
-        <v>421</v>
-      </c>
-      <c r="G12" s="70" t="s">
-        <v>420</v>
-      </c>
-      <c r="I12" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="J12" s="28">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K12" s="28">
-        <v>1.1299999999999999E-2</v>
-      </c>
-      <c r="L12" s="28">
-        <v>6.1500000000000001E-3</v>
-      </c>
-      <c r="M12" s="37"/>
-    </row>
-    <row r="13" spans="1:13" s="52" customFormat="1">
-      <c r="A13" s="51">
-        <v>1</v>
-      </c>
-      <c r="B13" s="64" t="s">
-        <v>315</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>262</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>335</v>
-      </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="37"/>
-    </row>
-    <row r="14" spans="1:13" s="52" customFormat="1">
-      <c r="A14" s="51">
-        <v>1</v>
-      </c>
-      <c r="B14" s="64" t="s">
-        <v>290</v>
-      </c>
-      <c r="C14" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" s="51" t="s">
-        <v>291</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="F14" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="G14" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="28">
-        <v>1.41</v>
-      </c>
-      <c r="J14" s="28">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="K14" s="28">
-        <v>0.83</v>
-      </c>
-      <c r="L14" s="28">
-        <v>0.52</v>
-      </c>
-      <c r="M14" s="37"/>
-    </row>
-    <row r="15" spans="1:13" s="52" customFormat="1">
-      <c r="A15" s="54"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="44"/>
-    </row>
-    <row r="16" spans="1:13" s="52" customFormat="1">
-      <c r="A16" s="51">
-        <v>4</v>
-      </c>
-      <c r="B16" s="61" t="s">
-        <v>400</v>
-      </c>
-      <c r="C16" s="51" t="s">
-        <v>279</v>
-      </c>
-      <c r="D16" s="51" t="s">
-        <v>280</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="43"/>
-      <c r="I16" s="28">
-        <v>0.4</v>
-      </c>
-      <c r="J16" s="28">
-        <v>0.31</v>
-      </c>
-      <c r="K16" s="28">
-        <v>0.216</v>
-      </c>
-      <c r="L16" s="28">
-        <v>0.11</v>
-      </c>
-      <c r="M16" s="37"/>
-    </row>
-    <row r="17" spans="1:13" s="52" customFormat="1" ht="16" customHeight="1">
-      <c r="A17" s="51">
-        <v>13</v>
-      </c>
-      <c r="B17" s="61" t="s">
-        <v>401</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>292</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>293</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>294</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>249</v>
-      </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="31">
-        <v>0.77</v>
-      </c>
-      <c r="J17" s="31">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="K17" s="31">
-        <v>0.51990000000000003</v>
-      </c>
-      <c r="L17" s="31">
-        <v>0.30854999999999999</v>
-      </c>
-      <c r="M17" s="37"/>
-    </row>
-    <row r="18" spans="1:13" s="52" customFormat="1">
-      <c r="A18" s="54"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="44"/>
-    </row>
-    <row r="19" spans="1:13" s="52" customFormat="1">
-      <c r="A19" s="51">
-        <v>6</v>
-      </c>
-      <c r="B19" s="61" t="s">
-        <v>402</v>
-      </c>
-      <c r="C19" s="51" t="s">
-        <v>302</v>
-      </c>
-      <c r="D19" s="51" t="s">
-        <v>339</v>
-      </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="G19" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="H19" s="38"/>
-      <c r="I19" s="30">
-        <v>0.33</v>
-      </c>
-      <c r="J19" s="30">
-        <v>0.315</v>
-      </c>
-      <c r="K19" s="30">
-        <v>0.2205</v>
-      </c>
-      <c r="L19" s="30">
-        <v>0.1575</v>
-      </c>
-      <c r="M19" s="37"/>
-    </row>
-    <row r="20" spans="1:13" s="52" customFormat="1" ht="14" customHeight="1">
-      <c r="A20" s="51">
-        <v>2</v>
-      </c>
-      <c r="B20" s="61" t="s">
-        <v>403</v>
-      </c>
-      <c r="C20" s="51" t="s">
-        <v>302</v>
-      </c>
-      <c r="D20" s="51" t="s">
-        <v>303</v>
-      </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38" t="s">
-        <v>422</v>
-      </c>
-      <c r="G20" s="38" t="s">
-        <v>357</v>
-      </c>
-      <c r="H20" s="38"/>
-      <c r="I20" s="30">
-        <v>0.45</v>
-      </c>
-      <c r="J20" s="30">
-        <v>0.42</v>
-      </c>
-      <c r="K20" s="30">
-        <v>0.32200000000000001</v>
-      </c>
-      <c r="L20" s="30">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="M20" s="37"/>
-    </row>
-    <row r="21" spans="1:13" s="52" customFormat="1" ht="14" customHeight="1">
-      <c r="A21" s="51">
-        <v>2</v>
-      </c>
-      <c r="B21" s="61" t="s">
-        <v>404</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>302</v>
-      </c>
-      <c r="D21" s="51" t="s">
-        <v>309</v>
-      </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38" t="s">
-        <v>423</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>358</v>
-      </c>
-      <c r="H21" s="38"/>
-      <c r="I21" s="30">
-        <v>0.45</v>
-      </c>
-      <c r="J21" s="30">
-        <v>0.42199999999999999</v>
-      </c>
-      <c r="K21" s="30">
-        <v>0.32379999999999998</v>
-      </c>
-      <c r="L21" s="30">
-        <v>0.23232</v>
-      </c>
-      <c r="M21" s="37"/>
-    </row>
-    <row r="22" spans="1:13" s="52" customFormat="1">
-      <c r="A22" s="51">
-        <v>4</v>
-      </c>
-      <c r="B22" s="61" t="s">
-        <v>405</v>
-      </c>
-      <c r="C22" s="51" t="s">
-        <v>302</v>
-      </c>
-      <c r="D22" s="51" t="s">
-        <v>340</v>
-      </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38" t="s">
-        <v>424</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>359</v>
-      </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="30">
-        <v>0.77</v>
-      </c>
-      <c r="J22" s="30">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="K22" s="30">
-        <v>0.58209999999999995</v>
-      </c>
-      <c r="L22" s="30">
-        <v>0.42336000000000001</v>
-      </c>
-      <c r="M22" s="37"/>
-    </row>
-    <row r="23" spans="1:13" s="52" customFormat="1">
-      <c r="A23" s="51">
-        <v>1</v>
-      </c>
-      <c r="B23" s="64" t="s">
-        <v>336</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>338</v>
-      </c>
-      <c r="D23" s="51" t="s">
-        <v>337</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>342</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="H23" s="46"/>
-      <c r="I23" s="34">
-        <v>0.97</v>
-      </c>
-      <c r="J23" s="34">
-        <v>0.75</v>
-      </c>
-      <c r="K23" s="34">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="L23" s="34">
-        <v>0.41</v>
-      </c>
-      <c r="M23" s="37"/>
-    </row>
-    <row r="24" spans="1:13" s="52" customFormat="1">
-      <c r="A24" s="51">
-        <v>7</v>
-      </c>
-      <c r="B24" s="61" t="s">
-        <v>406</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>301</v>
-      </c>
-      <c r="D24" s="51" t="s">
-        <v>300</v>
-      </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="37"/>
-    </row>
-    <row r="25" spans="1:13" s="52" customFormat="1">
-      <c r="A25" s="51">
-        <v>1</v>
-      </c>
-      <c r="B25" s="64" t="s">
-        <v>322</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>324</v>
-      </c>
-      <c r="D25" s="51" t="s">
-        <v>323</v>
-      </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="G25" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="H25" s="43"/>
-      <c r="I25" s="28">
-        <v>0.48</v>
-      </c>
-      <c r="J25" s="28">
-        <v>0.45</v>
-      </c>
-      <c r="K25" s="28">
-        <v>0.35</v>
-      </c>
-      <c r="L25" s="28">
-        <v>0.25</v>
-      </c>
-      <c r="M25" s="37"/>
-    </row>
-    <row r="26" spans="1:13" s="52" customFormat="1">
-      <c r="A26" s="51">
-        <v>1</v>
-      </c>
-      <c r="B26" s="64" t="s">
-        <v>326</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>327</v>
-      </c>
-      <c r="D26" s="51" t="s">
-        <v>328</v>
-      </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38" t="s">
-        <v>328</v>
-      </c>
-      <c r="G26" s="38" t="s">
-        <v>360</v>
-      </c>
-      <c r="H26" s="38"/>
-      <c r="I26" s="30">
-        <v>1.2</v>
-      </c>
-      <c r="J26" s="30">
-        <v>1.0589999999999999</v>
-      </c>
-      <c r="K26" s="30">
-        <v>0.9133</v>
-      </c>
-      <c r="L26" s="30">
-        <v>0.6512</v>
-      </c>
-      <c r="M26" s="37"/>
-    </row>
-    <row r="27" spans="1:13" s="52" customFormat="1">
-      <c r="A27" s="54"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="44"/>
-    </row>
-    <row r="28" spans="1:13" s="52" customFormat="1">
-      <c r="A28" s="51">
-        <v>1</v>
-      </c>
-      <c r="B28" s="64" t="s">
-        <v>385</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>386</v>
-      </c>
-      <c r="D28" s="51" t="s">
-        <v>389</v>
-      </c>
-      <c r="E28" s="38" t="s">
-        <v>388</v>
-      </c>
-      <c r="F28" s="38" t="s">
-        <v>426</v>
-      </c>
-      <c r="G28" s="38" t="s">
-        <v>425</v>
-      </c>
-      <c r="H28" s="38" t="s">
-        <v>387</v>
-      </c>
-      <c r="I28" s="30">
-        <v>0.95</v>
-      </c>
-      <c r="J28" s="30">
-        <v>0.77</v>
-      </c>
-      <c r="K28" s="30">
-        <v>0.63</v>
-      </c>
-      <c r="L28" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="M28" s="37" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="52" customFormat="1">
-      <c r="A29" s="54"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="44"/>
-    </row>
-    <row r="30" spans="1:13" s="52" customFormat="1">
-      <c r="A30" s="51">
-        <v>1</v>
-      </c>
-      <c r="B30" s="64" t="s">
-        <v>329</v>
-      </c>
-      <c r="C30" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" s="51"/>
-      <c r="E30" s="38" t="s">
-        <v>330</v>
-      </c>
-      <c r="F30" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="H30" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="I30" s="30">
-        <v>1.79</v>
-      </c>
-      <c r="J30" s="30">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="K30" s="30">
-        <v>1.03</v>
-      </c>
-      <c r="L30" s="30">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="M30" s="37" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="52" customFormat="1">
-      <c r="A31" s="51">
-        <v>8</v>
-      </c>
-      <c r="B31" s="61" t="s">
-        <v>407</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>295</v>
-      </c>
-      <c r="D31" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="38" t="s">
-        <v>296</v>
-      </c>
-      <c r="F31" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="G31" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="H31" s="38"/>
-      <c r="I31" s="30">
-        <v>0.09</v>
-      </c>
-      <c r="J31" s="30">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="K31" s="30">
-        <v>5.8799999999999998E-2</v>
-      </c>
-      <c r="L31" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="M31" s="37"/>
-    </row>
-    <row r="32" spans="1:13" s="52" customFormat="1">
-      <c r="A32" s="54"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="44"/>
-    </row>
-    <row r="33" spans="1:13" s="52" customFormat="1">
-      <c r="A33" s="51">
-        <v>1</v>
-      </c>
-      <c r="B33" s="64" t="s">
-        <v>276</v>
-      </c>
-      <c r="C33" s="51" t="s">
-        <v>277</v>
-      </c>
-      <c r="D33" s="51" t="s">
-        <v>278</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="F33" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="G33" s="38" t="s">
-        <v>364</v>
-      </c>
-      <c r="H33" s="38"/>
-      <c r="I33" s="30">
-        <v>0.22</v>
-      </c>
-      <c r="J33" s="30">
-        <v>0.19800000000000001</v>
-      </c>
-      <c r="K33" s="30">
-        <v>0.111</v>
-      </c>
-      <c r="L33" s="30">
-        <v>4.0500000000000001E-2</v>
-      </c>
-      <c r="M33" s="37"/>
-    </row>
-    <row r="34" spans="1:13" s="52" customFormat="1">
-      <c r="A34" s="54"/>
-      <c r="B34" s="65"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="44"/>
-    </row>
-    <row r="35" spans="1:13" s="52" customFormat="1">
-      <c r="A35" s="51">
-        <v>3</v>
-      </c>
-      <c r="B35" s="61" t="s">
-        <v>408</v>
-      </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="38" t="s">
+      <c r="E35" s="58" t="s">
         <v>345</v>
       </c>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="28"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
       <c r="J35" s="28"/>
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
-      <c r="M35" s="37"/>
-    </row>
-    <row r="36" spans="1:13" s="52" customFormat="1">
-      <c r="A36" s="55">
+      <c r="M35" s="28"/>
+      <c r="N35" s="59"/>
+    </row>
+    <row r="36" spans="1:14" s="60" customFormat="1">
+      <c r="A36" s="61">
         <v>2</v>
       </c>
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="62" t="s">
+        <v>407</v>
+      </c>
+      <c r="C36" s="61" t="s">
+        <v>256</v>
+      </c>
+      <c r="D36" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="63" t="s">
+        <v>365</v>
+      </c>
+      <c r="F36" s="83" t="s">
+        <v>456</v>
+      </c>
+      <c r="G36" s="63" t="s">
+        <v>423</v>
+      </c>
+      <c r="H36" s="63" t="s">
+        <v>366</v>
+      </c>
+      <c r="I36" s="63"/>
+      <c r="J36" s="64" t="s">
+        <v>367</v>
+      </c>
+      <c r="K36" s="64">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L36" s="64">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="M36" s="64">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="N36" s="65"/>
+    </row>
+    <row r="37" spans="1:14" s="60" customFormat="1">
+      <c r="A37" s="33">
+        <v>1</v>
+      </c>
+      <c r="B37" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="58">
+        <v>120</v>
+      </c>
+      <c r="F37" s="84" t="s">
+        <v>457</v>
+      </c>
+      <c r="G37" s="58" t="s">
+        <v>438</v>
+      </c>
+      <c r="H37" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="I37" s="33"/>
+      <c r="J37" s="29">
+        <v>0.17</v>
+      </c>
+      <c r="K37" s="29">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L37" s="29">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="M37" s="29">
+        <v>2.3560000000000001E-2</v>
+      </c>
+      <c r="N37" s="59"/>
+    </row>
+    <row r="38" spans="1:14" s="60" customFormat="1">
+      <c r="A38" s="33">
+        <v>8</v>
+      </c>
+      <c r="B38" s="57" t="s">
+        <v>408</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="58">
+        <v>649</v>
+      </c>
+      <c r="F38" s="84" t="s">
+        <v>193</v>
+      </c>
+      <c r="G38" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="H38" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="I38" s="32"/>
+      <c r="J38" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="K38" s="28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L38" s="28">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="M38" s="28">
+        <v>3.8400000000000001E-3</v>
+      </c>
+      <c r="N38" s="59"/>
+    </row>
+    <row r="39" spans="1:14" s="60" customFormat="1">
+      <c r="A39" s="76">
+        <v>1</v>
+      </c>
+      <c r="B39" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>256</v>
+      </c>
+      <c r="D39" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="78">
+        <v>675</v>
+      </c>
+      <c r="F39" s="87"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="78"/>
+      <c r="J39" s="79"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="80" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="60" customFormat="1">
+      <c r="A40" s="33">
+        <v>1</v>
+      </c>
+      <c r="B40" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="58" t="s">
+        <v>266</v>
+      </c>
+      <c r="F40" s="84" t="s">
+        <v>458</v>
+      </c>
+      <c r="G40" s="58" t="s">
+        <v>424</v>
+      </c>
+      <c r="H40" s="58" t="s">
+        <v>369</v>
+      </c>
+      <c r="I40" s="33"/>
+      <c r="J40" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="K40" s="29">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L40" s="29">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="M40" s="29">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N40" s="59"/>
+    </row>
+    <row r="41" spans="1:14" s="60" customFormat="1">
+      <c r="A41" s="33">
+        <v>11</v>
+      </c>
+      <c r="B41" s="57" t="s">
         <v>409</v>
       </c>
-      <c r="C36" s="55" t="s">
+      <c r="C41" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="D36" s="55" t="s">
+      <c r="D41" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="48" t="s">
-        <v>366</v>
-      </c>
-      <c r="F36" s="48" t="s">
+      <c r="E41" s="58" t="s">
+        <v>268</v>
+      </c>
+      <c r="F41" s="84" t="s">
+        <v>459</v>
+      </c>
+      <c r="G41" s="58" t="s">
+        <v>425</v>
+      </c>
+      <c r="H41" s="58" t="s">
+        <v>370</v>
+      </c>
+      <c r="I41" s="33"/>
+      <c r="J41" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="K41" s="29">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L41" s="29">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="M41" s="29">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N41" s="59"/>
+    </row>
+    <row r="42" spans="1:14" s="60" customFormat="1" ht="14" customHeight="1">
+      <c r="A42" s="33">
+        <v>30</v>
+      </c>
+      <c r="B42" s="57" t="s">
+        <v>391</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="58" t="s">
+        <v>348</v>
+      </c>
+      <c r="F42" s="84" t="s">
+        <v>460</v>
+      </c>
+      <c r="G42" s="58" t="s">
+        <v>426</v>
+      </c>
+      <c r="H42" s="58" t="s">
+        <v>349</v>
+      </c>
+      <c r="I42" s="58"/>
+      <c r="J42" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M42" s="29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="N42" s="59"/>
+    </row>
+    <row r="43" spans="1:14" s="60" customFormat="1" ht="14" customHeight="1">
+      <c r="A43" s="33">
+        <v>1</v>
+      </c>
+      <c r="B43" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" s="84" t="s">
+        <v>104</v>
+      </c>
+      <c r="G43" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="H43" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="I43" s="32"/>
+      <c r="J43" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="K43" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L43" s="28">
+        <v>1.14E-2</v>
+      </c>
+      <c r="M43" s="28">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="N43" s="59"/>
+    </row>
+    <row r="44" spans="1:14" s="60" customFormat="1">
+      <c r="A44" s="33">
+        <v>6</v>
+      </c>
+      <c r="B44" s="57" t="s">
+        <v>410</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="58" t="s">
+        <v>263</v>
+      </c>
+      <c r="F44" s="84" t="s">
+        <v>462</v>
+      </c>
+      <c r="G44" s="58" t="s">
         <v>427</v>
       </c>
-      <c r="G36" s="48" t="s">
-        <v>367</v>
-      </c>
-      <c r="H36" s="48"/>
-      <c r="I36" s="35" t="s">
-        <v>368</v>
-      </c>
-      <c r="J36" s="35">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K36" s="35">
-        <v>4.7000000000000002E-3</v>
-      </c>
-      <c r="L36" s="35">
-        <v>2.0999999999999999E-3</v>
-      </c>
-      <c r="M36" s="47" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" s="52" customFormat="1">
-      <c r="A37" s="51">
+      <c r="H44" s="58" t="s">
+        <v>461</v>
+      </c>
+      <c r="I44" s="58"/>
+      <c r="J44" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="K44" s="29">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L44" s="29">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="M44" s="29">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N44" s="59"/>
+    </row>
+    <row r="45" spans="1:14" s="60" customFormat="1">
+      <c r="A45" s="33">
         <v>1</v>
       </c>
-      <c r="B37" s="61" t="s">
-        <v>260</v>
-      </c>
-      <c r="C37" s="51" t="s">
+      <c r="B45" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="C45" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="D37" s="51" t="s">
+      <c r="D45" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="38">
-        <v>120</v>
-      </c>
-      <c r="F37" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="G37" s="42" t="s">
-        <v>441</v>
-      </c>
-      <c r="H37" s="42"/>
-      <c r="I37" s="31">
-        <v>0.17</v>
-      </c>
-      <c r="J37" s="31">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K37" s="31">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="L37" s="31">
-        <v>2.3560000000000001E-2</v>
-      </c>
-      <c r="M37" s="37"/>
-    </row>
-    <row r="38" spans="1:13" s="52" customFormat="1">
-      <c r="A38" s="51">
-        <v>8</v>
-      </c>
-      <c r="B38" s="61" t="s">
-        <v>410</v>
-      </c>
-      <c r="C38" s="51" t="s">
+      <c r="E45" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F45" s="84" t="s">
+        <v>199</v>
+      </c>
+      <c r="G45" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="H45" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="I45" s="32"/>
+      <c r="J45" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="K45" s="28">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L45" s="28">
+        <v>1.14E-2</v>
+      </c>
+      <c r="M45" s="28">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="N45" s="59"/>
+    </row>
+    <row r="46" spans="1:14" s="60" customFormat="1">
+      <c r="A46" s="33">
+        <v>1</v>
+      </c>
+      <c r="B46" s="66" t="s">
+        <v>346</v>
+      </c>
+      <c r="C46" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="D38" s="51" t="s">
+      <c r="D46" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="38">
-        <v>649</v>
-      </c>
-      <c r="F38" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="G38" s="39" t="s">
-        <v>196</v>
-      </c>
-      <c r="H38" s="39"/>
-      <c r="I38" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="J38" s="28">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K38" s="28">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="L38" s="28">
-        <v>3.8400000000000001E-3</v>
-      </c>
-      <c r="M38" s="37"/>
-    </row>
-    <row r="39" spans="1:13" s="52" customFormat="1">
-      <c r="A39" s="53">
+      <c r="E46" s="58" t="s">
+        <v>347</v>
+      </c>
+      <c r="F46" s="84" t="s">
+        <v>463</v>
+      </c>
+      <c r="G46" s="58" t="s">
+        <v>428</v>
+      </c>
+      <c r="H46" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="I46" s="32"/>
+      <c r="J46" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="K46" s="29">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L46" s="29">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="M46" s="29">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N46" s="59"/>
+    </row>
+    <row r="47" spans="1:14" s="60" customFormat="1">
+      <c r="A47" s="70"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="72"/>
+      <c r="I47" s="72"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="73"/>
+    </row>
+    <row r="48" spans="1:14" s="60" customFormat="1">
+      <c r="A48" s="33">
+        <v>2</v>
+      </c>
+      <c r="B48" s="57" t="s">
+        <v>411</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="D48" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="E48" s="58" t="s">
+        <v>321</v>
+      </c>
+      <c r="F48" s="84" t="s">
+        <v>121</v>
+      </c>
+      <c r="G48" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="H48" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="I48" s="34"/>
+      <c r="J48" s="28">
+        <v>0.21</v>
+      </c>
+      <c r="K48" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="L48" s="28">
+        <v>0.18</v>
+      </c>
+      <c r="M48" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="N48" s="59"/>
+    </row>
+    <row r="49" spans="1:14" s="60" customFormat="1">
+      <c r="A49" s="70"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="70"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="86"/>
+      <c r="G49" s="72"/>
+      <c r="H49" s="72"/>
+      <c r="I49" s="72"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="73"/>
+    </row>
+    <row r="50" spans="1:14" s="60" customFormat="1">
+      <c r="A50" s="33">
         <v>1</v>
       </c>
-      <c r="B39" s="67" t="s">
-        <v>261</v>
-      </c>
-      <c r="C39" s="53" t="s">
-        <v>256</v>
-      </c>
-      <c r="D39" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="41">
-        <v>675</v>
-      </c>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="40" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" s="52" customFormat="1">
-      <c r="A40" s="51">
+      <c r="B50" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="E50" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="H50" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="74"/>
+      <c r="J50" s="28">
+        <v>15.75</v>
+      </c>
+      <c r="K50" s="28">
+        <v>14.318</v>
+      </c>
+      <c r="L50" s="28">
+        <v>12.170299999999999</v>
+      </c>
+      <c r="M50" s="28">
+        <v>9.5214700000000008</v>
+      </c>
+      <c r="N50" s="59"/>
+    </row>
+    <row r="51" spans="1:14" s="60" customFormat="1">
+      <c r="A51" s="33">
         <v>1</v>
       </c>
-      <c r="B40" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="C40" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="D40" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="F40" s="38" t="s">
-        <v>428</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>370</v>
-      </c>
-      <c r="H40" s="51"/>
-      <c r="I40" s="30">
-        <v>0.08</v>
-      </c>
-      <c r="J40" s="30">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="K40" s="30">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="L40" s="30">
-        <v>2.4E-2</v>
-      </c>
-      <c r="M40" s="37"/>
-    </row>
-    <row r="41" spans="1:13" s="52" customFormat="1">
-      <c r="A41" s="51">
-        <v>11</v>
-      </c>
-      <c r="B41" s="61" t="s">
-        <v>411</v>
-      </c>
-      <c r="C41" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="D41" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E41" s="38" t="s">
-        <v>268</v>
-      </c>
-      <c r="F41" s="38" t="s">
+      <c r="B51" s="57" t="s">
+        <v>314</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="E51" s="58" t="s">
+        <v>350</v>
+      </c>
+      <c r="F51" s="84" t="s">
+        <v>464</v>
+      </c>
+      <c r="G51" s="58" t="s">
         <v>429</v>
       </c>
-      <c r="G41" s="38" t="s">
-        <v>371</v>
-      </c>
-      <c r="H41" s="51"/>
-      <c r="I41" s="30">
-        <v>0.08</v>
-      </c>
-      <c r="J41" s="30">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="K41" s="30">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="L41" s="30">
-        <v>2.4E-2</v>
-      </c>
-      <c r="M41" s="37"/>
-    </row>
-    <row r="42" spans="1:13" s="52" customFormat="1" ht="14" customHeight="1">
-      <c r="A42" s="51">
-        <v>30</v>
-      </c>
-      <c r="B42" s="61" t="s">
-        <v>393</v>
-      </c>
-      <c r="C42" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="D42" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>348</v>
-      </c>
-      <c r="F42" s="38" t="s">
+      <c r="H51" s="74" t="s">
+        <v>374</v>
+      </c>
+      <c r="I51" s="74"/>
+      <c r="J51" s="28">
+        <v>0.61</v>
+      </c>
+      <c r="K51" s="28">
+        <v>0.51</v>
+      </c>
+      <c r="L51" s="28">
+        <v>0.39</v>
+      </c>
+      <c r="M51" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="N51" s="59"/>
+    </row>
+    <row r="52" spans="1:14" s="60" customFormat="1">
+      <c r="A52" s="33">
+        <v>1</v>
+      </c>
+      <c r="B52" s="57" t="s">
+        <v>325</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="E52" s="58" t="s">
+        <v>354</v>
+      </c>
+      <c r="F52" s="84" t="s">
+        <v>465</v>
+      </c>
+      <c r="G52" s="58" t="s">
         <v>430</v>
       </c>
-      <c r="G42" s="38" t="s">
-        <v>349</v>
-      </c>
-      <c r="H42" s="38"/>
-      <c r="I42" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="L42" s="30">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="M42" s="37"/>
-    </row>
-    <row r="43" spans="1:13" s="52" customFormat="1" ht="14" customHeight="1">
-      <c r="A43" s="51">
+      <c r="H52" s="74" t="s">
+        <v>375</v>
+      </c>
+      <c r="I52" s="33"/>
+      <c r="J52" s="28">
+        <v>0.97</v>
+      </c>
+      <c r="K52" s="28">
+        <v>8.6199999999999999E-2</v>
+      </c>
+      <c r="L52" s="28">
+        <v>0.72</v>
+      </c>
+      <c r="M52" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="N52" s="59"/>
+    </row>
+    <row r="53" spans="1:14" s="60" customFormat="1">
+      <c r="A53" s="33">
         <v>1</v>
       </c>
-      <c r="B43" s="64" t="s">
-        <v>270</v>
-      </c>
-      <c r="C43" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="D43" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="F43" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="G43" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="H43" s="39"/>
-      <c r="I43" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="J43" s="28" t="s">
+      <c r="B53" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="E53" s="58" t="s">
+        <v>356</v>
+      </c>
+      <c r="F53" s="84" t="s">
+        <v>171</v>
+      </c>
+      <c r="G53" s="58" t="s">
+        <v>431</v>
+      </c>
+      <c r="H53" s="34" t="s">
+        <v>376</v>
+      </c>
+      <c r="I53" s="34"/>
+      <c r="J53" s="28">
+        <v>0.79</v>
+      </c>
+      <c r="K53" s="28">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="L53" s="28">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="M53" s="28">
+        <v>0.317</v>
+      </c>
+      <c r="N53" s="59"/>
+    </row>
+    <row r="54" spans="1:14" s="60" customFormat="1">
+      <c r="A54" s="33">
+        <v>1</v>
+      </c>
+      <c r="B54" s="57" t="s">
+        <v>310</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="E54" s="58" t="s">
+        <v>313</v>
+      </c>
+      <c r="F54" s="84" t="s">
+        <v>217</v>
+      </c>
+      <c r="G54" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="H54" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="I54" s="35"/>
+      <c r="J54" s="29">
+        <v>1.82</v>
+      </c>
+      <c r="K54" s="29">
+        <v>1.7290000000000001</v>
+      </c>
+      <c r="L54" s="29">
+        <v>1.5556000000000001</v>
+      </c>
+      <c r="M54" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="K43" s="28">
-        <v>1.14E-2</v>
-      </c>
-      <c r="L43" s="28">
-        <v>4.1599999999999996E-3</v>
-      </c>
-      <c r="M43" s="37"/>
-    </row>
-    <row r="44" spans="1:13" s="52" customFormat="1">
-      <c r="A44" s="51">
-        <v>6</v>
-      </c>
-      <c r="B44" s="61" t="s">
+      <c r="N54" s="59"/>
+    </row>
+    <row r="55" spans="1:14" s="60" customFormat="1" ht="15" customHeight="1">
+      <c r="A55" s="33">
+        <v>1</v>
+      </c>
+      <c r="B55" s="57" t="s">
+        <v>286</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="E55" s="58" t="s">
+        <v>289</v>
+      </c>
+      <c r="F55" s="84" t="s">
+        <v>223</v>
+      </c>
+      <c r="G55" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="H55" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="I55" s="35"/>
+      <c r="J55" s="29">
+        <v>6.97</v>
+      </c>
+      <c r="K55" s="29">
+        <v>6.26</v>
+      </c>
+      <c r="L55" s="29">
+        <v>5.157</v>
+      </c>
+      <c r="M55" s="29">
+        <v>3.375</v>
+      </c>
+      <c r="N55" s="59"/>
+    </row>
+    <row r="56" spans="1:14" s="60" customFormat="1">
+      <c r="A56" s="33">
+        <v>4</v>
+      </c>
+      <c r="B56" s="57" t="s">
         <v>412</v>
       </c>
-      <c r="C44" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="D44" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E44" s="38" t="s">
-        <v>263</v>
-      </c>
-      <c r="F44" s="38" t="s">
-        <v>431</v>
-      </c>
-      <c r="G44" s="38" t="s">
-        <v>372</v>
-      </c>
-      <c r="H44" s="38"/>
-      <c r="I44" s="30">
-        <v>0.08</v>
-      </c>
-      <c r="J44" s="30">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="K44" s="30">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="L44" s="30">
-        <v>2.4E-2</v>
-      </c>
-      <c r="M44" s="37"/>
-    </row>
-    <row r="45" spans="1:13" s="52" customFormat="1">
-      <c r="A45" s="51">
+      <c r="C56" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="E56" s="58" t="s">
+        <v>299</v>
+      </c>
+      <c r="F56" s="84" t="s">
+        <v>466</v>
+      </c>
+      <c r="G56" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="H56" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="I56" s="36"/>
+      <c r="J56" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="K56" s="29">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="L56" s="29">
+        <v>0.63</v>
+      </c>
+      <c r="M56" s="29">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="N56" s="59"/>
+    </row>
+    <row r="57" spans="1:14" s="60" customFormat="1">
+      <c r="A57" s="33">
         <v>1</v>
       </c>
-      <c r="B45" s="64" t="s">
-        <v>269</v>
-      </c>
-      <c r="C45" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="D45" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E45" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="F45" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="G45" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="H45" s="39"/>
-      <c r="I45" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="J45" s="28">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="K45" s="28">
-        <v>1.14E-2</v>
-      </c>
-      <c r="L45" s="28">
-        <v>4.1599999999999996E-3</v>
-      </c>
-      <c r="M45" s="37"/>
-    </row>
-    <row r="46" spans="1:13" s="52" customFormat="1">
-      <c r="A46" s="51">
+      <c r="B57" s="57" t="s">
+        <v>305</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="E57" s="58" t="s">
+        <v>306</v>
+      </c>
+      <c r="F57" s="84" t="s">
+        <v>467</v>
+      </c>
+      <c r="G57" s="58" t="s">
+        <v>432</v>
+      </c>
+      <c r="H57" s="58" t="s">
+        <v>377</v>
+      </c>
+      <c r="I57" s="58"/>
+      <c r="J57" s="29">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K57" s="29">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="L57" s="29">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="M57" s="29">
+        <v>0.21657999999999999</v>
+      </c>
+      <c r="N57" s="59"/>
+    </row>
+    <row r="58" spans="1:14" s="60" customFormat="1">
+      <c r="A58" s="33">
         <v>1</v>
       </c>
-      <c r="B46" s="62" t="s">
-        <v>346</v>
-      </c>
-      <c r="C46" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="D46" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="38" t="s">
-        <v>347</v>
-      </c>
-      <c r="F46" s="38" t="s">
-        <v>432</v>
-      </c>
-      <c r="G46" s="39" t="s">
-        <v>373</v>
-      </c>
-      <c r="H46" s="39"/>
-      <c r="I46" s="30">
-        <v>0.08</v>
-      </c>
-      <c r="J46" s="30">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="K46" s="30">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="L46" s="30">
-        <v>2.4E-2</v>
-      </c>
-      <c r="M46" s="37"/>
-    </row>
-    <row r="47" spans="1:13" s="52" customFormat="1">
-      <c r="A47" s="54"/>
-      <c r="B47" s="65"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="44"/>
-    </row>
-    <row r="48" spans="1:13" s="52" customFormat="1">
-      <c r="A48" s="51">
-        <v>2</v>
-      </c>
-      <c r="B48" s="61" t="s">
-        <v>413</v>
-      </c>
-      <c r="C48" s="51" t="s">
-        <v>319</v>
-      </c>
-      <c r="D48" s="51" t="s">
-        <v>320</v>
-      </c>
-      <c r="E48" s="38" t="s">
-        <v>321</v>
-      </c>
-      <c r="F48" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="G48" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="H48" s="43"/>
-      <c r="I48" s="28">
-        <v>0.21</v>
-      </c>
-      <c r="J48" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="K48" s="28">
-        <v>0.18</v>
-      </c>
-      <c r="L48" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="M48" s="37"/>
-    </row>
-    <row r="49" spans="1:13" s="52" customFormat="1">
-      <c r="A49" s="54"/>
-      <c r="B49" s="65"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
-      <c r="M49" s="44"/>
-    </row>
-    <row r="50" spans="1:13" s="52" customFormat="1">
-      <c r="A50" s="51">
+      <c r="B58" s="57" t="s">
+        <v>283</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="D58" s="33"/>
+      <c r="E58" s="58" t="s">
+        <v>285</v>
+      </c>
+      <c r="F58" s="84" t="s">
+        <v>468</v>
+      </c>
+      <c r="G58" s="58" t="s">
+        <v>433</v>
+      </c>
+      <c r="H58" s="58" t="s">
+        <v>378</v>
+      </c>
+      <c r="I58" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="J58" s="29">
+        <v>1.88</v>
+      </c>
+      <c r="K58" s="29">
+        <v>1.704</v>
+      </c>
+      <c r="L58" s="29">
+        <v>1.4608000000000001</v>
+      </c>
+      <c r="M58" s="29">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="N58" s="59"/>
+    </row>
+    <row r="59" spans="1:14" s="60" customFormat="1">
+      <c r="A59" s="33">
         <v>1</v>
       </c>
-      <c r="B50" s="64" t="s">
-        <v>255</v>
-      </c>
-      <c r="C50" s="51" t="s">
-        <v>282</v>
-      </c>
-      <c r="D50" s="51" t="s">
-        <v>258</v>
-      </c>
-      <c r="E50" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="H50" s="46"/>
-      <c r="I50" s="28">
-        <v>15.75</v>
-      </c>
-      <c r="J50" s="28">
-        <v>14.318</v>
-      </c>
-      <c r="K50" s="28">
-        <v>12.170299999999999</v>
-      </c>
-      <c r="L50" s="28">
-        <v>9.5214700000000008</v>
-      </c>
-      <c r="M50" s="37"/>
-    </row>
-    <row r="51" spans="1:13" s="52" customFormat="1">
-      <c r="A51" s="51">
+      <c r="B59" s="57" t="s">
+        <v>331</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="D59" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="E59" s="58" t="s">
+        <v>334</v>
+      </c>
+      <c r="F59" s="84" t="s">
+        <v>469</v>
+      </c>
+      <c r="G59" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="H59" s="58" t="s">
+        <v>380</v>
+      </c>
+      <c r="I59" s="33"/>
+      <c r="J59" s="29">
+        <v>1.86</v>
+      </c>
+      <c r="K59" s="29">
+        <v>1.55</v>
+      </c>
+      <c r="L59" s="29">
+        <v>1.18</v>
+      </c>
+      <c r="M59" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N59" s="59"/>
+    </row>
+    <row r="60" spans="1:14" s="60" customFormat="1">
+      <c r="A60" s="70"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="72"/>
+      <c r="F60" s="86"/>
+      <c r="G60" s="72"/>
+      <c r="H60" s="72"/>
+      <c r="I60" s="72"/>
+      <c r="J60" s="30"/>
+      <c r="K60" s="30"/>
+      <c r="L60" s="30"/>
+      <c r="M60" s="30"/>
+      <c r="N60" s="73"/>
+    </row>
+    <row r="61" spans="1:14" s="75" customFormat="1">
+      <c r="A61" s="33">
         <v>1</v>
       </c>
-      <c r="B51" s="64" t="s">
-        <v>314</v>
-      </c>
-      <c r="C51" s="51" t="s">
-        <v>355</v>
-      </c>
-      <c r="D51" s="51" t="s">
-        <v>351</v>
-      </c>
-      <c r="E51" s="38" t="s">
-        <v>350</v>
-      </c>
-      <c r="F51" s="38" t="s">
-        <v>433</v>
-      </c>
-      <c r="G51" s="46" t="s">
-        <v>376</v>
-      </c>
-      <c r="H51" s="46"/>
-      <c r="I51" s="28">
-        <v>0.61</v>
-      </c>
-      <c r="J51" s="28">
-        <v>0.51</v>
-      </c>
-      <c r="K51" s="28">
-        <v>0.39</v>
-      </c>
-      <c r="L51" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="M51" s="37"/>
-    </row>
-    <row r="52" spans="1:13" s="52" customFormat="1">
-      <c r="A52" s="51">
+      <c r="B61" s="57" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="D61" s="33"/>
+      <c r="E61" s="58" t="s">
+        <v>227</v>
+      </c>
+      <c r="F61" s="84" t="s">
+        <v>470</v>
+      </c>
+      <c r="G61" s="58" t="s">
+        <v>230</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="I61" s="35"/>
+      <c r="J61" s="29">
+        <v>0.73</v>
+      </c>
+      <c r="K61" s="29">
+        <v>0.65</v>
+      </c>
+      <c r="L61" s="29">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="M61" s="29">
+        <v>0.42502000000000001</v>
+      </c>
+      <c r="N61" s="59"/>
+    </row>
+    <row r="62" spans="1:14" s="75" customFormat="1">
+      <c r="A62" s="33">
         <v>1</v>
       </c>
-      <c r="B52" s="64" t="s">
-        <v>325</v>
-      </c>
-      <c r="C52" s="51" t="s">
-        <v>352</v>
-      </c>
-      <c r="D52" s="51" t="s">
-        <v>353</v>
-      </c>
-      <c r="E52" s="38" t="s">
-        <v>354</v>
-      </c>
-      <c r="F52" s="38" t="s">
-        <v>434</v>
-      </c>
-      <c r="G52" s="46" t="s">
-        <v>377</v>
-      </c>
-      <c r="H52" s="51"/>
-      <c r="I52" s="28">
-        <v>0.97</v>
-      </c>
-      <c r="J52" s="28">
-        <v>8.6199999999999999E-2</v>
-      </c>
-      <c r="K52" s="28">
-        <v>0.72</v>
-      </c>
-      <c r="L52" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="M52" s="37"/>
-    </row>
-    <row r="53" spans="1:13" s="52" customFormat="1">
-      <c r="A53" s="51">
-        <v>1</v>
-      </c>
-      <c r="B53" s="64" t="s">
-        <v>271</v>
-      </c>
-      <c r="C53" s="51" t="s">
-        <v>272</v>
-      </c>
-      <c r="D53" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E53" s="38" t="s">
-        <v>356</v>
-      </c>
-      <c r="F53" s="38" t="s">
-        <v>435</v>
-      </c>
-      <c r="G53" s="43" t="s">
-        <v>378</v>
-      </c>
-      <c r="H53" s="43"/>
-      <c r="I53" s="28">
-        <v>0.79</v>
-      </c>
-      <c r="J53" s="28">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="K53" s="28">
-        <v>0.39600000000000002</v>
-      </c>
-      <c r="L53" s="28">
-        <v>0.317</v>
-      </c>
-      <c r="M53" s="37"/>
-    </row>
-    <row r="54" spans="1:13" s="52" customFormat="1">
-      <c r="A54" s="51">
-        <v>1</v>
-      </c>
-      <c r="B54" s="64" t="s">
-        <v>310</v>
-      </c>
-      <c r="C54" s="51" t="s">
-        <v>311</v>
-      </c>
-      <c r="D54" s="51" t="s">
-        <v>312</v>
-      </c>
-      <c r="E54" s="38" t="s">
-        <v>313</v>
-      </c>
-      <c r="F54" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="G54" s="49" t="s">
-        <v>219</v>
-      </c>
-      <c r="H54" s="49"/>
-      <c r="I54" s="31">
-        <v>1.82</v>
-      </c>
-      <c r="J54" s="31">
-        <v>1.7290000000000001</v>
-      </c>
-      <c r="K54" s="31">
-        <v>1.5556000000000001</v>
-      </c>
-      <c r="L54" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="M54" s="37"/>
-    </row>
-    <row r="55" spans="1:13" s="52" customFormat="1" ht="15" customHeight="1">
-      <c r="A55" s="51">
-        <v>1</v>
-      </c>
-      <c r="B55" s="64" t="s">
-        <v>286</v>
-      </c>
-      <c r="C55" s="51" t="s">
-        <v>287</v>
-      </c>
-      <c r="D55" s="51" t="s">
-        <v>288</v>
-      </c>
-      <c r="E55" s="38" t="s">
-        <v>289</v>
-      </c>
-      <c r="F55" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="G55" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="H55" s="49"/>
-      <c r="I55" s="31">
-        <v>6.97</v>
-      </c>
-      <c r="J55" s="31">
-        <v>6.26</v>
-      </c>
-      <c r="K55" s="31">
-        <v>5.157</v>
-      </c>
-      <c r="L55" s="31">
-        <v>3.375</v>
-      </c>
-      <c r="M55" s="37"/>
-    </row>
-    <row r="56" spans="1:13" s="52" customFormat="1">
-      <c r="A56" s="51">
-        <v>4</v>
-      </c>
-      <c r="B56" s="61" t="s">
-        <v>414</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>297</v>
-      </c>
-      <c r="D56" s="51" t="s">
-        <v>298</v>
-      </c>
-      <c r="E56" s="38" t="s">
-        <v>299</v>
-      </c>
-      <c r="F56" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="G56" s="50" t="s">
-        <v>253</v>
-      </c>
-      <c r="H56" s="50"/>
-      <c r="I56" s="31">
-        <v>0.9</v>
-      </c>
-      <c r="J56" s="31">
-        <v>0.79800000000000004</v>
-      </c>
-      <c r="K56" s="31">
-        <v>0.63</v>
-      </c>
-      <c r="L56" s="31">
-        <v>0.38750000000000001</v>
-      </c>
-      <c r="M56" s="37"/>
-    </row>
-    <row r="57" spans="1:13" s="52" customFormat="1">
-      <c r="A57" s="51">
-        <v>1</v>
-      </c>
-      <c r="B57" s="64" t="s">
-        <v>305</v>
-      </c>
-      <c r="C57" s="51" t="s">
-        <v>308</v>
-      </c>
-      <c r="D57" s="51" t="s">
-        <v>307</v>
-      </c>
-      <c r="E57" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="F57" s="38" t="s">
-        <v>436</v>
-      </c>
-      <c r="G57" s="38" t="s">
-        <v>379</v>
-      </c>
-      <c r="H57" s="38"/>
-      <c r="I57" s="30">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="J57" s="30">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="K57" s="30">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="L57" s="30">
-        <v>0.21657999999999999</v>
-      </c>
-      <c r="M57" s="37"/>
-    </row>
-    <row r="58" spans="1:13" s="52" customFormat="1">
-      <c r="A58" s="51">
-        <v>1</v>
-      </c>
-      <c r="B58" s="64" t="s">
-        <v>283</v>
-      </c>
-      <c r="C58" s="51" t="s">
-        <v>284</v>
-      </c>
-      <c r="D58" s="51"/>
-      <c r="E58" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="F58" s="38" t="s">
-        <v>437</v>
-      </c>
-      <c r="G58" s="38" t="s">
-        <v>380</v>
-      </c>
-      <c r="H58" s="51" t="s">
-        <v>381</v>
-      </c>
-      <c r="I58" s="30">
-        <v>1.88</v>
-      </c>
-      <c r="J58" s="30">
-        <v>1.704</v>
-      </c>
-      <c r="K58" s="30">
-        <v>1.4608000000000001</v>
-      </c>
-      <c r="L58" s="30">
-        <v>1.0229999999999999</v>
-      </c>
-      <c r="M58" s="37"/>
-    </row>
-    <row r="59" spans="1:13" s="52" customFormat="1">
-      <c r="A59" s="51">
-        <v>1</v>
-      </c>
-      <c r="B59" s="64" t="s">
-        <v>331</v>
-      </c>
-      <c r="C59" s="51" t="s">
-        <v>332</v>
-      </c>
-      <c r="D59" s="51" t="s">
-        <v>333</v>
-      </c>
-      <c r="E59" s="38" t="s">
-        <v>334</v>
-      </c>
-      <c r="F59" s="38" t="s">
-        <v>438</v>
-      </c>
-      <c r="G59" s="38" t="s">
-        <v>382</v>
-      </c>
-      <c r="H59" s="51"/>
-      <c r="I59" s="30">
-        <v>1.86</v>
-      </c>
-      <c r="J59" s="30">
-        <v>1.55</v>
-      </c>
-      <c r="K59" s="30">
-        <v>1.18</v>
-      </c>
-      <c r="L59" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="M59" s="37"/>
-    </row>
-    <row r="60" spans="1:13" s="52" customFormat="1">
-      <c r="A60" s="54"/>
-      <c r="B60" s="68"/>
-      <c r="C60" s="54"/>
-      <c r="D60" s="54"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="33"/>
-      <c r="M60" s="44"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="51">
-        <v>1</v>
-      </c>
-      <c r="B61" s="64" t="s">
-        <v>274</v>
-      </c>
-      <c r="C61" s="51" t="s">
-        <v>275</v>
-      </c>
-      <c r="D61" s="51"/>
-      <c r="E61" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="F61" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="G61" s="49" t="s">
-        <v>231</v>
-      </c>
-      <c r="H61" s="49"/>
-      <c r="I61" s="31">
-        <v>0.73</v>
-      </c>
-      <c r="J61" s="31">
-        <v>0.65</v>
-      </c>
-      <c r="K61" s="31">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="L61" s="31">
-        <v>0.42502000000000001</v>
-      </c>
-      <c r="M61" s="37"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="51">
-        <v>1</v>
-      </c>
-      <c r="B62" s="64" t="s">
+      <c r="B62" s="57" t="s">
         <v>316</v>
       </c>
-      <c r="C62" s="51" t="s">
+      <c r="C62" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D62" s="51" t="s">
+      <c r="D62" s="33" t="s">
         <v>317</v>
       </c>
-      <c r="E62" s="38" t="s">
+      <c r="E62" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="F62" s="38" t="s">
+      <c r="F62" s="84" t="s">
+        <v>471</v>
+      </c>
+      <c r="G62" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G62" s="39" t="s">
+      <c r="H62" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="H62" s="39"/>
-      <c r="I62" s="56">
+      <c r="I62" s="32"/>
+      <c r="J62" s="81">
         <v>0.95</v>
       </c>
-      <c r="J62" s="56">
+      <c r="K62" s="81">
         <v>0.84</v>
       </c>
-      <c r="K62" s="56">
+      <c r="L62" s="81">
         <v>0.69</v>
       </c>
-      <c r="L62" s="56">
+      <c r="M62" s="81">
         <v>0.54</v>
       </c>
-      <c r="M62" s="37"/>
+      <c r="N62" s="59"/>
     </row>
   </sheetData>
   <sortState ref="C19:AR30">
@@ -4933,16 +5161,17 @@
     <sortCondition ref="D19:D30"/>
   </sortState>
   <dataConsolidate/>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4983,54 +5212,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="80" t="s">
+      <c r="G1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="82" t="s">
+      <c r="H1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="82" t="s">
+      <c r="I1" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="82" t="s">
+      <c r="J1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Accidently had 0603metric components instead of 0603in components. Fixed this and finished mouser partnumbers as well.
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="0" windowWidth="19620" windowHeight="16280" tabRatio="986"/>
+    <workbookView xWindow="5160" yWindow="20" windowWidth="29040" windowHeight="20580" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="475">
   <si>
     <t>Part</t>
   </si>
@@ -805,9 +805,6 @@
     <t>R29</t>
   </si>
   <si>
-    <t>R12</t>
-  </si>
-  <si>
     <t>CAPACITOR</t>
   </si>
   <si>
@@ -1126,9 +1123,6 @@
     <t>0,1</t>
   </si>
   <si>
-    <t>This value is not available, consider changing value to 649.  It shouldn’t be an issue</t>
-  </si>
-  <si>
     <t>MCT0603-1.00K-CFCT-ND</t>
   </si>
   <si>
@@ -1168,9 +1162,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>OOPS!! This is not the right part.  Digikey/Mouser do not carry an 0603 cap with this value.  Consider changing to 0402 package</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -1186,9 +1177,6 @@
     <t>3.2 mm x 3.2 mm</t>
   </si>
   <si>
-    <t>Digikey has no stock</t>
-  </si>
-  <si>
     <t>C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C24, C26, C29, C31, C36, C44, C47, C83, C85, C86</t>
   </si>
   <si>
@@ -1246,9 +1234,6 @@
     <t>R13, R14</t>
   </si>
   <si>
-    <t>R21, R22, R23, R24, R25, R26, R27, R28</t>
-  </si>
-  <si>
     <t>R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R17</t>
   </si>
   <si>
@@ -1445,6 +1430,21 @@
   </si>
   <si>
     <t>CONN HEADER 2 POS 2.54</t>
+  </si>
+  <si>
+    <t>R12, R21, R22, R23, R24, R25, R26, R27, R28</t>
+  </si>
+  <si>
+    <t>MLCC - SMD/SMT 0402 4.4pF 50volts C0G +/-0.25pF</t>
+  </si>
+  <si>
+    <t>GRM1555C1H4R4CA01D</t>
+  </si>
+  <si>
+    <t>81-GRM1555C1H4R4CA1D</t>
+  </si>
+  <si>
+    <t>This is 0402 package size, Digikey doesn’t have anything even close to this value/size.  Mouser has 0603 but 18wk lead time.</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1510,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1538,12 +1538,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2045,7 +2039,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2154,10 +2148,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2231,15 +2221,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2263,19 +2244,19 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="340">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2951,75 +2932,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="112.5" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.5" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.5" style="54" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.5" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="26" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="96.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="98.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="37" customFormat="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>254</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>413</v>
-      </c>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="39" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>257</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="47" t="s">
-        <v>414</v>
-      </c>
-      <c r="H1" s="47" t="s">
-        <v>341</v>
-      </c>
-      <c r="I1" s="47" t="s">
-        <v>361</v>
-      </c>
-      <c r="J1" s="45" t="s">
+      <c r="G1" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>340</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>360</v>
+      </c>
+      <c r="J1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="43" t="s">
-        <v>381</v>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="41" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="37" customFormat="1" ht="15" thickBot="1">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
       <c r="J2" s="27">
         <v>1</v>
       </c>
@@ -3032,28 +3013,28 @@
       <c r="M2" s="3">
         <v>1000</v>
       </c>
-      <c r="N2" s="44"/>
-    </row>
-    <row r="3" spans="1:14" s="60" customFormat="1" ht="15" customHeight="1">
+      <c r="N2" s="42"/>
+    </row>
+    <row r="3" spans="1:14" s="58" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="33">
         <v>25</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>389</v>
+      <c r="B3" s="55" t="s">
+        <v>385</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D3" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="56" t="s">
         <v>75</v>
       </c>
       <c r="H3" s="32" t="s">
@@ -3072,73 +3053,73 @@
       <c r="M3" s="28">
         <v>6.3E-3</v>
       </c>
-      <c r="N3" s="59"/>
-    </row>
-    <row r="4" spans="1:14" s="60" customFormat="1">
-      <c r="A4" s="61">
+      <c r="N3" s="57"/>
+    </row>
+    <row r="4" spans="1:14" s="58" customFormat="1">
+      <c r="A4" s="59">
         <v>1</v>
       </c>
-      <c r="B4" s="62" t="s">
-        <v>304</v>
-      </c>
-      <c r="C4" s="61" t="s">
-        <v>262</v>
-      </c>
-      <c r="D4" s="61" t="s">
+      <c r="B4" s="60" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="63" t="s">
-        <v>264</v>
-      </c>
-      <c r="F4" s="83" t="s">
-        <v>441</v>
-      </c>
-      <c r="G4" s="63" t="s">
-        <v>440</v>
-      </c>
-      <c r="H4" s="61" t="s">
-        <v>439</v>
-      </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="64">
+      <c r="E4" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" s="76" t="s">
+        <v>436</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>435</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>434</v>
+      </c>
+      <c r="I4" s="61"/>
+      <c r="J4" s="62">
         <v>0.26</v>
       </c>
-      <c r="K4" s="64">
+      <c r="K4" s="62">
         <v>0.17899999999999999</v>
       </c>
-      <c r="L4" s="64">
+      <c r="L4" s="62">
         <v>0.1017</v>
       </c>
-      <c r="M4" s="64">
+      <c r="M4" s="62">
         <v>0.06</v>
       </c>
-      <c r="N4" s="65"/>
-    </row>
-    <row r="5" spans="1:14" s="60" customFormat="1">
+      <c r="N4" s="63"/>
+    </row>
+    <row r="5" spans="1:14" s="58" customFormat="1">
       <c r="A5" s="33">
         <v>1</v>
       </c>
-      <c r="B5" s="66" t="s">
-        <v>267</v>
+      <c r="B5" s="64" t="s">
+        <v>266</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="58" t="s">
-        <v>415</v>
-      </c>
-      <c r="H5" s="59" t="s">
+      <c r="F5" s="75"/>
+      <c r="G5" s="56" t="s">
+        <v>410</v>
+      </c>
+      <c r="H5" s="57" t="s">
         <v>26</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J5" s="29">
         <v>0.08</v>
@@ -3152,30 +3133,30 @@
       <c r="M5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="59" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="60" customFormat="1">
+      <c r="N5" s="57" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="58" customFormat="1">
       <c r="A6" s="33">
         <v>3</v>
       </c>
-      <c r="B6" s="57" t="s">
-        <v>392</v>
+      <c r="B6" s="55" t="s">
+        <v>388</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="84" t="s">
+      <c r="F6" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="56" t="s">
         <v>99</v>
       </c>
       <c r="H6" s="32" t="s">
@@ -3194,32 +3175,32 @@
       <c r="M6" s="28">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="N6" s="59"/>
-    </row>
-    <row r="7" spans="1:14" s="60" customFormat="1">
+      <c r="N6" s="57"/>
+    </row>
+    <row r="7" spans="1:14" s="58" customFormat="1">
       <c r="A7" s="33">
         <v>2</v>
       </c>
-      <c r="B7" s="57" t="s">
-        <v>393</v>
+      <c r="B7" s="55" t="s">
+        <v>389</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D7" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="56" t="s">
         <v>232</v>
       </c>
-      <c r="F7" s="84" t="s">
-        <v>442</v>
-      </c>
-      <c r="G7" s="58" t="s">
-        <v>436</v>
+      <c r="F7" s="77" t="s">
+        <v>437</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>431</v>
       </c>
       <c r="H7" s="33" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I7" s="33"/>
       <c r="J7" s="29">
@@ -3234,28 +3215,28 @@
       <c r="M7" s="29">
         <v>1.17E-2</v>
       </c>
-      <c r="N7" s="59"/>
-    </row>
-    <row r="8" spans="1:14" s="60" customFormat="1">
+      <c r="N7" s="57"/>
+    </row>
+    <row r="8" spans="1:14" s="58" customFormat="1">
       <c r="A8" s="33">
         <v>14</v>
       </c>
-      <c r="B8" s="57" t="s">
-        <v>394</v>
+      <c r="B8" s="55" t="s">
+        <v>390</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="58" t="s">
+      <c r="G8" s="56" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="32" t="s">
@@ -3274,28 +3255,28 @@
       <c r="M8" s="28">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="N8" s="59"/>
-    </row>
-    <row r="9" spans="1:14" s="60" customFormat="1">
+      <c r="N8" s="57"/>
+    </row>
+    <row r="9" spans="1:14" s="58" customFormat="1">
       <c r="A9" s="33">
         <v>3</v>
       </c>
-      <c r="B9" s="57" t="s">
-        <v>395</v>
+      <c r="B9" s="55" t="s">
+        <v>391</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="84" t="s">
+      <c r="F9" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="56" t="s">
         <v>87</v>
       </c>
       <c r="H9" s="32" t="s">
@@ -3314,68 +3295,74 @@
       <c r="M9" s="28">
         <v>0.31630000000000003</v>
       </c>
-      <c r="N9" s="59"/>
-    </row>
-    <row r="10" spans="1:14" s="60" customFormat="1">
-      <c r="A10" s="67">
+      <c r="N9" s="57"/>
+    </row>
+    <row r="10" spans="1:14" s="82" customFormat="1">
+      <c r="A10" s="71">
         <v>2</v>
       </c>
-      <c r="B10" s="68" t="s">
-        <v>396</v>
-      </c>
-      <c r="C10" s="67" t="s">
-        <v>262</v>
-      </c>
-      <c r="D10" s="67" t="s">
+      <c r="B10" s="72" t="s">
+        <v>392</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>261</v>
+      </c>
+      <c r="D10" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="69" t="s">
-        <v>343</v>
-      </c>
-      <c r="F10" s="85"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="38">
+      <c r="E10" s="73" t="s">
+        <v>342</v>
+      </c>
+      <c r="F10" s="79" t="s">
+        <v>471</v>
+      </c>
+      <c r="G10" s="73" t="s">
+        <v>472</v>
+      </c>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73" t="s">
+        <v>473</v>
+      </c>
+      <c r="J10" s="80">
         <v>0.12</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="80">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L10" s="38">
+      <c r="L10" s="80">
         <v>3.9E-2</v>
       </c>
-      <c r="M10" s="38">
+      <c r="M10" s="80">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="N10" s="39" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="60" customFormat="1">
+      <c r="N10" s="81" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="58" customFormat="1">
       <c r="A11" s="33">
         <v>2</v>
       </c>
-      <c r="B11" s="57" t="s">
-        <v>397</v>
+      <c r="B11" s="55" t="s">
+        <v>393</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="84" t="s">
-        <v>444</v>
-      </c>
-      <c r="G11" s="58" t="s">
-        <v>445</v>
+      <c r="F11" s="77" t="s">
+        <v>439</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>440</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="28">
@@ -3390,34 +3377,34 @@
       <c r="M11" s="28">
         <v>4.2079999999999999E-2</v>
       </c>
-      <c r="N11" s="59" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="60" customFormat="1">
+      <c r="N11" s="57" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="58" customFormat="1">
       <c r="A12" s="33">
         <v>30</v>
       </c>
-      <c r="B12" s="57" t="s">
-        <v>390</v>
+      <c r="B12" s="55" t="s">
+        <v>386</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="58" t="s">
-        <v>344</v>
-      </c>
-      <c r="F12" s="84" t="s">
-        <v>447</v>
-      </c>
-      <c r="G12" s="58" t="s">
-        <v>417</v>
+      <c r="E12" s="56" t="s">
+        <v>343</v>
+      </c>
+      <c r="F12" s="77" t="s">
+        <v>442</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>412</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="J12" s="28">
         <v>0.1</v>
@@ -3431,54 +3418,54 @@
       <c r="M12" s="28">
         <v>6.1500000000000001E-3</v>
       </c>
-      <c r="N12" s="59"/>
-    </row>
-    <row r="13" spans="1:14" s="60" customFormat="1">
+      <c r="N12" s="57"/>
+    </row>
+    <row r="13" spans="1:14" s="58" customFormat="1">
       <c r="A13" s="33">
         <v>1</v>
       </c>
-      <c r="B13" s="57" t="s">
-        <v>315</v>
+      <c r="B13" s="55" t="s">
+        <v>314</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="58" t="s">
-        <v>335</v>
-      </c>
-      <c r="F13" s="82"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
+      <c r="E13" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="F13" s="75"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
       <c r="J13" s="29"/>
       <c r="K13" s="29"/>
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
-      <c r="N13" s="59"/>
-    </row>
-    <row r="14" spans="1:14" s="60" customFormat="1">
+      <c r="N13" s="57"/>
+    </row>
+    <row r="14" spans="1:14" s="58" customFormat="1">
       <c r="A14" s="33">
         <v>1</v>
       </c>
-      <c r="B14" s="57" t="s">
-        <v>290</v>
+      <c r="B14" s="55" t="s">
+        <v>289</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>126</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>291</v>
-      </c>
-      <c r="E14" s="58" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="F14" s="84" t="s">
+      <c r="F14" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="56" t="s">
         <v>131</v>
       </c>
       <c r="H14" s="34" t="s">
@@ -3497,44 +3484,44 @@
       <c r="M14" s="28">
         <v>0.52</v>
       </c>
-      <c r="N14" s="59"/>
-    </row>
-    <row r="15" spans="1:14" s="60" customFormat="1">
-      <c r="A15" s="70"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
+      <c r="N14" s="57"/>
+    </row>
+    <row r="15" spans="1:14" s="58" customFormat="1">
+      <c r="A15" s="65"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
-      <c r="N15" s="73"/>
-    </row>
-    <row r="16" spans="1:14" s="60" customFormat="1">
+      <c r="N15" s="68"/>
+    </row>
+    <row r="16" spans="1:14" s="58" customFormat="1">
       <c r="A16" s="33">
         <v>4</v>
       </c>
-      <c r="B16" s="57" t="s">
-        <v>398</v>
+      <c r="B16" s="55" t="s">
+        <v>394</v>
       </c>
       <c r="C16" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="D16" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="82" t="s">
+      <c r="F16" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="58" t="s">
+      <c r="G16" s="56" t="s">
         <v>67</v>
       </c>
       <c r="H16" s="34" t="s">
@@ -3553,28 +3540,28 @@
       <c r="M16" s="28">
         <v>0.11</v>
       </c>
-      <c r="N16" s="59"/>
-    </row>
-    <row r="17" spans="1:14" s="60" customFormat="1" ht="16" customHeight="1">
+      <c r="N16" s="57"/>
+    </row>
+    <row r="17" spans="1:14" s="58" customFormat="1" ht="16" customHeight="1">
       <c r="A17" s="33">
         <v>13</v>
       </c>
-      <c r="B17" s="57" t="s">
-        <v>399</v>
+      <c r="B17" s="55" t="s">
+        <v>395</v>
       </c>
       <c r="C17" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="D17" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="E17" s="56" t="s">
         <v>293</v>
       </c>
-      <c r="E17" s="58" t="s">
-        <v>294</v>
-      </c>
-      <c r="F17" s="82" t="s">
-        <v>448</v>
-      </c>
-      <c r="G17" s="58" t="s">
+      <c r="F17" s="75" t="s">
+        <v>443</v>
+      </c>
+      <c r="G17" s="56" t="s">
         <v>248</v>
       </c>
       <c r="H17" s="25" t="s">
@@ -3593,48 +3580,48 @@
       <c r="M17" s="29">
         <v>0.30854999999999999</v>
       </c>
-      <c r="N17" s="59"/>
-    </row>
-    <row r="18" spans="1:14" s="60" customFormat="1">
-      <c r="A18" s="70"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
+      <c r="N17" s="57"/>
+    </row>
+    <row r="18" spans="1:14" s="58" customFormat="1">
+      <c r="A18" s="65"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
       <c r="M18" s="30"/>
-      <c r="N18" s="73"/>
-    </row>
-    <row r="19" spans="1:14" s="60" customFormat="1">
+      <c r="N18" s="68"/>
+    </row>
+    <row r="19" spans="1:14" s="58" customFormat="1">
       <c r="A19" s="33">
         <v>6</v>
       </c>
-      <c r="B19" s="57" t="s">
-        <v>400</v>
+      <c r="B19" s="55" t="s">
+        <v>396</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="E19" s="58"/>
-      <c r="F19" s="82" t="s">
+        <v>338</v>
+      </c>
+      <c r="E19" s="56"/>
+      <c r="F19" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="H19" s="58" t="s">
+      <c r="H19" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="I19" s="58"/>
+      <c r="I19" s="56"/>
       <c r="J19" s="29">
         <v>0.33</v>
       </c>
@@ -3647,32 +3634,32 @@
       <c r="M19" s="29">
         <v>0.1575</v>
       </c>
-      <c r="N19" s="59"/>
-    </row>
-    <row r="20" spans="1:14" s="60" customFormat="1" ht="14" customHeight="1">
+      <c r="N19" s="57"/>
+    </row>
+    <row r="20" spans="1:14" s="58" customFormat="1" ht="14" customHeight="1">
       <c r="A20" s="33">
         <v>2</v>
       </c>
-      <c r="B20" s="57" t="s">
-        <v>401</v>
+      <c r="B20" s="55" t="s">
+        <v>397</v>
       </c>
       <c r="C20" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="D20" s="33" t="s">
         <v>302</v>
       </c>
-      <c r="D20" s="33" t="s">
-        <v>303</v>
-      </c>
-      <c r="E20" s="58"/>
-      <c r="F20" s="82" t="s">
-        <v>449</v>
-      </c>
-      <c r="G20" s="58" t="s">
-        <v>418</v>
-      </c>
-      <c r="H20" s="58" t="s">
-        <v>357</v>
-      </c>
-      <c r="I20" s="58"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="75" t="s">
+        <v>444</v>
+      </c>
+      <c r="G20" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="H20" s="56" t="s">
+        <v>356</v>
+      </c>
+      <c r="I20" s="56"/>
       <c r="J20" s="29">
         <v>0.45</v>
       </c>
@@ -3685,32 +3672,32 @@
       <c r="M20" s="29">
         <v>0.23100000000000001</v>
       </c>
-      <c r="N20" s="59"/>
-    </row>
-    <row r="21" spans="1:14" s="60" customFormat="1" ht="14" customHeight="1">
+      <c r="N20" s="57"/>
+    </row>
+    <row r="21" spans="1:14" s="58" customFormat="1" ht="14" customHeight="1">
       <c r="A21" s="33">
         <v>2</v>
       </c>
-      <c r="B21" s="57" t="s">
-        <v>402</v>
+      <c r="B21" s="55" t="s">
+        <v>398</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>309</v>
-      </c>
-      <c r="E21" s="58"/>
-      <c r="F21" s="84" t="s">
-        <v>450</v>
-      </c>
-      <c r="G21" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="H21" s="58" t="s">
-        <v>358</v>
-      </c>
-      <c r="I21" s="58"/>
+        <v>308</v>
+      </c>
+      <c r="E21" s="56"/>
+      <c r="F21" s="77" t="s">
+        <v>445</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>414</v>
+      </c>
+      <c r="H21" s="56" t="s">
+        <v>357</v>
+      </c>
+      <c r="I21" s="56"/>
       <c r="J21" s="29">
         <v>0.45</v>
       </c>
@@ -3723,32 +3710,32 @@
       <c r="M21" s="29">
         <v>0.23232</v>
       </c>
-      <c r="N21" s="59"/>
-    </row>
-    <row r="22" spans="1:14" s="60" customFormat="1">
+      <c r="N21" s="57"/>
+    </row>
+    <row r="22" spans="1:14" s="58" customFormat="1">
       <c r="A22" s="33">
         <v>4</v>
       </c>
-      <c r="B22" s="57" t="s">
-        <v>403</v>
+      <c r="B22" s="55" t="s">
+        <v>399</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>340</v>
-      </c>
-      <c r="E22" s="58"/>
-      <c r="F22" s="82" t="s">
-        <v>451</v>
-      </c>
-      <c r="G22" s="58" t="s">
-        <v>420</v>
-      </c>
-      <c r="H22" s="58" t="s">
-        <v>359</v>
-      </c>
-      <c r="I22" s="58"/>
+        <v>339</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="75" t="s">
+        <v>446</v>
+      </c>
+      <c r="G22" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="H22" s="56" t="s">
+        <v>358</v>
+      </c>
+      <c r="I22" s="56"/>
       <c r="J22" s="29">
         <v>0.77</v>
       </c>
@@ -3761,34 +3748,34 @@
       <c r="M22" s="29">
         <v>0.42336000000000001</v>
       </c>
-      <c r="N22" s="59"/>
-    </row>
-    <row r="23" spans="1:14" s="60" customFormat="1">
+      <c r="N22" s="57"/>
+    </row>
+    <row r="23" spans="1:14" s="58" customFormat="1">
       <c r="A23" s="33">
         <v>1</v>
       </c>
-      <c r="B23" s="57" t="s">
+      <c r="B23" s="55" t="s">
+        <v>335</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="D23" s="33" t="s">
         <v>336</v>
       </c>
-      <c r="C23" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="E23" s="58" t="s">
-        <v>342</v>
-      </c>
-      <c r="F23" s="82" t="s">
+      <c r="E23" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="F23" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="74" t="s">
+      <c r="H23" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="I23" s="74"/>
+      <c r="I23" s="69"/>
       <c r="J23" s="28">
         <v>0.97</v>
       </c>
@@ -3801,56 +3788,56 @@
       <c r="M23" s="28">
         <v>0.41</v>
       </c>
-      <c r="N23" s="59"/>
-    </row>
-    <row r="24" spans="1:14" s="60" customFormat="1">
+      <c r="N23" s="57"/>
+    </row>
+    <row r="24" spans="1:14" s="58" customFormat="1">
       <c r="A24" s="33">
         <v>7</v>
       </c>
-      <c r="B24" s="57" t="s">
-        <v>404</v>
+      <c r="B24" s="55" t="s">
+        <v>400</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="E24" s="58"/>
-      <c r="F24" s="82" t="s">
-        <v>474</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>473</v>
-      </c>
-      <c r="H24" s="58" t="s">
-        <v>472</v>
-      </c>
-      <c r="I24" s="58"/>
+        <v>299</v>
+      </c>
+      <c r="E24" s="56"/>
+      <c r="F24" s="75" t="s">
+        <v>469</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>468</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>467</v>
+      </c>
+      <c r="I24" s="56"/>
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
-      <c r="N24" s="59"/>
-    </row>
-    <row r="25" spans="1:14" s="60" customFormat="1">
+      <c r="N24" s="57"/>
+    </row>
+    <row r="25" spans="1:14" s="58" customFormat="1">
       <c r="A25" s="33">
         <v>1</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="55" t="s">
+        <v>321</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="D25" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="C25" s="33" t="s">
-        <v>324</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="E25" s="58"/>
-      <c r="F25" s="84" t="s">
+      <c r="E25" s="56"/>
+      <c r="F25" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="G25" s="58" t="s">
+      <c r="G25" s="56" t="s">
         <v>118</v>
       </c>
       <c r="H25" s="34" t="s">
@@ -3869,32 +3856,32 @@
       <c r="M25" s="28">
         <v>0.25</v>
       </c>
-      <c r="N25" s="59"/>
-    </row>
-    <row r="26" spans="1:14" s="60" customFormat="1">
+      <c r="N25" s="57"/>
+    </row>
+    <row r="26" spans="1:14" s="58" customFormat="1">
       <c r="A26" s="33">
         <v>1</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="55" t="s">
+        <v>325</v>
+      </c>
+      <c r="C26" s="33" t="s">
         <v>326</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="D26" s="33" t="s">
         <v>327</v>
       </c>
-      <c r="D26" s="33" t="s">
-        <v>328</v>
-      </c>
-      <c r="E26" s="58"/>
-      <c r="F26" s="84" t="s">
-        <v>452</v>
-      </c>
-      <c r="G26" s="58" t="s">
-        <v>328</v>
-      </c>
-      <c r="H26" s="58" t="s">
-        <v>360</v>
-      </c>
-      <c r="I26" s="58"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="77" t="s">
+        <v>447</v>
+      </c>
+      <c r="G26" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="H26" s="56" t="s">
+        <v>359</v>
+      </c>
+      <c r="I26" s="56"/>
       <c r="J26" s="29">
         <v>1.2</v>
       </c>
@@ -3907,51 +3894,51 @@
       <c r="M26" s="29">
         <v>0.6512</v>
       </c>
-      <c r="N26" s="59"/>
-    </row>
-    <row r="27" spans="1:14" s="60" customFormat="1">
-      <c r="A27" s="70"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
+      <c r="N26" s="57"/>
+    </row>
+    <row r="27" spans="1:14" s="58" customFormat="1">
+      <c r="A27" s="65"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
       <c r="M27" s="30"/>
-      <c r="N27" s="73"/>
-    </row>
-    <row r="28" spans="1:14" s="60" customFormat="1">
+      <c r="N27" s="68"/>
+    </row>
+    <row r="28" spans="1:14" s="58" customFormat="1">
       <c r="A28" s="33">
         <v>1</v>
       </c>
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="55" t="s">
+        <v>380</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>381</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="E28" s="56" t="s">
         <v>383</v>
       </c>
-      <c r="C28" s="33" t="s">
-        <v>384</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>387</v>
-      </c>
-      <c r="E28" s="58" t="s">
-        <v>386</v>
-      </c>
-      <c r="F28" s="82" t="s">
-        <v>453</v>
-      </c>
-      <c r="G28" s="58" t="s">
-        <v>422</v>
-      </c>
-      <c r="H28" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="I28" s="58" t="s">
-        <v>385</v>
+      <c r="F28" s="75" t="s">
+        <v>448</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>417</v>
+      </c>
+      <c r="H28" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="I28" s="56" t="s">
+        <v>382</v>
       </c>
       <c r="J28" s="29">
         <v>0.95</v>
@@ -3965,48 +3952,46 @@
       <c r="M28" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="N28" s="59" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="60" customFormat="1">
-      <c r="A29" s="70"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
+      <c r="N28" s="57"/>
+    </row>
+    <row r="29" spans="1:14" s="58" customFormat="1">
+      <c r="A29" s="65"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
       <c r="J29" s="30"/>
       <c r="K29" s="30"/>
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
-      <c r="N29" s="73"/>
-    </row>
-    <row r="30" spans="1:14" s="60" customFormat="1">
+      <c r="N29" s="68"/>
+    </row>
+    <row r="30" spans="1:14" s="58" customFormat="1">
       <c r="A30" s="33">
         <v>1</v>
       </c>
-      <c r="B30" s="57" t="s">
-        <v>329</v>
+      <c r="B30" s="55" t="s">
+        <v>328</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>133</v>
       </c>
       <c r="D30" s="33"/>
-      <c r="E30" s="58" t="s">
-        <v>330</v>
-      </c>
-      <c r="F30" s="82" t="s">
-        <v>454</v>
-      </c>
-      <c r="G30" s="58" t="s">
+      <c r="E30" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="F30" s="75" t="s">
+        <v>449</v>
+      </c>
+      <c r="G30" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="H30" s="58" t="s">
-        <v>362</v>
+      <c r="H30" s="56" t="s">
+        <v>361</v>
       </c>
       <c r="I30" s="33" t="s">
         <v>138</v>
@@ -4023,36 +4008,36 @@
       <c r="M30" s="29">
         <v>0.67700000000000005</v>
       </c>
-      <c r="N30" s="59" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="60" customFormat="1">
+      <c r="N30" s="57" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="58" customFormat="1">
       <c r="A31" s="33">
         <v>8</v>
       </c>
-      <c r="B31" s="57" t="s">
-        <v>405</v>
+      <c r="B31" s="55" t="s">
+        <v>401</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D31" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="58" t="s">
-        <v>296</v>
-      </c>
-      <c r="F31" s="84" t="s">
+      <c r="E31" s="56" t="s">
+        <v>295</v>
+      </c>
+      <c r="F31" s="77" t="s">
         <v>183</v>
       </c>
-      <c r="G31" s="58" t="s">
+      <c r="G31" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="H31" s="58" t="s">
+      <c r="H31" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="I31" s="58"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="29">
         <v>0.09</v>
       </c>
@@ -4065,50 +4050,50 @@
       <c r="M31" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="N31" s="59"/>
-    </row>
-    <row r="32" spans="1:14" s="60" customFormat="1">
-      <c r="A32" s="70"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="72"/>
+      <c r="N31" s="57"/>
+    </row>
+    <row r="32" spans="1:14" s="58" customFormat="1">
+      <c r="A32" s="65"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
       <c r="L32" s="30"/>
       <c r="M32" s="30"/>
-      <c r="N32" s="73"/>
-    </row>
-    <row r="33" spans="1:14" s="60" customFormat="1">
+      <c r="N32" s="68"/>
+    </row>
+    <row r="33" spans="1:14" s="58" customFormat="1">
       <c r="A33" s="33">
         <v>1</v>
       </c>
-      <c r="B33" s="57" t="s">
+      <c r="B33" s="55" t="s">
+        <v>275</v>
+      </c>
+      <c r="C33" s="33" t="s">
         <v>276</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="D33" s="33" t="s">
         <v>277</v>
       </c>
-      <c r="D33" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="E33" s="58" t="s">
-        <v>281</v>
-      </c>
-      <c r="F33" s="84" t="s">
-        <v>455</v>
-      </c>
-      <c r="G33" s="58" t="s">
-        <v>281</v>
-      </c>
-      <c r="H33" s="58" t="s">
-        <v>364</v>
-      </c>
-      <c r="I33" s="58"/>
+      <c r="E33" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="F33" s="77" t="s">
+        <v>450</v>
+      </c>
+      <c r="G33" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="H33" s="56" t="s">
+        <v>363</v>
+      </c>
+      <c r="I33" s="56"/>
       <c r="J33" s="29">
         <v>0.22</v>
       </c>
@@ -4121,93 +4106,93 @@
       <c r="M33" s="29">
         <v>4.0500000000000001E-2</v>
       </c>
-      <c r="N33" s="59"/>
-    </row>
-    <row r="34" spans="1:14" s="60" customFormat="1">
-      <c r="A34" s="70"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
+      <c r="N33" s="57"/>
+    </row>
+    <row r="34" spans="1:14" s="58" customFormat="1">
+      <c r="A34" s="65"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="67"/>
       <c r="J34" s="30"/>
       <c r="K34" s="30"/>
       <c r="L34" s="30"/>
       <c r="M34" s="30"/>
-      <c r="N34" s="73"/>
-    </row>
-    <row r="35" spans="1:14" s="60" customFormat="1">
+      <c r="N34" s="68"/>
+    </row>
+    <row r="35" spans="1:14" s="58" customFormat="1">
       <c r="A35" s="33">
         <v>3</v>
       </c>
-      <c r="B35" s="57" t="s">
-        <v>406</v>
+      <c r="B35" s="55" t="s">
+        <v>402</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="58" t="s">
-        <v>345</v>
-      </c>
-      <c r="F35" s="82"/>
-      <c r="G35" s="58"/>
+      <c r="E35" s="56" t="s">
+        <v>344</v>
+      </c>
+      <c r="F35" s="75"/>
+      <c r="G35" s="56"/>
       <c r="H35" s="32"/>
       <c r="I35" s="32"/>
       <c r="J35" s="28"/>
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
       <c r="M35" s="28"/>
-      <c r="N35" s="59"/>
-    </row>
-    <row r="36" spans="1:14" s="60" customFormat="1">
-      <c r="A36" s="61">
+      <c r="N35" s="57"/>
+    </row>
+    <row r="36" spans="1:14" s="58" customFormat="1">
+      <c r="A36" s="59">
         <v>2</v>
       </c>
-      <c r="B36" s="62" t="s">
-        <v>407</v>
-      </c>
-      <c r="C36" s="61" t="s">
+      <c r="B36" s="60" t="s">
+        <v>403</v>
+      </c>
+      <c r="C36" s="59" t="s">
         <v>256</v>
       </c>
-      <c r="D36" s="61" t="s">
+      <c r="D36" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="63" t="s">
+      <c r="E36" s="61" t="s">
+        <v>364</v>
+      </c>
+      <c r="F36" s="76" t="s">
+        <v>451</v>
+      </c>
+      <c r="G36" s="61" t="s">
+        <v>418</v>
+      </c>
+      <c r="H36" s="61" t="s">
         <v>365</v>
       </c>
-      <c r="F36" s="83" t="s">
-        <v>456</v>
-      </c>
-      <c r="G36" s="63" t="s">
-        <v>423</v>
-      </c>
-      <c r="H36" s="63" t="s">
+      <c r="I36" s="61"/>
+      <c r="J36" s="62" t="s">
         <v>366</v>
       </c>
-      <c r="I36" s="63"/>
-      <c r="J36" s="64" t="s">
-        <v>367</v>
-      </c>
-      <c r="K36" s="64">
+      <c r="K36" s="62">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="L36" s="64">
+      <c r="L36" s="62">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="M36" s="64">
+      <c r="M36" s="62">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="N36" s="65"/>
-    </row>
-    <row r="37" spans="1:14" s="60" customFormat="1">
+      <c r="N36" s="63"/>
+    </row>
+    <row r="37" spans="1:14" s="58" customFormat="1">
       <c r="A37" s="33">
         <v>1</v>
       </c>
-      <c r="B37" s="57" t="s">
+      <c r="B37" s="55" t="s">
         <v>260</v>
       </c>
       <c r="C37" s="33" t="s">
@@ -4216,17 +4201,17 @@
       <c r="D37" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="58">
+      <c r="E37" s="56">
         <v>120</v>
       </c>
-      <c r="F37" s="84" t="s">
-        <v>457</v>
-      </c>
-      <c r="G37" s="58" t="s">
-        <v>438</v>
+      <c r="F37" s="77" t="s">
+        <v>452</v>
+      </c>
+      <c r="G37" s="56" t="s">
+        <v>433</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I37" s="33"/>
       <c r="J37" s="29">
@@ -4241,14 +4226,14 @@
       <c r="M37" s="29">
         <v>2.3560000000000001E-2</v>
       </c>
-      <c r="N37" s="59"/>
-    </row>
-    <row r="38" spans="1:14" s="60" customFormat="1">
+      <c r="N37" s="57"/>
+    </row>
+    <row r="38" spans="1:14" s="58" customFormat="1">
       <c r="A38" s="33">
-        <v>8</v>
-      </c>
-      <c r="B38" s="57" t="s">
-        <v>408</v>
+        <v>9</v>
+      </c>
+      <c r="B38" s="55" t="s">
+        <v>470</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>256</v>
@@ -4256,13 +4241,13 @@
       <c r="D38" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="58">
+      <c r="E38" s="56">
         <v>649</v>
       </c>
-      <c r="F38" s="84" t="s">
+      <c r="F38" s="77" t="s">
         <v>193</v>
       </c>
-      <c r="G38" s="58" t="s">
+      <c r="G38" s="56" t="s">
         <v>195</v>
       </c>
       <c r="H38" s="32" t="s">
@@ -4281,42 +4266,54 @@
       <c r="M38" s="28">
         <v>3.8400000000000001E-3</v>
       </c>
-      <c r="N38" s="59"/>
-    </row>
-    <row r="39" spans="1:14" s="60" customFormat="1">
-      <c r="A39" s="76">
+      <c r="N38" s="57"/>
+    </row>
+    <row r="39" spans="1:14" s="58" customFormat="1">
+      <c r="A39" s="33">
         <v>1</v>
       </c>
-      <c r="B39" s="77" t="s">
-        <v>261</v>
-      </c>
-      <c r="C39" s="76" t="s">
+      <c r="B39" s="55" t="s">
+        <v>264</v>
+      </c>
+      <c r="C39" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="D39" s="76" t="s">
+      <c r="D39" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="78">
-        <v>675</v>
-      </c>
-      <c r="F39" s="87"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="78"/>
-      <c r="I39" s="78"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="80" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" s="60" customFormat="1">
+      <c r="E39" s="56" t="s">
+        <v>265</v>
+      </c>
+      <c r="F39" s="77" t="s">
+        <v>453</v>
+      </c>
+      <c r="G39" s="56" t="s">
+        <v>419</v>
+      </c>
+      <c r="H39" s="56" t="s">
+        <v>367</v>
+      </c>
+      <c r="I39" s="33"/>
+      <c r="J39" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="K39" s="29">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L39" s="29">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="M39" s="29">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N39" s="57"/>
+    </row>
+    <row r="40" spans="1:14" s="58" customFormat="1">
       <c r="A40" s="33">
-        <v>1</v>
-      </c>
-      <c r="B40" s="57" t="s">
-        <v>265</v>
+        <v>11</v>
+      </c>
+      <c r="B40" s="55" t="s">
+        <v>404</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>256</v>
@@ -4324,17 +4321,17 @@
       <c r="D40" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="58" t="s">
-        <v>266</v>
-      </c>
-      <c r="F40" s="84" t="s">
-        <v>458</v>
-      </c>
-      <c r="G40" s="58" t="s">
-        <v>424</v>
-      </c>
-      <c r="H40" s="58" t="s">
-        <v>369</v>
+      <c r="E40" s="56" t="s">
+        <v>267</v>
+      </c>
+      <c r="F40" s="77" t="s">
+        <v>454</v>
+      </c>
+      <c r="G40" s="56" t="s">
+        <v>420</v>
+      </c>
+      <c r="H40" s="56" t="s">
+        <v>368</v>
       </c>
       <c r="I40" s="33"/>
       <c r="J40" s="29">
@@ -4349,14 +4346,14 @@
       <c r="M40" s="29">
         <v>2.4E-2</v>
       </c>
-      <c r="N40" s="59"/>
-    </row>
-    <row r="41" spans="1:14" s="60" customFormat="1">
+      <c r="N40" s="57"/>
+    </row>
+    <row r="41" spans="1:14" s="58" customFormat="1" ht="14" customHeight="1">
       <c r="A41" s="33">
-        <v>11</v>
-      </c>
-      <c r="B41" s="57" t="s">
-        <v>409</v>
+        <v>30</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>387</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>256</v>
@@ -4364,39 +4361,37 @@
       <c r="D41" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="58" t="s">
-        <v>268</v>
-      </c>
-      <c r="F41" s="84" t="s">
-        <v>459</v>
-      </c>
-      <c r="G41" s="58" t="s">
-        <v>425</v>
-      </c>
-      <c r="H41" s="58" t="s">
-        <v>370</v>
-      </c>
-      <c r="I41" s="33"/>
+      <c r="E41" s="56" t="s">
+        <v>347</v>
+      </c>
+      <c r="F41" s="77" t="s">
+        <v>455</v>
+      </c>
+      <c r="G41" s="56" t="s">
+        <v>421</v>
+      </c>
+      <c r="H41" s="56" t="s">
+        <v>348</v>
+      </c>
+      <c r="I41" s="56"/>
       <c r="J41" s="29">
-        <v>0.08</v>
-      </c>
-      <c r="K41" s="29">
-        <v>6.9000000000000006E-2</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="K41" s="29"/>
       <c r="L41" s="29">
-        <v>4.0800000000000003E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="M41" s="29">
-        <v>2.4E-2</v>
-      </c>
-      <c r="N41" s="59"/>
-    </row>
-    <row r="42" spans="1:14" s="60" customFormat="1" ht="14" customHeight="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="N41" s="57"/>
+    </row>
+    <row r="42" spans="1:14" s="58" customFormat="1" ht="14" customHeight="1">
       <c r="A42" s="33">
-        <v>30</v>
-      </c>
-      <c r="B42" s="57" t="s">
-        <v>391</v>
+        <v>1</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>269</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>256</v>
@@ -4404,37 +4399,39 @@
       <c r="D42" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="58" t="s">
-        <v>348</v>
-      </c>
-      <c r="F42" s="84" t="s">
-        <v>460</v>
-      </c>
-      <c r="G42" s="58" t="s">
-        <v>426</v>
-      </c>
-      <c r="H42" s="58" t="s">
-        <v>349</v>
-      </c>
-      <c r="I42" s="58"/>
-      <c r="J42" s="29">
+      <c r="E42" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="G42" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="H42" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="I42" s="32"/>
+      <c r="J42" s="28">
         <v>0.1</v>
       </c>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="M42" s="29">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="N42" s="59"/>
-    </row>
-    <row r="43" spans="1:14" s="60" customFormat="1" ht="14" customHeight="1">
+      <c r="K42" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L42" s="28">
+        <v>1.14E-2</v>
+      </c>
+      <c r="M42" s="28">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="N42" s="57"/>
+    </row>
+    <row r="43" spans="1:14" s="58" customFormat="1">
       <c r="A43" s="33">
-        <v>1</v>
-      </c>
-      <c r="B43" s="57" t="s">
-        <v>270</v>
+        <v>6</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>405</v>
       </c>
       <c r="C43" s="33" t="s">
         <v>256</v>
@@ -4442,39 +4439,39 @@
       <c r="D43" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E43" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="F43" s="84" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="H43" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="I43" s="32"/>
-      <c r="J43" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="K43" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="L43" s="28">
-        <v>1.14E-2</v>
-      </c>
-      <c r="M43" s="28">
-        <v>4.1599999999999996E-3</v>
-      </c>
-      <c r="N43" s="59"/>
-    </row>
-    <row r="44" spans="1:14" s="60" customFormat="1">
+      <c r="E43" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="F43" s="77" t="s">
+        <v>457</v>
+      </c>
+      <c r="G43" s="56" t="s">
+        <v>422</v>
+      </c>
+      <c r="H43" s="56" t="s">
+        <v>456</v>
+      </c>
+      <c r="I43" s="56"/>
+      <c r="J43" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="K43" s="29">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L43" s="29">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="M43" s="29">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N43" s="57"/>
+    </row>
+    <row r="44" spans="1:14" s="58" customFormat="1">
       <c r="A44" s="33">
-        <v>6</v>
-      </c>
-      <c r="B44" s="57" t="s">
-        <v>410</v>
+        <v>1</v>
+      </c>
+      <c r="B44" s="55" t="s">
+        <v>268</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>256</v>
@@ -4482,39 +4479,39 @@
       <c r="D44" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="58" t="s">
-        <v>263</v>
-      </c>
-      <c r="F44" s="84" t="s">
-        <v>462</v>
-      </c>
-      <c r="G44" s="58" t="s">
-        <v>427</v>
-      </c>
-      <c r="H44" s="58" t="s">
-        <v>461</v>
-      </c>
-      <c r="I44" s="58"/>
-      <c r="J44" s="29">
-        <v>0.08</v>
-      </c>
-      <c r="K44" s="29">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="L44" s="29">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="M44" s="29">
-        <v>2.4E-2</v>
-      </c>
-      <c r="N44" s="59"/>
-    </row>
-    <row r="45" spans="1:14" s="60" customFormat="1">
+      <c r="E44" s="56" t="s">
+        <v>198</v>
+      </c>
+      <c r="F44" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="G44" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="H44" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="I44" s="32"/>
+      <c r="J44" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="K44" s="28">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L44" s="28">
+        <v>1.14E-2</v>
+      </c>
+      <c r="M44" s="28">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="N44" s="57"/>
+    </row>
+    <row r="45" spans="1:14" s="58" customFormat="1">
       <c r="A45" s="33">
         <v>1</v>
       </c>
-      <c r="B45" s="57" t="s">
-        <v>269</v>
+      <c r="B45" s="64" t="s">
+        <v>345</v>
       </c>
       <c r="C45" s="33" t="s">
         <v>256</v>
@@ -4522,638 +4519,598 @@
       <c r="D45" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="58" t="s">
-        <v>198</v>
-      </c>
-      <c r="F45" s="84" t="s">
-        <v>199</v>
-      </c>
-      <c r="G45" s="58" t="s">
-        <v>200</v>
+      <c r="E45" s="56" t="s">
+        <v>346</v>
+      </c>
+      <c r="F45" s="77" t="s">
+        <v>458</v>
+      </c>
+      <c r="G45" s="56" t="s">
+        <v>423</v>
       </c>
       <c r="H45" s="32" t="s">
-        <v>201</v>
+        <v>369</v>
       </c>
       <c r="I45" s="32"/>
-      <c r="J45" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="K45" s="28">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="L45" s="28">
-        <v>1.14E-2</v>
-      </c>
-      <c r="M45" s="28">
-        <v>4.1599999999999996E-3</v>
-      </c>
-      <c r="N45" s="59"/>
-    </row>
-    <row r="46" spans="1:14" s="60" customFormat="1">
-      <c r="A46" s="33">
+      <c r="J45" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="K45" s="29">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L45" s="29">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="M45" s="29">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N45" s="57"/>
+    </row>
+    <row r="46" spans="1:14" s="58" customFormat="1">
+      <c r="A46" s="65"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="67"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="68"/>
+    </row>
+    <row r="47" spans="1:14" s="58" customFormat="1">
+      <c r="A47" s="33">
+        <v>2</v>
+      </c>
+      <c r="B47" s="55" t="s">
+        <v>406</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="E47" s="56" t="s">
+        <v>320</v>
+      </c>
+      <c r="F47" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="G47" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="H47" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="I47" s="34"/>
+      <c r="J47" s="28">
+        <v>0.21</v>
+      </c>
+      <c r="K47" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="L47" s="28">
+        <v>0.18</v>
+      </c>
+      <c r="M47" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="N47" s="57"/>
+    </row>
+    <row r="48" spans="1:14" s="58" customFormat="1">
+      <c r="A48" s="65"/>
+      <c r="B48" s="66"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="68"/>
+    </row>
+    <row r="49" spans="1:14" s="58" customFormat="1">
+      <c r="A49" s="33">
         <v>1</v>
       </c>
-      <c r="B46" s="66" t="s">
-        <v>346</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="D46" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="58" t="s">
-        <v>347</v>
-      </c>
-      <c r="F46" s="84" t="s">
-        <v>463</v>
-      </c>
-      <c r="G46" s="58" t="s">
-        <v>428</v>
-      </c>
-      <c r="H46" s="32" t="s">
-        <v>371</v>
-      </c>
-      <c r="I46" s="32"/>
-      <c r="J46" s="29">
-        <v>0.08</v>
-      </c>
-      <c r="K46" s="29">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="L46" s="29">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="M46" s="29">
-        <v>2.4E-2</v>
-      </c>
-      <c r="N46" s="59"/>
-    </row>
-    <row r="47" spans="1:14" s="60" customFormat="1">
-      <c r="A47" s="70"/>
-      <c r="B47" s="71"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="86"/>
-      <c r="G47" s="72"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="72"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="73"/>
-    </row>
-    <row r="48" spans="1:14" s="60" customFormat="1">
-      <c r="A48" s="33">
-        <v>2</v>
-      </c>
-      <c r="B48" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>319</v>
-      </c>
-      <c r="D48" s="33" t="s">
-        <v>320</v>
-      </c>
-      <c r="E48" s="58" t="s">
-        <v>321</v>
-      </c>
-      <c r="F48" s="84" t="s">
-        <v>121</v>
-      </c>
-      <c r="G48" s="58" t="s">
-        <v>123</v>
-      </c>
-      <c r="H48" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="I48" s="34"/>
-      <c r="J48" s="28">
-        <v>0.21</v>
-      </c>
-      <c r="K48" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="L48" s="28">
-        <v>0.18</v>
-      </c>
-      <c r="M48" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="N48" s="59"/>
-    </row>
-    <row r="49" spans="1:14" s="60" customFormat="1">
-      <c r="A49" s="70"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="70"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="86"/>
-      <c r="G49" s="72"/>
-      <c r="H49" s="72"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="31"/>
-      <c r="K49" s="31"/>
-      <c r="L49" s="31"/>
-      <c r="M49" s="31"/>
-      <c r="N49" s="73"/>
-    </row>
-    <row r="50" spans="1:14" s="60" customFormat="1">
+      <c r="B49" s="55" t="s">
+        <v>255</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="E49" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="69"/>
+      <c r="J49" s="28">
+        <v>15.75</v>
+      </c>
+      <c r="K49" s="28">
+        <v>14.318</v>
+      </c>
+      <c r="L49" s="28">
+        <v>12.170299999999999</v>
+      </c>
+      <c r="M49" s="28">
+        <v>9.5214700000000008</v>
+      </c>
+      <c r="N49" s="57"/>
+    </row>
+    <row r="50" spans="1:14" s="58" customFormat="1">
       <c r="A50" s="33">
         <v>1</v>
       </c>
-      <c r="B50" s="57" t="s">
-        <v>255</v>
+      <c r="B50" s="55" t="s">
+        <v>313</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>282</v>
+        <v>354</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="E50" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="84" t="s">
-        <v>21</v>
-      </c>
-      <c r="G50" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="H50" s="74" t="s">
-        <v>24</v>
-      </c>
-      <c r="I50" s="74"/>
+        <v>350</v>
+      </c>
+      <c r="E50" s="56" t="s">
+        <v>349</v>
+      </c>
+      <c r="F50" s="77" t="s">
+        <v>459</v>
+      </c>
+      <c r="G50" s="56" t="s">
+        <v>424</v>
+      </c>
+      <c r="H50" s="69" t="s">
+        <v>372</v>
+      </c>
+      <c r="I50" s="69"/>
       <c r="J50" s="28">
-        <v>15.75</v>
+        <v>0.61</v>
       </c>
       <c r="K50" s="28">
-        <v>14.318</v>
+        <v>0.51</v>
       </c>
       <c r="L50" s="28">
-        <v>12.170299999999999</v>
-      </c>
-      <c r="M50" s="28">
-        <v>9.5214700000000008</v>
-      </c>
-      <c r="N50" s="59"/>
-    </row>
-    <row r="51" spans="1:14" s="60" customFormat="1">
+        <v>0.39</v>
+      </c>
+      <c r="M50" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="N50" s="57"/>
+    </row>
+    <row r="51" spans="1:14" s="58" customFormat="1">
       <c r="A51" s="33">
         <v>1</v>
       </c>
-      <c r="B51" s="57" t="s">
-        <v>314</v>
+      <c r="B51" s="55" t="s">
+        <v>324</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="E51" s="58" t="s">
-        <v>350</v>
-      </c>
-      <c r="F51" s="84" t="s">
-        <v>464</v>
-      </c>
-      <c r="G51" s="58" t="s">
-        <v>429</v>
-      </c>
-      <c r="H51" s="74" t="s">
-        <v>374</v>
-      </c>
-      <c r="I51" s="74"/>
+        <v>352</v>
+      </c>
+      <c r="E51" s="56" t="s">
+        <v>353</v>
+      </c>
+      <c r="F51" s="77" t="s">
+        <v>460</v>
+      </c>
+      <c r="G51" s="56" t="s">
+        <v>425</v>
+      </c>
+      <c r="H51" s="69" t="s">
+        <v>373</v>
+      </c>
+      <c r="I51" s="33"/>
       <c r="J51" s="28">
-        <v>0.61</v>
+        <v>0.97</v>
       </c>
       <c r="K51" s="28">
-        <v>0.51</v>
+        <v>8.6199999999999999E-2</v>
       </c>
       <c r="L51" s="28">
-        <v>0.39</v>
+        <v>0.72</v>
       </c>
       <c r="M51" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="N51" s="59"/>
-    </row>
-    <row r="52" spans="1:14" s="60" customFormat="1">
+      <c r="N51" s="57"/>
+    </row>
+    <row r="52" spans="1:14" s="58" customFormat="1">
       <c r="A52" s="33">
         <v>1</v>
       </c>
-      <c r="B52" s="57" t="s">
-        <v>325</v>
+      <c r="B52" s="55" t="s">
+        <v>270</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>352</v>
+        <v>271</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>353</v>
-      </c>
-      <c r="E52" s="58" t="s">
-        <v>354</v>
-      </c>
-      <c r="F52" s="84" t="s">
-        <v>465</v>
-      </c>
-      <c r="G52" s="58" t="s">
-        <v>430</v>
-      </c>
-      <c r="H52" s="74" t="s">
-        <v>375</v>
-      </c>
-      <c r="I52" s="33"/>
+        <v>272</v>
+      </c>
+      <c r="E52" s="56" t="s">
+        <v>355</v>
+      </c>
+      <c r="F52" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="G52" s="56" t="s">
+        <v>426</v>
+      </c>
+      <c r="H52" s="34" t="s">
+        <v>374</v>
+      </c>
+      <c r="I52" s="34"/>
       <c r="J52" s="28">
-        <v>0.97</v>
+        <v>0.79</v>
       </c>
       <c r="K52" s="28">
-        <v>8.6199999999999999E-2</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="L52" s="28">
-        <v>0.72</v>
-      </c>
-      <c r="M52" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="N52" s="59"/>
-    </row>
-    <row r="53" spans="1:14" s="60" customFormat="1">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="M52" s="28">
+        <v>0.317</v>
+      </c>
+      <c r="N52" s="57"/>
+    </row>
+    <row r="53" spans="1:14" s="58" customFormat="1">
       <c r="A53" s="33">
         <v>1</v>
       </c>
-      <c r="B53" s="57" t="s">
-        <v>271</v>
+      <c r="B53" s="55" t="s">
+        <v>309</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>272</v>
+        <v>310</v>
       </c>
       <c r="D53" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="E53" s="58" t="s">
-        <v>356</v>
-      </c>
-      <c r="F53" s="84" t="s">
-        <v>171</v>
-      </c>
-      <c r="G53" s="58" t="s">
-        <v>431</v>
-      </c>
-      <c r="H53" s="34" t="s">
-        <v>376</v>
-      </c>
-      <c r="I53" s="34"/>
-      <c r="J53" s="28">
-        <v>0.79</v>
-      </c>
-      <c r="K53" s="28">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="L53" s="28">
-        <v>0.39600000000000002</v>
-      </c>
-      <c r="M53" s="28">
-        <v>0.317</v>
-      </c>
-      <c r="N53" s="59"/>
-    </row>
-    <row r="54" spans="1:14" s="60" customFormat="1">
+        <v>311</v>
+      </c>
+      <c r="E53" s="56" t="s">
+        <v>312</v>
+      </c>
+      <c r="F53" s="77" t="s">
+        <v>217</v>
+      </c>
+      <c r="G53" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="H53" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="I53" s="35"/>
+      <c r="J53" s="29">
+        <v>1.82</v>
+      </c>
+      <c r="K53" s="29">
+        <v>1.7290000000000001</v>
+      </c>
+      <c r="L53" s="29">
+        <v>1.5556000000000001</v>
+      </c>
+      <c r="M53" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N53" s="57"/>
+    </row>
+    <row r="54" spans="1:14" s="58" customFormat="1" ht="15" customHeight="1">
       <c r="A54" s="33">
         <v>1</v>
       </c>
-      <c r="B54" s="57" t="s">
-        <v>310</v>
+      <c r="B54" s="55" t="s">
+        <v>285</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>311</v>
+        <v>286</v>
       </c>
       <c r="D54" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="E54" s="58" t="s">
-        <v>313</v>
-      </c>
-      <c r="F54" s="84" t="s">
-        <v>217</v>
-      </c>
-      <c r="G54" s="58" t="s">
-        <v>214</v>
+        <v>287</v>
+      </c>
+      <c r="E54" s="56" t="s">
+        <v>288</v>
+      </c>
+      <c r="F54" s="77" t="s">
+        <v>223</v>
+      </c>
+      <c r="G54" s="56" t="s">
+        <v>225</v>
       </c>
       <c r="H54" s="35" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="I54" s="35"/>
       <c r="J54" s="29">
-        <v>1.82</v>
+        <v>6.97</v>
       </c>
       <c r="K54" s="29">
-        <v>1.7290000000000001</v>
+        <v>6.26</v>
       </c>
       <c r="L54" s="29">
-        <v>1.5556000000000001</v>
-      </c>
-      <c r="M54" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="N54" s="59"/>
-    </row>
-    <row r="55" spans="1:14" s="60" customFormat="1" ht="15" customHeight="1">
+        <v>5.157</v>
+      </c>
+      <c r="M54" s="29">
+        <v>3.375</v>
+      </c>
+      <c r="N54" s="57"/>
+    </row>
+    <row r="55" spans="1:14" s="58" customFormat="1">
       <c r="A55" s="33">
+        <v>4</v>
+      </c>
+      <c r="B55" s="55" t="s">
+        <v>407</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="E55" s="56" t="s">
+        <v>298</v>
+      </c>
+      <c r="F55" s="77" t="s">
+        <v>461</v>
+      </c>
+      <c r="G55" s="56" t="s">
+        <v>250</v>
+      </c>
+      <c r="H55" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="I55" s="36"/>
+      <c r="J55" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="K55" s="29">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="L55" s="29">
+        <v>0.63</v>
+      </c>
+      <c r="M55" s="29">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="N55" s="57"/>
+    </row>
+    <row r="56" spans="1:14" s="58" customFormat="1">
+      <c r="A56" s="33">
         <v>1</v>
       </c>
-      <c r="B55" s="57" t="s">
-        <v>286</v>
-      </c>
-      <c r="C55" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="D55" s="33" t="s">
-        <v>288</v>
-      </c>
-      <c r="E55" s="58" t="s">
-        <v>289</v>
-      </c>
-      <c r="F55" s="84" t="s">
-        <v>223</v>
-      </c>
-      <c r="G55" s="58" t="s">
-        <v>225</v>
-      </c>
-      <c r="H55" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="I55" s="35"/>
-      <c r="J55" s="29">
-        <v>6.97</v>
-      </c>
-      <c r="K55" s="29">
-        <v>6.26</v>
-      </c>
-      <c r="L55" s="29">
-        <v>5.157</v>
-      </c>
-      <c r="M55" s="29">
-        <v>3.375</v>
-      </c>
-      <c r="N55" s="59"/>
-    </row>
-    <row r="56" spans="1:14" s="60" customFormat="1">
-      <c r="A56" s="33">
-        <v>4</v>
-      </c>
-      <c r="B56" s="57" t="s">
-        <v>412</v>
+      <c r="B56" s="55" t="s">
+        <v>304</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="D56" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="E56" s="58" t="s">
-        <v>299</v>
-      </c>
-      <c r="F56" s="84" t="s">
-        <v>466</v>
-      </c>
-      <c r="G56" s="58" t="s">
-        <v>250</v>
-      </c>
-      <c r="H56" s="36" t="s">
-        <v>253</v>
-      </c>
-      <c r="I56" s="36"/>
+        <v>306</v>
+      </c>
+      <c r="E56" s="56" t="s">
+        <v>305</v>
+      </c>
+      <c r="F56" s="77" t="s">
+        <v>462</v>
+      </c>
+      <c r="G56" s="56" t="s">
+        <v>427</v>
+      </c>
+      <c r="H56" s="56" t="s">
+        <v>375</v>
+      </c>
+      <c r="I56" s="56"/>
       <c r="J56" s="29">
-        <v>0.9</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K56" s="29">
-        <v>0.79800000000000004</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="L56" s="29">
-        <v>0.63</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="M56" s="29">
-        <v>0.38750000000000001</v>
-      </c>
-      <c r="N56" s="59"/>
-    </row>
-    <row r="57" spans="1:14" s="60" customFormat="1">
+        <v>0.21657999999999999</v>
+      </c>
+      <c r="N56" s="57"/>
+    </row>
+    <row r="57" spans="1:14" s="58" customFormat="1">
       <c r="A57" s="33">
         <v>1</v>
       </c>
-      <c r="B57" s="57" t="s">
-        <v>305</v>
+      <c r="B57" s="55" t="s">
+        <v>282</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>308</v>
-      </c>
-      <c r="D57" s="33" t="s">
-        <v>307</v>
-      </c>
-      <c r="E57" s="58" t="s">
-        <v>306</v>
-      </c>
-      <c r="F57" s="84" t="s">
-        <v>467</v>
-      </c>
-      <c r="G57" s="58" t="s">
-        <v>432</v>
-      </c>
-      <c r="H57" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="D57" s="33"/>
+      <c r="E57" s="56" t="s">
+        <v>284</v>
+      </c>
+      <c r="F57" s="77" t="s">
+        <v>463</v>
+      </c>
+      <c r="G57" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="H57" s="56" t="s">
+        <v>376</v>
+      </c>
+      <c r="I57" s="33" t="s">
         <v>377</v>
       </c>
-      <c r="I57" s="58"/>
       <c r="J57" s="29">
-        <v>0.28000000000000003</v>
+        <v>1.88</v>
       </c>
       <c r="K57" s="29">
-        <v>0.27900000000000003</v>
+        <v>1.704</v>
       </c>
       <c r="L57" s="29">
-        <v>0.22900000000000001</v>
+        <v>1.4608000000000001</v>
       </c>
       <c r="M57" s="29">
-        <v>0.21657999999999999</v>
-      </c>
-      <c r="N57" s="59"/>
-    </row>
-    <row r="58" spans="1:14" s="60" customFormat="1">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="N57" s="57"/>
+    </row>
+    <row r="58" spans="1:14" s="58" customFormat="1">
       <c r="A58" s="33">
         <v>1</v>
       </c>
-      <c r="B58" s="57" t="s">
-        <v>283</v>
+      <c r="B58" s="55" t="s">
+        <v>330</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>284</v>
-      </c>
-      <c r="D58" s="33"/>
-      <c r="E58" s="58" t="s">
-        <v>285</v>
-      </c>
-      <c r="F58" s="84" t="s">
-        <v>468</v>
-      </c>
-      <c r="G58" s="58" t="s">
-        <v>433</v>
-      </c>
-      <c r="H58" s="58" t="s">
+        <v>331</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="E58" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="F58" s="77" t="s">
+        <v>464</v>
+      </c>
+      <c r="G58" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="H58" s="56" t="s">
         <v>378</v>
       </c>
-      <c r="I58" s="33" t="s">
-        <v>379</v>
-      </c>
+      <c r="I58" s="33"/>
       <c r="J58" s="29">
-        <v>1.88</v>
+        <v>1.86</v>
       </c>
       <c r="K58" s="29">
-        <v>1.704</v>
+        <v>1.55</v>
       </c>
       <c r="L58" s="29">
-        <v>1.4608000000000001</v>
-      </c>
-      <c r="M58" s="29">
-        <v>1.0229999999999999</v>
-      </c>
-      <c r="N58" s="59"/>
-    </row>
-    <row r="59" spans="1:14" s="60" customFormat="1">
-      <c r="A59" s="33">
+        <v>1.18</v>
+      </c>
+      <c r="M58" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="N58" s="57"/>
+    </row>
+    <row r="59" spans="1:14" s="58" customFormat="1">
+      <c r="A59" s="65"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="67"/>
+      <c r="F59" s="78"/>
+      <c r="G59" s="67"/>
+      <c r="H59" s="67"/>
+      <c r="I59" s="67"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="30"/>
+      <c r="L59" s="30"/>
+      <c r="M59" s="30"/>
+      <c r="N59" s="68"/>
+    </row>
+    <row r="60" spans="1:14" s="70" customFormat="1">
+      <c r="A60" s="33">
         <v>1</v>
       </c>
-      <c r="B59" s="57" t="s">
-        <v>331</v>
-      </c>
-      <c r="C59" s="33" t="s">
-        <v>332</v>
-      </c>
-      <c r="D59" s="33" t="s">
-        <v>333</v>
-      </c>
-      <c r="E59" s="58" t="s">
-        <v>334</v>
-      </c>
-      <c r="F59" s="84" t="s">
-        <v>469</v>
-      </c>
-      <c r="G59" s="58" t="s">
-        <v>434</v>
-      </c>
-      <c r="H59" s="58" t="s">
-        <v>380</v>
-      </c>
-      <c r="I59" s="33"/>
-      <c r="J59" s="29">
-        <v>1.86</v>
-      </c>
-      <c r="K59" s="29">
-        <v>1.55</v>
-      </c>
-      <c r="L59" s="29">
-        <v>1.18</v>
-      </c>
-      <c r="M59" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="N59" s="59"/>
-    </row>
-    <row r="60" spans="1:14" s="60" customFormat="1">
-      <c r="A60" s="70"/>
-      <c r="B60" s="71"/>
-      <c r="C60" s="70"/>
-      <c r="D60" s="70"/>
-      <c r="E60" s="72"/>
-      <c r="F60" s="86"/>
-      <c r="G60" s="72"/>
-      <c r="H60" s="72"/>
-      <c r="I60" s="72"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="30"/>
-      <c r="M60" s="30"/>
-      <c r="N60" s="73"/>
-    </row>
-    <row r="61" spans="1:14" s="75" customFormat="1">
+      <c r="B60" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="D60" s="33"/>
+      <c r="E60" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="F60" s="77" t="s">
+        <v>465</v>
+      </c>
+      <c r="G60" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="H60" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="I60" s="35"/>
+      <c r="J60" s="29">
+        <v>0.73</v>
+      </c>
+      <c r="K60" s="29">
+        <v>0.65</v>
+      </c>
+      <c r="L60" s="29">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="M60" s="29">
+        <v>0.42502000000000001</v>
+      </c>
+      <c r="N60" s="57"/>
+    </row>
+    <row r="61" spans="1:14" s="70" customFormat="1">
       <c r="A61" s="33">
         <v>1</v>
       </c>
-      <c r="B61" s="57" t="s">
-        <v>274</v>
+      <c r="B61" s="55" t="s">
+        <v>315</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="D61" s="33"/>
-      <c r="E61" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="F61" s="84" t="s">
-        <v>470</v>
-      </c>
-      <c r="G61" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="H61" s="35" t="s">
-        <v>231</v>
-      </c>
-      <c r="I61" s="35"/>
-      <c r="J61" s="29">
-        <v>0.73</v>
-      </c>
-      <c r="K61" s="29">
-        <v>0.65</v>
-      </c>
-      <c r="L61" s="29">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="M61" s="29">
-        <v>0.42502000000000001</v>
-      </c>
-      <c r="N61" s="59"/>
-    </row>
-    <row r="62" spans="1:14" s="75" customFormat="1">
-      <c r="A62" s="33">
-        <v>1</v>
-      </c>
-      <c r="B62" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" s="33" t="s">
         <v>316</v>
       </c>
-      <c r="C62" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="D62" s="33" t="s">
+      <c r="E61" s="56" t="s">
         <v>317</v>
       </c>
-      <c r="E62" s="58" t="s">
-        <v>318</v>
-      </c>
-      <c r="F62" s="84" t="s">
-        <v>471</v>
-      </c>
-      <c r="G62" s="58" t="s">
+      <c r="F61" s="77" t="s">
+        <v>466</v>
+      </c>
+      <c r="G61" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="H62" s="32" t="s">
+      <c r="H61" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="I62" s="32"/>
-      <c r="J62" s="81">
+      <c r="I61" s="32"/>
+      <c r="J61" s="74">
         <v>0.95</v>
       </c>
-      <c r="K62" s="81">
+      <c r="K61" s="74">
         <v>0.84</v>
       </c>
-      <c r="L62" s="81">
+      <c r="L61" s="74">
         <v>0.69</v>
       </c>
-      <c r="M62" s="81">
+      <c r="M61" s="74">
         <v>0.54</v>
       </c>
-      <c r="N62" s="59"/>
+      <c r="N61" s="57"/>
     </row>
   </sheetData>
   <sortState ref="C19:AR30">
@@ -5177,7 +5134,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="D6 D31 D3 D36 D38:D39 D45 D8:D13" numberStoredAsText="1"/>
+    <ignoredError sqref="D6 D31 D3 D36 D38 D44 D8:D13" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5212,54 +5169,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>

</xml_diff>